<commit_message>
Finished Sheets and Belongings
</commit_message>
<xml_diff>
--- a/src/data/TDE5_de-DE.xlsx
+++ b/src/data/TDE5_de-DE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="30" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3279" uniqueCount="2798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3308" uniqueCount="2821">
   <si>
     <t>id</t>
   </si>
@@ -7198,9 +7198,6 @@
     <t>Der Tanz ist so gut, dass der Held mehr Applaus erhält.</t>
   </si>
   <si>
-    <t>Der Held bringt die Tanzschritte durcheinander.</t>
-  </si>
-  <si>
     <t>Die Aufmerksamkeit der Zuschauer fällt wegen des perfekten Tanzes auf den Helden. Für Qualitätsstufen, Vergleichs- und Sammelproben gilt: FP = doppelter FW.</t>
   </si>
   <si>
@@ -8438,6 +8435,78 @@
   </si>
   <si>
     <t>Geschwinder Schritt</t>
+  </si>
+  <si>
+    <t>attributeAdjustments</t>
+  </si>
+  <si>
+    <t>commonAdvantages</t>
+  </si>
+  <si>
+    <t>commonDisadvantages</t>
+  </si>
+  <si>
+    <t>uncommonAdvantages</t>
+  </si>
+  <si>
+    <t>uncommonDisadvantages</t>
+  </si>
+  <si>
+    <t>eine beliebige Eigenschaft nach Wahl +1</t>
+  </si>
+  <si>
+    <t>Emtfernungssinn, Kälteresistenz</t>
+  </si>
+  <si>
+    <t>effect</t>
+  </si>
+  <si>
+    <t>castingtime</t>
+  </si>
+  <si>
+    <t>aecost</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>Das Talent *Sinnesschärfe* wird während der Wirkungsdauer um QS +3 des Zaubers erhöht.</t>
+  </si>
+  <si>
+    <t>2 Aktionen</t>
+  </si>
+  <si>
+    <t>4 AsP (Aktivierung des Zaubers) + 2 AsP pro 5 Minuten</t>
+  </si>
+  <si>
+    <t>selbst</t>
+  </si>
+  <si>
+    <t>aufrechterhaltend</t>
+  </si>
+  <si>
+    <t>Wesen</t>
+  </si>
+  <si>
+    <t>Der Verzauberte erleidet schmerzhafte Muskelschwäche. Während der Wirkungsdauer erleidet er den Zustand *Schmerz*.\n**QS 1:** 1 Stufe *Schmerz*, aber nur für 1 KR\n**QS 2:** 1 Stufe *Schmerz*\n**QS 3:** 2 Stufen *Schmerz*\n**QS 4:** 3 Stufen *Schmerz*\n**QS 5:** 4 Stufen *Schmerz*\n**QS 6:** 4 Stufen *Schmerz*, aber für die doppelte Wirkungsdauer.</t>
+  </si>
+  <si>
+    <t>16 AsP</t>
+  </si>
+  <si>
+    <t>8 Schritt</t>
+  </si>
+  <si>
+    <t>QS x 2 in Kampfrunden</t>
+  </si>
+  <si>
+    <t>Lebewesen</t>
   </si>
 </sst>
 </file>
@@ -8596,7 +8665,7 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="95">
+  <dxfs count="112">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -8938,6 +9007,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -9208,6 +9298,36 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -9258,7 +9378,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1">
-      <tableStyleElement type="headerRow" dxfId="94"/>
+      <tableStyleElement type="headerRow" dxfId="111"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -9622,20 +9742,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
   <autoFilter ref="A1:B10"/>
   <sortState ref="A2:B10">
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="id" dataDxfId="91"/>
-    <tableColumn id="2" name="name" dataDxfId="90"/>
+    <tableColumn id="1" name="id" dataDxfId="108"/>
+    <tableColumn id="2" name="name" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="A1:B44" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:B44">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="id" dataDxfId="41"/>
+    <tableColumn id="2" name="name" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle5" displayName="Tabelle5" ref="A1:B193" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:B193">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -9649,7 +9783,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="A1:B13" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:B13">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -9663,7 +9797,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="A1:J502" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:J502">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -9693,7 +9827,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:B111">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -9707,7 +9841,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:D76">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -9725,7 +9859,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:B36">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -9739,7 +9873,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="A1:B466" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:B466">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -9753,7 +9887,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabelle9" displayName="Tabelle9" ref="A1:B484" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:B484">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -9771,21 +9905,47 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
   <autoFilter ref="A1:B8">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="id" dataDxfId="87"/>
-    <tableColumn id="2" name="name" dataDxfId="86"/>
+    <tableColumn id="1" name="id" dataDxfId="104"/>
+    <tableColumn id="2" name="name" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabelle18" displayName="Tabelle18" ref="A1:H13" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+  <autoFilter ref="A1:H13">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" name="id" dataDxfId="100"/>
+    <tableColumn id="2" name="name" dataDxfId="99"/>
+    <tableColumn id="3" name="attributeAdjustments" dataDxfId="98"/>
+    <tableColumn id="4" name="commonAdvantages" dataDxfId="97"/>
+    <tableColumn id="5" name="commonDisadvantages" dataDxfId="96"/>
+    <tableColumn id="6" name="uncommonAdvantages" dataDxfId="95"/>
+    <tableColumn id="7" name="uncommonDisadvantages" dataDxfId="94"/>
+    <tableColumn id="8" name="src" dataDxfId="93"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
   <autoFilter ref="A1:G95">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9796,36 +9956,36 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="id" dataDxfId="83"/>
-    <tableColumn id="2" name="name" dataDxfId="82"/>
-    <tableColumn id="18" name="name_f" dataDxfId="81"/>
-    <tableColumn id="15" name="subname" dataDxfId="80"/>
-    <tableColumn id="19" name="subname_f" dataDxfId="79"/>
-    <tableColumn id="3" name="req" dataDxfId="78"/>
-    <tableColumn id="4" name="src" dataDxfId="77"/>
+    <tableColumn id="1" name="id" dataDxfId="90"/>
+    <tableColumn id="2" name="name" dataDxfId="89"/>
+    <tableColumn id="18" name="name_f" dataDxfId="88"/>
+    <tableColumn id="15" name="subname" dataDxfId="87"/>
+    <tableColumn id="19" name="subname_f" dataDxfId="86"/>
+    <tableColumn id="3" name="req" dataDxfId="85"/>
+    <tableColumn id="4" name="src" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:C1048576">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="id" dataDxfId="74"/>
-    <tableColumn id="2" name="name" dataDxfId="73"/>
-    <tableColumn id="9" name="name_f" dataDxfId="72"/>
+    <tableColumn id="1" name="id" dataDxfId="81"/>
+    <tableColumn id="2" name="name" dataDxfId="80"/>
+    <tableColumn id="9" name="name_f" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle8" displayName="Tabelle8" ref="A1:D76" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle8" displayName="Tabelle8" ref="A1:D76" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A1:D76">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9833,17 +9993,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="id" dataDxfId="69"/>
-    <tableColumn id="2" name="name" dataDxfId="68"/>
-    <tableColumn id="6" name="sel" dataDxfId="67"/>
-    <tableColumn id="7" name="input" dataDxfId="66"/>
+    <tableColumn id="1" name="id" dataDxfId="76"/>
+    <tableColumn id="2" name="name" dataDxfId="75"/>
+    <tableColumn id="6" name="sel" dataDxfId="74"/>
+    <tableColumn id="7" name="input" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:D72" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:D72" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A1:D72">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9851,17 +10011,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="id" dataDxfId="63"/>
-    <tableColumn id="2" name="name" dataDxfId="62"/>
-    <tableColumn id="6" name="sel" dataDxfId="61"/>
-    <tableColumn id="7" name="input" dataDxfId="60"/>
+    <tableColumn id="1" name="id" dataDxfId="70"/>
+    <tableColumn id="2" name="name" dataDxfId="69"/>
+    <tableColumn id="6" name="sel" dataDxfId="68"/>
+    <tableColumn id="7" name="input" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A1:J60">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9878,46 +10038,39 @@
     <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="id" dataDxfId="57"/>
-    <tableColumn id="2" name="name" dataDxfId="56"/>
-    <tableColumn id="7" name="spec" dataDxfId="55"/>
-    <tableColumn id="8" name="spec_input" dataDxfId="54"/>
-    <tableColumn id="3" name="tools" dataDxfId="53"/>
-    <tableColumn id="4" name="quality" dataDxfId="52"/>
-    <tableColumn id="5" name="failed" dataDxfId="51"/>
-    <tableColumn id="6" name="critical" dataDxfId="50"/>
-    <tableColumn id="9" name="botch" dataDxfId="49"/>
-    <tableColumn id="10" name="src" dataDxfId="48"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A1:B1048576" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="A1:B1048576">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" name="id" dataDxfId="45"/>
-    <tableColumn id="2" name="name" dataDxfId="44"/>
+    <tableColumn id="1" name="id" dataDxfId="64"/>
+    <tableColumn id="2" name="name" dataDxfId="63"/>
+    <tableColumn id="7" name="spec" dataDxfId="62"/>
+    <tableColumn id="8" name="spec_input" dataDxfId="61"/>
+    <tableColumn id="3" name="tools" dataDxfId="60"/>
+    <tableColumn id="4" name="quality" dataDxfId="59"/>
+    <tableColumn id="5" name="failed" dataDxfId="58"/>
+    <tableColumn id="6" name="critical" dataDxfId="57"/>
+    <tableColumn id="9" name="botch" dataDxfId="56"/>
+    <tableColumn id="10" name="src" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="A1:B44" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:B44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:I1048576">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" name="id" dataDxfId="41"/>
-    <tableColumn id="2" name="name" dataDxfId="40"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id" dataDxfId="52"/>
+    <tableColumn id="2" name="name" dataDxfId="51"/>
+    <tableColumn id="3" name="effect" dataDxfId="50"/>
+    <tableColumn id="4" name="castingtime" dataDxfId="49"/>
+    <tableColumn id="5" name="aecost" dataDxfId="48"/>
+    <tableColumn id="6" name="range" dataDxfId="47"/>
+    <tableColumn id="7" name="duration" dataDxfId="46"/>
+    <tableColumn id="8" name="target" dataDxfId="45"/>
+    <tableColumn id="9" name="src" dataDxfId="44"/>
   </tableColumns>
-  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -10322,8 +10475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView topLeftCell="E14" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10656,13 +10809,13 @@
         <v>2383</v>
       </c>
       <c r="G12" s="11" t="s">
+        <v>2380</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>2384</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>2385</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>2386</v>
       </c>
       <c r="J12" s="10">
         <v>192</v>
@@ -10679,19 +10832,19 @@
         <v>2275</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>2386</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>2387</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>2388</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>2389</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>2390</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>2391</v>
       </c>
       <c r="J13" s="10">
         <v>192</v>
@@ -10708,16 +10861,16 @@
         <v>2276</v>
       </c>
       <c r="F14" s="11" t="s">
+        <v>2391</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>2392</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>2393</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>2394</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>2395</v>
       </c>
       <c r="J14" s="10">
         <v>193</v>
@@ -10734,16 +10887,16 @@
         <v>2277</v>
       </c>
       <c r="F15" s="11" t="s">
+        <v>2395</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>2396</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="H15" s="11" t="s">
         <v>2397</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="I15" s="11" t="s">
         <v>2398</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>2399</v>
       </c>
       <c r="J15" s="10">
         <v>193</v>
@@ -10760,16 +10913,16 @@
         <v>2278</v>
       </c>
       <c r="F16" s="11" t="s">
+        <v>2399</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>2400</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>2401</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>2402</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>2403</v>
       </c>
       <c r="J16" s="10">
         <v>194</v>
@@ -10786,16 +10939,16 @@
         <v>2279</v>
       </c>
       <c r="F17" s="11" t="s">
+        <v>2403</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>2404</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>2405</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>2406</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>2407</v>
       </c>
       <c r="J17" s="10">
         <v>195</v>
@@ -10812,16 +10965,16 @@
         <v>2280</v>
       </c>
       <c r="F18" s="11" t="s">
+        <v>2407</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>2408</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="H18" s="11" t="s">
         <v>2409</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>2410</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>2411</v>
       </c>
       <c r="J18" s="10">
         <v>195</v>
@@ -10838,16 +10991,16 @@
         <v>2281</v>
       </c>
       <c r="F19" s="11" t="s">
+        <v>2411</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>2412</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>2413</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="I19" s="11" t="s">
         <v>2414</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>2415</v>
       </c>
       <c r="J19" s="10">
         <v>196</v>
@@ -10864,16 +11017,16 @@
         <v>2282</v>
       </c>
       <c r="F20" s="11" t="s">
+        <v>2415</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>2416</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="H20" s="11" t="s">
         <v>2417</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="I20" s="11" t="s">
         <v>2418</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>2419</v>
       </c>
       <c r="J20" s="10">
         <v>196</v>
@@ -10890,16 +11043,16 @@
         <v>2283</v>
       </c>
       <c r="F21" s="11" t="s">
+        <v>2419</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>2420</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>2421</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>2422</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>2423</v>
       </c>
       <c r="J21" s="10">
         <v>197</v>
@@ -11529,10 +11682,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B234"/>
+  <dimension ref="A1:I234"/>
   <sheetViews>
-    <sheetView topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="E224" sqref="E224"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11542,23 +11695,65 @@
     <col min="3" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="3" t="s">
+        <v>2804</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2805</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2806</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2807</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2808</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2809</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" s="1" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2811</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2812</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2813</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2814</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2815</v>
+      </c>
+      <c r="I2" s="1">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -11566,7 +11761,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -11574,7 +11769,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -11582,7 +11777,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -11590,7 +11785,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -11598,7 +11793,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -11606,7 +11801,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -11614,15 +11809,36 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10" s="1" t="s">
+        <v>2816</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2811</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>2817</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2818</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>2819</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>2820</v>
+      </c>
+      <c r="I10" s="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -11630,7 +11846,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -11638,7 +11854,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -11646,7 +11862,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -11654,7 +11870,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -11662,7 +11878,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -13019,7 +13235,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="12" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
@@ -13027,7 +13243,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.45">
@@ -13035,7 +13251,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="12" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.45">
@@ -13043,7 +13259,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.45">
@@ -13051,7 +13267,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.45">
@@ -13059,7 +13275,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
@@ -13067,7 +13283,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.45">
@@ -13075,7 +13291,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
@@ -13083,7 +13299,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.45">
@@ -13091,7 +13307,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.45">
@@ -13099,7 +13315,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="12" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.45">
@@ -13107,7 +13323,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="12" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.45">
@@ -13115,7 +13331,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.45">
@@ -13123,7 +13339,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.45">
@@ -13131,7 +13347,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="12" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.45">
@@ -13139,7 +13355,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="12" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.45">
@@ -13147,7 +13363,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="12" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.45">
@@ -13155,7 +13371,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="12" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.45">
@@ -13163,7 +13379,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="12" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.45">
@@ -13171,7 +13387,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="12" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.45">
@@ -13179,7 +13395,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="12" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.45">
@@ -13187,7 +13403,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="12" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.45">
@@ -13195,7 +13411,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="12" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.45">
@@ -13203,7 +13419,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="12" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.45">
@@ -13211,7 +13427,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.45">
@@ -13219,7 +13435,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="12" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.45">
@@ -13227,7 +13443,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="12" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.45">
@@ -13235,7 +13451,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="12" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.45">
@@ -13243,7 +13459,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="12" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.45">
@@ -13251,7 +13467,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.45">
@@ -13259,7 +13475,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="12" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.45">
@@ -13267,7 +13483,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="12" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.45">
@@ -13275,7 +13491,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="12" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.45">
@@ -13283,7 +13499,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.45">
@@ -13291,7 +13507,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="12" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.45">
@@ -13299,7 +13515,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="12" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.45">
@@ -13307,7 +13523,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.45">
@@ -13315,7 +13531,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="12" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.45">
@@ -13323,7 +13539,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="12" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.45">
@@ -13331,7 +13547,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="12" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.45">
@@ -13339,7 +13555,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="12" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.45">
@@ -13347,7 +13563,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="12" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.45">
@@ -13355,7 +13571,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="12" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.45">
@@ -13363,7 +13579,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.45">
@@ -13371,7 +13587,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="12" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.45">
@@ -13379,7 +13595,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="12" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.45">
@@ -13387,7 +13603,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="12" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.45">
@@ -13395,7 +13611,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.45">
@@ -13403,7 +13619,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="12" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.45">
@@ -13411,7 +13627,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="12" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
     </row>
   </sheetData>
@@ -13801,8 +14017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="E181" sqref="E181"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14145,7 +14361,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
@@ -14153,7 +14369,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
@@ -14161,7 +14377,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
@@ -14169,7 +14385,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
@@ -14177,7 +14393,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
@@ -14185,7 +14401,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
@@ -14193,7 +14409,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
@@ -14201,7 +14417,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
@@ -14209,7 +14425,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
@@ -14217,7 +14433,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
@@ -14225,7 +14441,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
@@ -14233,7 +14449,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>2658</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
@@ -14241,7 +14457,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>2659</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
@@ -14249,7 +14465,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
@@ -14257,7 +14473,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
@@ -14265,7 +14481,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
@@ -14273,7 +14489,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
@@ -14281,7 +14497,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
@@ -14289,7 +14505,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
@@ -14297,7 +14513,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
@@ -14305,7 +14521,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
@@ -14313,7 +14529,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
@@ -14321,7 +14537,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
@@ -14329,7 +14545,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
@@ -14337,7 +14553,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
@@ -14345,7 +14561,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
@@ -14353,7 +14569,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
@@ -14361,7 +14577,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
@@ -14369,7 +14585,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
@@ -14377,7 +14593,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
@@ -14385,7 +14601,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>2677</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
@@ -14393,7 +14609,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>2678</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
@@ -14401,7 +14617,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>2679</v>
+        <v>2678</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
@@ -14409,7 +14625,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>2680</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
@@ -14417,7 +14633,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
@@ -14425,7 +14641,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>2682</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
@@ -14433,7 +14649,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
@@ -14441,7 +14657,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.45">
@@ -14449,7 +14665,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>2685</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.45">
@@ -14457,7 +14673,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>2686</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.45">
@@ -14465,7 +14681,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>2687</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.45">
@@ -14473,7 +14689,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>2688</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.45">
@@ -14481,7 +14697,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>2689</v>
+        <v>2688</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.45">
@@ -14489,7 +14705,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
@@ -14497,7 +14713,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.45">
@@ -14505,7 +14721,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.45">
@@ -14513,7 +14729,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.45">
@@ -14521,7 +14737,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.45">
@@ -14529,7 +14745,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>2694</v>
+        <v>2693</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.45">
@@ -14537,7 +14753,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>2695</v>
+        <v>2694</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
@@ -14545,7 +14761,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>2696</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
@@ -14553,7 +14769,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
@@ -14561,7 +14777,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.45">
@@ -14569,7 +14785,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>2699</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.45">
@@ -14577,7 +14793,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.45">
@@ -14585,7 +14801,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.45">
@@ -14593,7 +14809,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.45">
@@ -14601,7 +14817,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>2703</v>
+        <v>2702</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.45">
@@ -14609,7 +14825,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.45">
@@ -14617,7 +14833,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.45">
@@ -14625,7 +14841,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.45">
@@ -14633,7 +14849,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.45">
@@ -14641,7 +14857,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.45">
@@ -14649,7 +14865,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.45">
@@ -14657,7 +14873,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
@@ -14665,7 +14881,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
@@ -14673,7 +14889,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">
@@ -14681,7 +14897,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.45">
@@ -14689,7 +14905,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>2714</v>
+        <v>2713</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
@@ -14697,7 +14913,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
@@ -14705,7 +14921,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>2716</v>
+        <v>2715</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -14713,7 +14929,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
@@ -14721,7 +14937,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
@@ -14729,7 +14945,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>2719</v>
+        <v>2718</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
@@ -14737,7 +14953,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>2720</v>
+        <v>2719</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
@@ -14745,7 +14961,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
@@ -14753,7 +14969,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
@@ -14761,7 +14977,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
@@ -14769,7 +14985,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
@@ -14777,7 +14993,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
@@ -14785,7 +15001,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>2726</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
@@ -14793,7 +15009,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>2727</v>
+        <v>2726</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
@@ -14801,7 +15017,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>2728</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
@@ -14809,7 +15025,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
@@ -14817,7 +15033,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
@@ -14825,7 +15041,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
@@ -14833,7 +15049,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
@@ -14841,7 +15057,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
@@ -14849,7 +15065,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
@@ -14857,7 +15073,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
@@ -14865,7 +15081,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
@@ -14873,7 +15089,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
@@ -14881,7 +15097,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
@@ -14889,7 +15105,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
@@ -14897,7 +15113,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
@@ -14905,7 +15121,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
@@ -14913,7 +15129,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
@@ -14921,7 +15137,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
@@ -14929,7 +15145,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
@@ -14937,7 +15153,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
@@ -14945,7 +15161,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
@@ -14953,7 +15169,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
@@ -14961,7 +15177,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.45">
@@ -14969,7 +15185,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.45">
@@ -14977,7 +15193,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.45">
@@ -14985,7 +15201,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.45">
@@ -14993,7 +15209,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.45">
@@ -15001,7 +15217,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.45">
@@ -15009,7 +15225,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.45">
@@ -15017,7 +15233,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.45">
@@ -15025,7 +15241,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.45">
@@ -15033,7 +15249,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.45">
@@ -15041,7 +15257,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.45">
@@ -15049,7 +15265,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.45">
@@ -15057,7 +15273,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.45">
@@ -15065,7 +15281,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.45">
@@ -15073,7 +15289,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.45">
@@ -15081,7 +15297,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.45">
@@ -15089,7 +15305,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.45">
@@ -15097,7 +15313,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.45">
@@ -15105,7 +15321,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.45">
@@ -15113,7 +15329,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.45">
@@ -15121,7 +15337,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.45">
@@ -15129,7 +15345,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.45">
@@ -15137,7 +15353,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.45">
@@ -15145,7 +15361,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>2770</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.45">
@@ -15153,7 +15369,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>2771</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.45">
@@ -15161,7 +15377,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.45">
@@ -15169,7 +15385,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.45">
@@ -15177,7 +15393,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.45">
@@ -15185,7 +15401,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.45">
@@ -15193,7 +15409,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.45">
@@ -15201,7 +15417,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.45">
@@ -15209,7 +15425,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.45">
@@ -15217,7 +15433,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.45">
@@ -15225,7 +15441,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.45">
@@ -15233,7 +15449,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.45">
@@ -15241,7 +15457,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.45">
@@ -15249,7 +15465,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.45">
@@ -15257,7 +15473,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.45">
@@ -15265,7 +15481,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.45">
@@ -15273,7 +15489,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.45">
@@ -15281,7 +15497,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.45">
@@ -15289,7 +15505,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
@@ -15297,7 +15513,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.45">
@@ -15305,7 +15521,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.45">
@@ -15321,7 +15537,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.45">
@@ -15329,7 +15545,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
@@ -15337,7 +15553,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.45">
@@ -15345,7 +15561,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
@@ -15353,7 +15569,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
     </row>
   </sheetData>
@@ -16251,7 +16467,7 @@
         <v>445</v>
       </c>
       <c r="C87" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.45">
@@ -16390,7 +16606,7 @@
         <v>445</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.45">
@@ -16401,7 +16617,7 @@
         <v>488</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="D104" s="5"/>
     </row>
@@ -17669,7 +17885,7 @@
         <v>1633</v>
       </c>
       <c r="C262" s="11" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.45">
@@ -19472,7 +19688,7 @@
         <v>486</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.45">
@@ -19480,7 +19696,7 @@
         <v>487</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.45">
@@ -19488,7 +19704,7 @@
         <v>488</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.45">
@@ -19496,7 +19712,7 @@
         <v>489</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.45">
@@ -19504,7 +19720,7 @@
         <v>490</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.45">
@@ -19512,7 +19728,7 @@
         <v>491</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.45">
@@ -19520,7 +19736,7 @@
         <v>492</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.45">
@@ -19528,7 +19744,7 @@
         <v>493</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.45">
@@ -19536,7 +19752,7 @@
         <v>494</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.45">
@@ -19544,7 +19760,7 @@
         <v>495</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.45">
@@ -19552,7 +19768,7 @@
         <v>496</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.45">
@@ -19560,7 +19776,7 @@
         <v>497</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.45">
@@ -19568,7 +19784,7 @@
         <v>498</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.45">
@@ -19576,7 +19792,7 @@
         <v>499</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.45">
@@ -19584,7 +19800,7 @@
         <v>500</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.45">
@@ -19592,7 +19808,7 @@
         <v>501</v>
       </c>
       <c r="B502" s="12" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
     </row>
   </sheetData>
@@ -29233,7 +29449,7 @@
         <v>474</v>
       </c>
       <c r="B475" s="18" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.45">
@@ -29241,7 +29457,7 @@
         <v>475</v>
       </c>
       <c r="B476" s="18" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.45">
@@ -29249,7 +29465,7 @@
         <v>476</v>
       </c>
       <c r="B477" s="18" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.45">
@@ -29257,7 +29473,7 @@
         <v>477</v>
       </c>
       <c r="B478" s="18" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.45">
@@ -29265,7 +29481,7 @@
         <v>478</v>
       </c>
       <c r="B479" s="18" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.45">
@@ -29281,7 +29497,7 @@
         <v>480</v>
       </c>
       <c r="B481" s="18" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.45">
@@ -29297,7 +29513,7 @@
         <v>482</v>
       </c>
       <c r="B483" s="18" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.45">
@@ -29305,7 +29521,7 @@
         <v>483</v>
       </c>
       <c r="B484" s="18" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
   </sheetData>
@@ -29319,10 +29535,180 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2797</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2798</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2799</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2800</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2801</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2802</v>
+      </c>
+      <c r="H2" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2802</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2803</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29345,7 +29731,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -29353,7 +29739,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -29361,7 +29747,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -29369,7 +29755,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -29377,7 +29763,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -29385,7 +29771,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -29393,7 +29779,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
@@ -29401,7 +29787,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -29409,7 +29795,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -29417,7 +29803,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -29425,7 +29811,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -29433,131 +29819,6 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="2.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -29670,7 +29931,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
     </row>
   </sheetData>
@@ -29685,8 +29946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -30635,7 +30896,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -30650,13 +30911,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="G59" s="12">
         <v>179</v>
@@ -30673,10 +30934,10 @@
         <v>751</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="F60" s="18"/>
       <c r="G60" s="12">
@@ -30694,11 +30955,11 @@
         <v>751</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="E61" s="18"/>
       <c r="F61" s="18" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="G61" s="12">
         <v>181</v>
@@ -30715,10 +30976,10 @@
         <v>751</v>
       </c>
       <c r="D62" s="18" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E62" s="18" t="s">
         <v>2488</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>2489</v>
       </c>
       <c r="F62" s="18"/>
       <c r="G62" s="12">
@@ -30736,10 +30997,10 @@
         <v>751</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="F63" s="18"/>
       <c r="G63" s="12">
@@ -30757,11 +31018,11 @@
         <v>273</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="E64" s="18"/>
       <c r="F64" s="18" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="G64" s="12">
         <v>184</v>
@@ -30778,7 +31039,7 @@
         <v>273</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="E65" s="18"/>
       <c r="F65" s="18"/>
@@ -30797,7 +31058,7 @@
         <v>273</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
@@ -30816,7 +31077,7 @@
         <v>273</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
@@ -30835,7 +31096,7 @@
         <v>273</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="E68" s="18"/>
       <c r="F68" s="18"/>
@@ -30873,7 +31134,7 @@
         <v>273</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
@@ -30886,7 +31147,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="C71" s="18"/>
       <c r="D71" s="18"/>
@@ -30901,10 +31162,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="18" t="s">
+        <v>2471</v>
+      </c>
+      <c r="C72" s="18" t="s">
         <v>2472</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>2473</v>
       </c>
       <c r="D72" s="18"/>
       <c r="E72" s="18"/>
@@ -30918,7 +31179,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="C73" s="18"/>
       <c r="D73" s="18"/>
@@ -30933,13 +31194,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="C74" s="18"/>
       <c r="D74" s="18"/>
       <c r="E74" s="18"/>
       <c r="F74" s="18" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="G74" s="12">
         <v>194</v>
@@ -30950,7 +31211,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="C75" s="18"/>
       <c r="D75" s="18"/>
@@ -30965,7 +31226,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="C76" s="18"/>
       <c r="D76" s="18"/>
@@ -30980,10 +31241,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="18" t="s">
+        <v>2477</v>
+      </c>
+      <c r="C77" s="18" t="s">
         <v>2478</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>2479</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="18"/>
@@ -31003,7 +31264,7 @@
         <v>272</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="E78" s="18"/>
       <c r="F78" s="18"/>
@@ -31022,10 +31283,10 @@
         <v>272</v>
       </c>
       <c r="D79" s="18" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E79" s="18" t="s">
         <v>2501</v>
-      </c>
-      <c r="E79" s="18" t="s">
-        <v>2502</v>
       </c>
       <c r="F79" s="18"/>
       <c r="G79" s="12">
@@ -31056,7 +31317,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="C81" s="18"/>
       <c r="D81" s="18"/>
@@ -31077,7 +31338,7 @@
         <v>752</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="E82" s="18"/>
       <c r="F82" s="17" t="s">
@@ -31098,13 +31359,13 @@
         <v>752</v>
       </c>
       <c r="D83" s="18" t="s">
+        <v>2523</v>
+      </c>
+      <c r="E83" s="18" t="s">
         <v>2524</v>
       </c>
-      <c r="E83" s="18" t="s">
-        <v>2525</v>
-      </c>
       <c r="F83" s="18" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="G83" s="12">
         <v>204</v>
@@ -31121,7 +31382,7 @@
         <v>752</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="E84" s="18"/>
       <c r="F84" s="18"/>
@@ -31134,10 +31395,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="18" t="s">
+        <v>2480</v>
+      </c>
+      <c r="C85" s="18" t="s">
         <v>2481</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>2482</v>
       </c>
       <c r="D85" s="18"/>
       <c r="E85" s="18"/>
@@ -31151,10 +31412,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="18" t="s">
+        <v>2482</v>
+      </c>
+      <c r="C86" s="18" t="s">
         <v>2483</v>
-      </c>
-      <c r="C86" s="18" t="s">
-        <v>2484</v>
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="18"/>
@@ -31168,10 +31429,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="18" t="s">
+        <v>2484</v>
+      </c>
+      <c r="C87" s="18" t="s">
         <v>2485</v>
-      </c>
-      <c r="C87" s="18" t="s">
-        <v>2486</v>
       </c>
       <c r="D87" s="18"/>
       <c r="E87" s="18"/>
@@ -31185,16 +31446,16 @@
         <v>87</v>
       </c>
       <c r="B88" s="18" t="s">
+        <v>2518</v>
+      </c>
+      <c r="C88" s="18" t="s">
         <v>2519</v>
       </c>
-      <c r="C88" s="18" t="s">
+      <c r="D88" s="18" t="s">
+        <v>2516</v>
+      </c>
+      <c r="E88" s="18" t="s">
         <v>2520</v>
-      </c>
-      <c r="D88" s="18" t="s">
-        <v>2517</v>
-      </c>
-      <c r="E88" s="18" t="s">
-        <v>2521</v>
       </c>
       <c r="F88" s="18"/>
       <c r="G88" s="18">
@@ -31206,16 +31467,16 @@
         <v>88</v>
       </c>
       <c r="B89" s="18" t="s">
+        <v>2518</v>
+      </c>
+      <c r="C89" s="18" t="s">
         <v>2519</v>
       </c>
-      <c r="C89" s="18" t="s">
-        <v>2520</v>
-      </c>
       <c r="D89" s="18" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="F89" s="18"/>
       <c r="G89" s="18">
@@ -31233,7 +31494,7 @@
         <v>273</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
@@ -31252,7 +31513,7 @@
         <v>752</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="E91" s="18"/>
       <c r="F91" s="18"/>
@@ -31265,13 +31526,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="C92" s="18" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="E92" s="18"/>
       <c r="F92" s="18"/>
@@ -31284,13 +31545,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="18" t="s">
+        <v>2511</v>
+      </c>
+      <c r="C93" s="18" t="s">
         <v>2512</v>
       </c>
-      <c r="C93" s="18" t="s">
-        <v>2513</v>
-      </c>
       <c r="D93" s="18" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="E93" s="18"/>
       <c r="F93" s="18"/>
@@ -31303,13 +31564,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="C94" s="18" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="E94" s="18"/>
       <c r="F94" s="18"/>
@@ -31322,16 +31583,16 @@
         <v>94</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="C95" s="18" t="s">
+        <v>2513</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>2507</v>
+      </c>
+      <c r="E95" s="18" t="s">
         <v>2514</v>
-      </c>
-      <c r="D95" s="18" t="s">
-        <v>2508</v>
-      </c>
-      <c r="E95" s="18" t="s">
-        <v>2515</v>
       </c>
       <c r="F95" s="18"/>
       <c r="G95" s="18">
@@ -32678,10 +32939,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="18" t="s">
+        <v>2526</v>
+      </c>
+      <c r="C120" s="18" t="s">
         <v>2527</v>
-      </c>
-      <c r="C120" s="18" t="s">
-        <v>2528</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
@@ -32689,10 +32950,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="18" t="s">
+        <v>2528</v>
+      </c>
+      <c r="C121" s="18" t="s">
         <v>2529</v>
-      </c>
-      <c r="C121" s="18" t="s">
-        <v>2530</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
@@ -32700,10 +32961,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="18" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C122" s="18" t="s">
         <v>2531</v>
-      </c>
-      <c r="C122" s="18" t="s">
-        <v>2532</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
@@ -32722,10 +32983,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="18" t="s">
+        <v>2532</v>
+      </c>
+      <c r="C124" s="18" t="s">
         <v>2533</v>
-      </c>
-      <c r="C124" s="18" t="s">
-        <v>2534</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
@@ -32733,10 +32994,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="18" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C125" s="18" t="s">
         <v>2535</v>
-      </c>
-      <c r="C125" s="18" t="s">
-        <v>2536</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
@@ -32744,10 +33005,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="18" t="s">
+        <v>2536</v>
+      </c>
+      <c r="C126" s="18" t="s">
         <v>2537</v>
-      </c>
-      <c r="C126" s="18" t="s">
-        <v>2538</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
@@ -32755,7 +33016,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="18" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="C127" s="18"/>
     </row>
@@ -32764,7 +33025,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="C128" s="18"/>
     </row>
@@ -32773,7 +33034,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="18" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="C129" s="18"/>
     </row>
@@ -32782,7 +33043,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="18" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="C130" s="18"/>
     </row>
@@ -32791,7 +33052,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="18" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="C131" s="18"/>
     </row>
@@ -32800,7 +33061,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="18" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="C132" s="18"/>
     </row>
@@ -32809,7 +33070,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="18" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="C133" s="18"/>
     </row>
@@ -32818,7 +33079,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="18" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="C134" s="18"/>
     </row>
@@ -32827,10 +33088,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="18" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="C135" s="18" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
@@ -32838,10 +33099,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="18" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="C136" s="18" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
@@ -32849,7 +33110,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="C137" s="18"/>
     </row>
@@ -32858,7 +33119,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="18" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="C138" s="18"/>
     </row>
@@ -32867,7 +33128,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="18" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="C139" s="18"/>
     </row>
@@ -32876,7 +33137,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="18" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="C140" s="18"/>
     </row>
@@ -32885,7 +33146,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="18" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="C141" s="18"/>
     </row>
@@ -32894,7 +33155,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="18" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="C142" s="18"/>
     </row>
@@ -32903,7 +33164,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="18" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="C143" s="18"/>
     </row>
@@ -32912,7 +33173,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="C144" s="18"/>
     </row>
@@ -32921,10 +33182,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="18" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="C145" s="18" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
@@ -32932,10 +33193,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="18" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="C146" s="18" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
@@ -32943,7 +33204,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="18" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="C147" s="18"/>
     </row>
@@ -32952,7 +33213,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="18" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="C148" s="18"/>
     </row>
@@ -32961,7 +33222,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="18" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="C149" s="18"/>
     </row>
@@ -32970,7 +33231,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="18" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="C150" s="18"/>
     </row>
@@ -32979,7 +33240,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="18" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="C151" s="18"/>
     </row>
@@ -32988,7 +33249,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="18" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="C152" s="18"/>
     </row>
@@ -32997,7 +33258,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="18" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="C153" s="18"/>
     </row>
@@ -33006,7 +33267,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="18" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="C154" s="18"/>
     </row>
@@ -33015,7 +33276,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="18" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="C155" s="18"/>
     </row>
@@ -33024,7 +33285,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="18" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="C156" s="18"/>
     </row>
@@ -33033,7 +33294,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="18" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C157" s="18"/>
     </row>
@@ -33042,7 +33303,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="18" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="C158" s="18"/>
     </row>
@@ -33051,7 +33312,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="15" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="C159" s="18"/>
     </row>
@@ -33060,7 +33321,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="15" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="C160" s="18"/>
     </row>
@@ -33069,10 +33330,10 @@
         <v>160</v>
       </c>
       <c r="B161" s="18" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="C161" s="18" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
@@ -33080,7 +33341,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="18" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="C162" s="18"/>
     </row>
@@ -33581,7 +33842,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
@@ -33589,7 +33850,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
@@ -33597,7 +33858,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
@@ -33605,7 +33866,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
@@ -33613,7 +33874,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
@@ -33621,7 +33882,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
@@ -33629,7 +33890,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
@@ -33637,7 +33898,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
@@ -33645,7 +33906,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
@@ -33653,7 +33914,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
@@ -33661,7 +33922,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
@@ -33669,7 +33930,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
@@ -33677,13 +33938,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
@@ -33691,7 +33952,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
@@ -33699,7 +33960,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
@@ -33707,7 +33968,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
@@ -33715,7 +33976,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
@@ -33723,7 +33984,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
@@ -33731,7 +33992,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
@@ -33739,7 +34000,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
     </row>
   </sheetData>
@@ -34338,7 +34599,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
@@ -34346,7 +34607,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
@@ -34354,7 +34615,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
@@ -34362,7 +34623,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
@@ -34370,7 +34631,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
@@ -34378,7 +34639,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
@@ -34386,7 +34647,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
@@ -34394,7 +34655,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temporary dropdown redesign done
</commit_message>
<xml_diff>
--- a/src/data/TDE5_de-DE.xlsx
+++ b/src/data/TDE5_de-DE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="30" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5109" uniqueCount="3027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5264" uniqueCount="3091">
   <si>
     <t>id</t>
   </si>
@@ -9136,6 +9136,198 @@
   </si>
   <si>
     <t xml:space="preserve">8 AsP + 4 AsP je zus. P. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS/KS x 3 AsP </t>
+  </si>
+  <si>
+    <t>20 m</t>
+  </si>
+  <si>
+    <t>KS AsP</t>
+  </si>
+  <si>
+    <t>QS x 20 m</t>
+  </si>
+  <si>
+    <t>4 m</t>
+  </si>
+  <si>
+    <t>8 m</t>
+  </si>
+  <si>
+    <t>16 m</t>
+  </si>
+  <si>
+    <t>1 m</t>
+  </si>
+  <si>
+    <t>32 m</t>
+  </si>
+  <si>
+    <t>2 m</t>
+  </si>
+  <si>
+    <t>8 / 16 AsP</t>
+  </si>
+  <si>
+    <t>4 AsP + 2 AsP pro 5 Min</t>
+  </si>
+  <si>
+    <t>4/8/16 AsP</t>
+  </si>
+  <si>
+    <t>2 AsP + 1 AsP pro Stunde</t>
+  </si>
+  <si>
+    <t>4 AsP + 2 AsP pro Minute</t>
+  </si>
+  <si>
+    <t>4 AsP + 2 AsP pro Kampfrunde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 AsP, 4 AsP pro Minute </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 AsP + 4 AsP pro Stunde </t>
+  </si>
+  <si>
+    <t>8 AsP + 4 AsP pro Stunde</t>
+  </si>
+  <si>
+    <t>4 AsP + 2 AsP pro KR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 AsP, + 2 AsP pro 30 Sekunden </t>
+  </si>
+  <si>
+    <t>8 AsP + 4 AsP pro 5 Min</t>
+  </si>
+  <si>
+    <t>2 AsP + 1 AsP pro 10 Min</t>
+  </si>
+  <si>
+    <t>4 AsP + 2 AsP pro 10 Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 AsP pro 5 Min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 AsP pro 5 Min </t>
+  </si>
+  <si>
+    <t>8 AsP + 4 AsP pro 10 Min</t>
+  </si>
+  <si>
+    <t>16 AsP + 8 AsP pro 5 Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mindestens 4 AsP (Aktivierung) + Hälfte der Aktivierungskosten pro 5 Min (Kosten sind nicht modifizierbar) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 AsP + 2 AsP pro 5 Min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 AsP + 4 AsP pro 10 Min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 AsP + 2 AsP pro 10 Min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 AsP + 4 AsP pro 5 Min </t>
+  </si>
+  <si>
+    <t>1 AsP pro LeP (4+)</t>
+  </si>
+  <si>
+    <t>4 AsP pro DG</t>
+  </si>
+  <si>
+    <t>4+ AsP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4+ AsP + 1/2 pro 5 Min </t>
+  </si>
+  <si>
+    <t>8 AsP + 1 AsP pro km</t>
+  </si>
+  <si>
+    <t>10+ AsP</t>
+  </si>
+  <si>
+    <t>2 Akt</t>
+  </si>
+  <si>
+    <t>16 Akt</t>
+  </si>
+  <si>
+    <t>4 Akt</t>
+  </si>
+  <si>
+    <t>8 Akt</t>
+  </si>
+  <si>
+    <t>1 Akt</t>
+  </si>
+  <si>
+    <t>2 h</t>
+  </si>
+  <si>
+    <t>1+ Akt</t>
+  </si>
+  <si>
+    <t>64 m</t>
+  </si>
+  <si>
+    <t>4 AsP pro h/1 pAsP</t>
+  </si>
+  <si>
+    <t>4 AsP pro h</t>
+  </si>
+  <si>
+    <t>QS x 3 m</t>
+  </si>
+  <si>
+    <t>permanent</t>
+  </si>
+  <si>
+    <t>Hören</t>
+  </si>
+  <si>
+    <t>Musizieren oder Singen</t>
+  </si>
+  <si>
+    <t>Musizieren/Singen</t>
+  </si>
+  <si>
+    <t>1 h</t>
+  </si>
+  <si>
+    <t>3 Tage</t>
+  </si>
+  <si>
+    <t>bel.</t>
+  </si>
+  <si>
+    <t>30+ Min</t>
+  </si>
+  <si>
+    <t>24 h</t>
+  </si>
+  <si>
+    <t>max. 5 Min</t>
+  </si>
+  <si>
+    <t>12 h</t>
+  </si>
+  <si>
+    <t>max. 2 KR</t>
+  </si>
+  <si>
+    <t>kpcost</t>
+  </si>
+  <si>
+    <t>kpcostShort</t>
   </si>
 </sst>
 </file>
@@ -9255,7 +9447,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9318,6 +9510,9 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Erklärender Text 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
@@ -9325,7 +9520,40 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
-  <dxfs count="119">
+  <dxfs count="130">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -10059,7 +10287,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="118"/>
+      <tableStyleElement type="headerRow" dxfId="129"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -10423,63 +10651,85 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
   <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <sortState ref="A2:B10">
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="115"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table14" displayName="Table14" ref="A1:B44" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table14" displayName="Table14" ref="A1:B44" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:B44" xr:uid="{00000000-0009-0000-0100-00000E000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="id" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="name" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="id" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="name" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:B193" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A1:B193" xr:uid="{00000000-0009-0000-0100-000005000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:M193" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+  <autoFilter ref="A1:M193" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="36"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{452BCF15-63D6-4F0D-8237-F453C9931794}" name="effect" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{3C4B8B30-E7ED-4AB5-BC66-F5C283820DD3}" name="castingtime" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{EDD4FA58-CDB8-416C-923B-13AE644AA21A}" name="castingtimeShort" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{E3A80605-B07C-400F-9DD6-DA1ECD45B17F}" name="kpcost" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{3735962A-FF4F-4E3D-9AFC-95B48BCF0758}" name="kpcostShort" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{4D0248C5-34EF-49A3-B1B4-33D1C05D9FBB}" name="range" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{D6111C84-C6C2-4C98-9BAC-040E9A31F2B9}" name="rangeShort" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{F33F5A8B-FEA1-4B00-AE2D-20CCBB24FF2A}" name="duration" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{66749CC6-D9C4-4BF4-BA63-F5A58FD8E6CB}" name="durationShort" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{BE17D95F-F42A-48F5-9E7F-A545D95D81C2}" name="target" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{1E0275F4-0996-4EC0-B571-4BB2870B8257}" name="src" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="A1:B13" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="A1:B13" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:B13" xr:uid="{00000000-0009-0000-0100-000010000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:J502" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:J502" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A1:J502" xr:uid="{00000000-0009-0000-0100-000006000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10493,37 +10743,37 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="sel" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="input" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column1" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column2" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column3" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Column4" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Column5" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Column6" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="sel" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="input" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column1" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column2" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column3" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Column4" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Column5" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Column6" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:B111" xr:uid="{00000000-0009-0000-0100-00000A000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:D76" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10531,45 +10781,45 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="spec" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="specInput" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="spec" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="specInput" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:B36" xr:uid="{00000000-0009-0000-0100-00000B000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table15" displayName="Table15" ref="A1:B466" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table15" displayName="Table15" ref="A1:B466" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A1:B466" xr:uid="{00000000-0009-0000-0100-00000F000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="3" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="14" dataCellStyle="Excel Built-in Normal"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:B484" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:B484" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:B484" xr:uid="{00000000-0009-0000-0100-000009000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10578,29 +10828,29 @@
     <sortCondition ref="A1:A474"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
   <autoFilter ref="A1:B8" xr:uid="{00000000-0009-0000-0100-00000D000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="122"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="121"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:K13" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:K13" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
   <autoFilter ref="A1:K13" xr:uid="{00000000-0009-0000-0100-000012000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10612,24 +10862,24 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="107"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="attributeAdjustments" dataDxfId="105"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="automaticAdvantages" dataDxfId="104"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="stronglyRecommendedAdvantages" dataDxfId="103"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="stronglyRecommendedDisadvantages" dataDxfId="102"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="commonAdvantages" dataDxfId="101"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="commonDisadvantages" dataDxfId="100"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="uncommonAdvantages" dataDxfId="99"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="uncommonDisadvantages" dataDxfId="98"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="src" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="118"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="117"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="attributeAdjustments" dataDxfId="116"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="automaticAdvantages" dataDxfId="115"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="stronglyRecommendedAdvantages" dataDxfId="114"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="stronglyRecommendedDisadvantages" dataDxfId="113"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="commonAdvantages" dataDxfId="112"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="commonDisadvantages" dataDxfId="111"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="uncommonAdvantages" dataDxfId="110"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="uncommonDisadvantages" dataDxfId="109"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="src" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A1:G95" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10640,36 +10890,36 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="id" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="name" dataDxfId="93"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="name_f" dataDxfId="92"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="subname" dataDxfId="91"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="subname_f" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="req" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="src" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="id" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="name" dataDxfId="104"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="name_f" dataDxfId="103"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="subname" dataDxfId="102"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="subname_f" dataDxfId="101"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="req" dataDxfId="100"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="src" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="id" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="name" dataDxfId="84"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="name_f" dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="id" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="name" dataDxfId="95"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="name_f" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:D76" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:D76" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="A1:D76" xr:uid="{00000000-0009-0000-0100-000008000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10677,17 +10927,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="79"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="sel" dataDxfId="78"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="input" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="sel" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="input" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:D72" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:D72" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
   <autoFilter ref="A1:D72" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10695,17 +10945,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="id" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="name" dataDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="sel" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="input" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="id" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="name" dataDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="sel" dataDxfId="83"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="input" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
   <autoFilter ref="A1:J60" xr:uid="{00000000-0009-0000-0100-000007000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10722,41 +10972,41 @@
     <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="id" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="name" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="spec" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="spec_input" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="tools" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="quality" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="failed" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="critical" dataDxfId="61"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="botch" dataDxfId="60"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="src" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="id" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="name" dataDxfId="78"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="spec" dataDxfId="77"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="spec_input" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="tools" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="quality" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="failed" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="critical" dataDxfId="72"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="botch" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="src" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:M1048576" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:M1048576" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="A1:M1048576" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="effect" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="castingtime" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{D89CFCD8-0667-4532-ADCB-656E0F380FC9}" name="castingtimeShort" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="aecost" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{AA76CB3A-D16A-4989-ACEE-9057F8B23848}" name="aecostShort" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="range" dataDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{DD92ED00-D630-4075-AFBB-75382F298664}" name="rangeShort" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="duration" dataDxfId="47"/>
-    <tableColumn id="13" xr3:uid="{35897220-D86D-43E4-9246-750CE8AD5E3B}" name="durationShort" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="target" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="src" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="effect" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="castingtime" dataDxfId="64"/>
+    <tableColumn id="10" xr3:uid="{D89CFCD8-0667-4532-ADCB-656E0F380FC9}" name="castingtimeShort" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="aecost" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{AA76CB3A-D16A-4989-ACEE-9057F8B23848}" name="aecostShort" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="range" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{DD92ED00-D630-4075-AFBB-75382F298664}" name="rangeShort" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="duration" dataDxfId="58"/>
+    <tableColumn id="13" xr3:uid="{35897220-D86D-43E4-9246-750CE8AD5E3B}" name="durationShort" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="target" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="src" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12372,8 +12622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="G187" sqref="G187"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12438,13 +12688,13 @@
         <v>2810</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2811</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>2811</v>
+        <v>3038</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>2812</v>
@@ -12476,7 +12726,7 @@
         <v>2810</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>2816</v>
@@ -12511,13 +12761,13 @@
         <v>2849</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>2857</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>2857</v>
+        <v>3039</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>2812</v>
@@ -12546,7 +12796,7 @@
         <v>2849</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2858</v>
@@ -12581,13 +12831,13 @@
         <v>2850</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2850</v>
+        <v>3067</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>2859</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>2859</v>
+        <v>3060</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>2910</v>
@@ -12616,7 +12866,7 @@
         <v>2851</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>2858</v>
@@ -12628,7 +12878,7 @@
         <v>2911</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>2918</v>
@@ -12651,7 +12901,7 @@
         <v>2851</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>2858</v>
@@ -12663,7 +12913,7 @@
         <v>2911</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>2813</v>
@@ -12686,7 +12936,7 @@
         <v>2849</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>2860</v>
@@ -12698,7 +12948,7 @@
         <v>2817</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>2920</v>
@@ -12724,7 +12974,7 @@
         <v>2810</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>2816</v>
@@ -12736,7 +12986,7 @@
         <v>2817</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>2818</v>
@@ -12762,13 +13012,13 @@
         <v>2852</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>2861</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>2861</v>
+        <v>3048</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>2812</v>
@@ -12797,13 +13047,13 @@
         <v>2810</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>2862</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>2862</v>
+        <v>3061</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>2910</v>
@@ -12832,7 +13082,7 @@
         <v>2810</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>2860</v>
@@ -12867,19 +13117,19 @@
         <v>2849</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>2863</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>2863</v>
+        <v>3040</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>2817</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>2813</v>
@@ -12902,7 +13152,7 @@
         <v>2849</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>2858</v>
@@ -12914,7 +13164,7 @@
         <v>2817</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>2917</v>
@@ -12937,13 +13187,13 @@
         <v>2849</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>2864</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>2864</v>
+        <v>3062</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>2812</v>
@@ -12972,7 +13222,7 @@
         <v>2810</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>2858</v>
@@ -13007,13 +13257,13 @@
         <v>2851</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>2861</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>2861</v>
+        <v>3048</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>2812</v>
@@ -13042,7 +13292,7 @@
         <v>2849</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>2860</v>
@@ -13077,7 +13327,7 @@
         <v>2849</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>2860</v>
@@ -13112,7 +13362,7 @@
         <v>2810</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>2858</v>
@@ -13124,7 +13374,7 @@
         <v>2817</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>2918</v>
@@ -13147,7 +13397,7 @@
         <v>2810</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>2858</v>
@@ -13159,7 +13409,7 @@
         <v>2912</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>2917</v>
@@ -13182,7 +13432,7 @@
         <v>2851</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>2860</v>
@@ -13194,7 +13444,7 @@
         <v>2913</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>2913</v>
+        <v>3034</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>2917</v>
@@ -13217,13 +13467,13 @@
         <v>2851</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>2865</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>2865</v>
+        <v>3049</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>2812</v>
@@ -13252,7 +13502,7 @@
         <v>2810</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>2866</v>
@@ -13287,7 +13537,7 @@
         <v>2851</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>2860</v>
@@ -13299,7 +13549,7 @@
         <v>2913</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>2913</v>
+        <v>3034</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>2917</v>
@@ -13322,13 +13572,13 @@
         <v>2810</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>2811</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>2811</v>
+        <v>3038</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>2812</v>
@@ -13357,19 +13607,19 @@
         <v>2810</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>2867</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>2867</v>
+        <v>3063</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>2817</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>2813</v>
@@ -13392,19 +13642,19 @@
         <v>2810</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>2864</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>2864</v>
+        <v>3062</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>2912</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>2925</v>
@@ -13427,19 +13677,19 @@
         <v>2851</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>2811</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>2811</v>
+        <v>3038</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>2817</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>2813</v>
@@ -13462,7 +13712,7 @@
         <v>2810</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>2860</v>
@@ -13474,7 +13724,7 @@
         <v>2817</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>2926</v>
@@ -13497,7 +13747,7 @@
         <v>2810</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>2858</v>
@@ -13509,7 +13759,7 @@
         <v>2817</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>2927</v>
@@ -13532,13 +13782,13 @@
         <v>2810</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>2868</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>2868</v>
+        <v>3041</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>2812</v>
@@ -13567,13 +13817,13 @@
         <v>2852</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>2869</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>2869</v>
+        <v>3050</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>2910</v>
@@ -13602,19 +13852,19 @@
         <v>2810</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>2870</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>2870</v>
+        <v>3046</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>2912</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>2813</v>
@@ -13637,7 +13887,7 @@
         <v>2810</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>2858</v>
@@ -13672,7 +13922,7 @@
         <v>2852</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>2816</v>
@@ -13707,7 +13957,7 @@
         <v>2810</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>2860</v>
@@ -13719,7 +13969,7 @@
         <v>2817</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>2918</v>
@@ -13742,7 +13992,7 @@
         <v>2851</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>2858</v>
@@ -13777,13 +14027,13 @@
         <v>2852</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>2811</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>2811</v>
+        <v>3038</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>2812</v>
@@ -13812,7 +14062,7 @@
         <v>2852</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>2858</v>
@@ -13824,7 +14074,7 @@
         <v>2817</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>2924</v>
@@ -13847,13 +14097,13 @@
         <v>2851</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>2811</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>2811</v>
+        <v>3038</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>2812</v>
@@ -13882,13 +14132,13 @@
         <v>2851</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>2811</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>2811</v>
+        <v>3038</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>2812</v>
@@ -13917,13 +14167,13 @@
         <v>2852</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>2871</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>2871</v>
+        <v>3064</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>2812</v>
@@ -13952,13 +14202,13 @@
         <v>2851</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>2861</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>2861</v>
+        <v>3048</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>2910</v>
@@ -13987,13 +14237,13 @@
         <v>2852</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>2811</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>2811</v>
+        <v>3038</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>2910</v>
@@ -14022,7 +14272,7 @@
         <v>2853</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>2853</v>
+        <v>3011</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>2816</v>
@@ -14034,7 +14284,7 @@
         <v>2817</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>2917</v>
@@ -14057,7 +14307,7 @@
         <v>2853</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>2853</v>
+        <v>3011</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>2872</v>
@@ -14069,7 +14319,7 @@
         <v>2817</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>2917</v>
@@ -14092,7 +14342,7 @@
         <v>2854</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>2854</v>
+        <v>3006</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>2816</v>
@@ -14104,7 +14354,7 @@
         <v>2817</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>2917</v>
@@ -14127,7 +14377,7 @@
         <v>2853</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>2853</v>
+        <v>3011</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>2872</v>
@@ -14139,7 +14389,7 @@
         <v>2817</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>2917</v>
@@ -14162,7 +14412,7 @@
         <v>2854</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>2854</v>
+        <v>3006</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>2816</v>
@@ -14174,7 +14424,7 @@
         <v>2817</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>2917</v>
@@ -14197,19 +14447,19 @@
         <v>2853</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>2853</v>
+        <v>3011</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>2873</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>2873</v>
+        <v>3065</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>2817</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>2930</v>
@@ -14228,11 +14478,17 @@
       <c r="B53" s="1" t="s">
         <v>455</v>
       </c>
+      <c r="E53" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F53" s="1" t="s">
         <v>2874</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>2874</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>2931</v>
@@ -14248,11 +14504,17 @@
       <c r="B54" s="1" t="s">
         <v>456</v>
       </c>
+      <c r="E54" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F54" s="1" t="s">
         <v>2874</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>2874</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>2931</v>
@@ -14268,11 +14530,17 @@
       <c r="B55" s="1" t="s">
         <v>457</v>
       </c>
+      <c r="E55" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F55" s="1" t="s">
         <v>2875</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>2875</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>2928</v>
@@ -14288,11 +14556,17 @@
       <c r="B56" s="1" t="s">
         <v>458</v>
       </c>
+      <c r="E56" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F56" s="1" t="s">
         <v>2874</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>2874</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>2929</v>
@@ -14308,11 +14582,17 @@
       <c r="B57" s="1" t="s">
         <v>459</v>
       </c>
+      <c r="E57" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F57" s="1" t="s">
         <v>2876</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>2876</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>2931</v>
@@ -14328,11 +14608,17 @@
       <c r="B58" s="1" t="s">
         <v>460</v>
       </c>
+      <c r="E58" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F58" s="1" t="s">
         <v>2877</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>2877</v>
+        <v>3029</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>2932</v>
@@ -14348,11 +14634,17 @@
       <c r="B59" s="1" t="s">
         <v>461</v>
       </c>
+      <c r="E59" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F59" s="1" t="s">
         <v>2874</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>2874</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>2931</v>
@@ -14368,11 +14660,17 @@
       <c r="B60" s="1" t="s">
         <v>462</v>
       </c>
+      <c r="E60" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F60" s="1" t="s">
         <v>2874</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>2874</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>2933</v>
@@ -14388,11 +14686,17 @@
       <c r="B61" s="1" t="s">
         <v>463</v>
       </c>
+      <c r="E61" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F61" s="1" t="s">
         <v>2876</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>2876</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>2931</v>
@@ -14408,11 +14712,17 @@
       <c r="B62" s="1" t="s">
         <v>464</v>
       </c>
+      <c r="E62" s="1" t="s">
+        <v>3072</v>
+      </c>
       <c r="F62" s="1" t="s">
         <v>2874</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>2874</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>3073</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>2929</v>
@@ -14428,11 +14738,23 @@
       <c r="B63" s="1" t="s">
         <v>465</v>
       </c>
+      <c r="E63" s="1" t="s">
+        <v>3083</v>
+      </c>
       <c r="F63" s="1" t="s">
         <v>2878</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>2878</v>
+        <v>3051</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>2812</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.45">
@@ -14442,11 +14764,23 @@
       <c r="B64" s="1" t="s">
         <v>466</v>
       </c>
+      <c r="E64" s="1" t="s">
+        <v>2992</v>
+      </c>
       <c r="F64" s="1" t="s">
         <v>2879</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>2879</v>
+        <v>3052</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>3076</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.45">
@@ -14456,11 +14790,23 @@
       <c r="B65" s="1" t="s">
         <v>467</v>
       </c>
+      <c r="E65" s="1" t="s">
+        <v>3082</v>
+      </c>
       <c r="F65" s="1" t="s">
         <v>2880</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>2880</v>
+        <v>3074</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>3078</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>3077</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>3077</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.45">
@@ -14470,11 +14816,23 @@
       <c r="B66" s="1" t="s">
         <v>468</v>
       </c>
+      <c r="E66" s="1" t="s">
+        <v>3083</v>
+      </c>
       <c r="F66" s="1" t="s">
         <v>2881</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>2881</v>
+        <v>3075</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>2812</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.45">
@@ -14484,11 +14842,23 @@
       <c r="B67" s="1" t="s">
         <v>469</v>
       </c>
+      <c r="E67" s="1" t="s">
+        <v>3083</v>
+      </c>
       <c r="F67" s="1" t="s">
         <v>2879</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>2879</v>
+        <v>3052</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>2812</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.45">
@@ -14498,11 +14868,23 @@
       <c r="B68" s="1" t="s">
         <v>470</v>
       </c>
+      <c r="E68" s="1" t="s">
+        <v>3081</v>
+      </c>
       <c r="F68" s="1" t="s">
         <v>2858</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>2858</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>2812</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>3079</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>3080</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.45">
@@ -14516,7 +14898,7 @@
         <v>2851</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>2858</v>
@@ -14551,7 +14933,7 @@
         <v>2849</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>2860</v>
@@ -14563,7 +14945,7 @@
         <v>2817</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>2920</v>
@@ -14586,13 +14968,13 @@
         <v>2852</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>2882</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>2882</v>
+        <v>3053</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>2910</v>
@@ -14621,7 +15003,7 @@
         <v>2810</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>2860</v>
@@ -14656,7 +15038,7 @@
         <v>2849</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>2858</v>
@@ -14668,7 +15050,7 @@
         <v>2912</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>2917</v>
@@ -14691,13 +15073,13 @@
         <v>2852</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>2883</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>2883</v>
+        <v>3054</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>2812</v>
@@ -14726,13 +15108,13 @@
         <v>2810</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>2870</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>2870</v>
+        <v>3042</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>2812</v>
@@ -14761,7 +15143,7 @@
         <v>2810</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>2816</v>
@@ -14773,7 +15155,7 @@
         <v>2817</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>2934</v>
@@ -14796,7 +15178,7 @@
         <v>2851</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>2884</v>
@@ -14808,7 +15190,7 @@
         <v>2817</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>2935</v>
@@ -14831,19 +15213,19 @@
         <v>2849</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>2885</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>2885</v>
+        <v>3055</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>2912</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>2813</v>
@@ -14866,7 +15248,7 @@
         <v>2851</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>2816</v>
@@ -14878,7 +15260,7 @@
         <v>2912</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>2936</v>
@@ -14901,7 +15283,7 @@
         <v>2851</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>2858</v>
@@ -14936,7 +15318,7 @@
         <v>2851</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>2872</v>
@@ -14948,7 +15330,7 @@
         <v>2914</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>2914</v>
+        <v>3035</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>2917</v>
@@ -14971,7 +15353,7 @@
         <v>2851</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>2886</v>
@@ -14983,7 +15365,7 @@
         <v>2911</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>2917</v>
@@ -15006,7 +15388,7 @@
         <v>2851</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>2887</v>
@@ -15018,7 +15400,7 @@
         <v>2913</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>2913</v>
+        <v>3034</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>2917</v>
@@ -15041,7 +15423,7 @@
         <v>2851</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>2816</v>
@@ -15053,7 +15435,7 @@
         <v>2817</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>2937</v>
@@ -15076,19 +15458,19 @@
         <v>2851</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>2888</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>2888</v>
+        <v>3043</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>2911</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>2813</v>
@@ -15111,7 +15493,7 @@
         <v>2851</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>2858</v>
@@ -15146,7 +15528,7 @@
         <v>2851</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>2889</v>
@@ -15158,7 +15540,7 @@
         <v>2817</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>2939</v>
@@ -15181,7 +15563,7 @@
         <v>2810</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>2858</v>
@@ -15193,7 +15575,7 @@
         <v>2817</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>2940</v>
@@ -15216,7 +15598,7 @@
         <v>2851</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>2816</v>
@@ -15228,7 +15610,7 @@
         <v>2817</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>2941</v>
@@ -15251,7 +15633,7 @@
         <v>2849</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>2858</v>
@@ -15286,7 +15668,7 @@
         <v>2852</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>2860</v>
@@ -15298,7 +15680,7 @@
         <v>2913</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>2913</v>
+        <v>3034</v>
       </c>
       <c r="J91" s="1" t="s">
         <v>2917</v>
@@ -15321,13 +15703,13 @@
         <v>2852</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>2890</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>2890</v>
+        <v>3044</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>2812</v>
@@ -15356,7 +15738,7 @@
         <v>2849</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>2858</v>
@@ -15368,7 +15750,7 @@
         <v>2912</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>2917</v>
@@ -15391,7 +15773,7 @@
         <v>2849</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>2860</v>
@@ -15403,7 +15785,7 @@
         <v>2817</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>2942</v>
@@ -15426,7 +15808,7 @@
         <v>2851</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>2860</v>
@@ -15461,7 +15843,7 @@
         <v>2851</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>2816</v>
@@ -15496,7 +15878,7 @@
         <v>2810</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>2858</v>
@@ -15508,7 +15890,7 @@
         <v>2912</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J97" s="1" t="s">
         <v>2917</v>
@@ -15531,7 +15913,7 @@
         <v>2851</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>2872</v>
@@ -15543,7 +15925,7 @@
         <v>2914</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>2914</v>
+        <v>3035</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>2917</v>
@@ -15566,19 +15948,19 @@
         <v>2851</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>2891</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>2891</v>
+        <v>3056</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>2817</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>2813</v>
@@ -15601,13 +15983,13 @@
         <v>2852</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>2892</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>2892</v>
+        <v>3057</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>2910</v>
@@ -15636,13 +16018,13 @@
         <v>2852</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>2892</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>2892</v>
+        <v>3057</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>2910</v>
@@ -15671,13 +16053,13 @@
         <v>2852</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>2892</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>2892</v>
+        <v>3057</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>2910</v>
@@ -15706,7 +16088,7 @@
         <v>2810</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>2860</v>
@@ -15718,7 +16100,7 @@
         <v>2912</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J103" s="1" t="s">
         <v>2917</v>
@@ -15741,7 +16123,7 @@
         <v>2850</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>2850</v>
+        <v>3067</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>2872</v>
@@ -15753,7 +16135,7 @@
         <v>2914</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>2914</v>
+        <v>3035</v>
       </c>
       <c r="J104" s="1" t="s">
         <v>2942</v>
@@ -15776,7 +16158,7 @@
         <v>2851</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>2866</v>
@@ -15811,19 +16193,19 @@
         <v>2851</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>2811</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>2811</v>
+        <v>3038</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>2817</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>2813</v>
@@ -15846,7 +16228,7 @@
         <v>2850</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>2850</v>
+        <v>3067</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>2858</v>
@@ -15858,7 +16240,7 @@
         <v>2817</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J107" s="1" t="s">
         <v>2945</v>
@@ -15881,7 +16263,7 @@
         <v>2851</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>2860</v>
@@ -15893,7 +16275,7 @@
         <v>2817</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J108" s="1" t="s">
         <v>2917</v>
@@ -15916,7 +16298,7 @@
         <v>2850</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>2850</v>
+        <v>3067</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>2816</v>
@@ -15928,7 +16310,7 @@
         <v>2817</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J109" s="1" t="s">
         <v>2940</v>
@@ -15951,7 +16333,7 @@
         <v>2810</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>2858</v>
@@ -15986,7 +16368,7 @@
         <v>2851</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>2893</v>
@@ -15998,7 +16380,7 @@
         <v>2817</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J111" s="1" t="s">
         <v>2917</v>
@@ -16021,7 +16403,7 @@
         <v>2849</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>2864</v>
@@ -16056,7 +16438,7 @@
         <v>2810</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>2816</v>
@@ -16091,7 +16473,7 @@
         <v>2852</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>2816</v>
@@ -16103,7 +16485,7 @@
         <v>2817</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J114" s="1" t="s">
         <v>2917</v>
@@ -16126,7 +16508,7 @@
         <v>2851</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>2893</v>
@@ -16138,7 +16520,7 @@
         <v>2817</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J115" s="1" t="s">
         <v>2917</v>
@@ -16161,7 +16543,7 @@
         <v>2851</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>2858</v>
@@ -16173,7 +16555,7 @@
         <v>2911</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J116" s="1" t="s">
         <v>2917</v>
@@ -16196,19 +16578,19 @@
         <v>2851</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>2893</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>2893</v>
+        <v>3037</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>2817</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J117" s="1" t="s">
         <v>2917</v>
@@ -16231,7 +16613,7 @@
         <v>2810</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>2860</v>
@@ -16243,7 +16625,7 @@
         <v>2911</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J118" s="1" t="s">
         <v>2947</v>
@@ -16266,7 +16648,7 @@
         <v>2851</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>2858</v>
@@ -16301,7 +16683,7 @@
         <v>2810</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>2860</v>
@@ -16313,7 +16695,7 @@
         <v>2915</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>2915</v>
+        <v>3030</v>
       </c>
       <c r="J120" s="1" t="s">
         <v>2948</v>
@@ -16336,7 +16718,7 @@
         <v>2849</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>2860</v>
@@ -16371,13 +16753,13 @@
         <v>2852</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>2894</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>2894</v>
+        <v>3045</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>2812</v>
@@ -16406,7 +16788,7 @@
         <v>2810</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>2858</v>
@@ -16441,7 +16823,7 @@
         <v>2851</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>2816</v>
@@ -16453,7 +16835,7 @@
         <v>2817</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J124" s="1" t="s">
         <v>2949</v>
@@ -16476,7 +16858,7 @@
         <v>2810</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>2860</v>
@@ -16488,7 +16870,7 @@
         <v>2911</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J125" s="1" t="s">
         <v>2947</v>
@@ -16511,7 +16893,7 @@
         <v>2852</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>2866</v>
@@ -16546,7 +16928,7 @@
         <v>2850</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>2850</v>
+        <v>3067</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>2860</v>
@@ -16558,7 +16940,7 @@
         <v>2916</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>2916</v>
+        <v>3036</v>
       </c>
       <c r="J127" s="1" t="s">
         <v>2950</v>
@@ -16581,7 +16963,7 @@
         <v>2851</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>2893</v>
@@ -16593,7 +16975,7 @@
         <v>2817</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J128" s="1" t="s">
         <v>2917</v>
@@ -16616,7 +16998,7 @@
         <v>2851</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>2893</v>
@@ -16628,7 +17010,7 @@
         <v>2817</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J129" s="1" t="s">
         <v>2917</v>
@@ -16651,7 +17033,7 @@
         <v>2852</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>2858</v>
@@ -16663,7 +17045,7 @@
         <v>2817</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J130" s="1" t="s">
         <v>2917</v>
@@ -16686,7 +17068,7 @@
         <v>2851</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>2816</v>
@@ -16721,7 +17103,7 @@
         <v>2852</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>2816</v>
@@ -16733,7 +17115,7 @@
         <v>2817</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J132" s="1" t="s">
         <v>2917</v>
@@ -16756,7 +17138,7 @@
         <v>2851</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>2858</v>
@@ -16768,7 +17150,7 @@
         <v>2912</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J133" s="1" t="s">
         <v>2946</v>
@@ -16791,7 +17173,7 @@
         <v>2851</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>2893</v>
@@ -16803,7 +17185,7 @@
         <v>2817</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>2917</v>
@@ -16826,7 +17208,7 @@
         <v>2850</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>2850</v>
+        <v>3067</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>2816</v>
@@ -16861,13 +17243,13 @@
         <v>2851</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>2895</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>2895</v>
+        <v>3058</v>
       </c>
       <c r="H136" s="1" t="s">
         <v>2812</v>
@@ -16896,7 +17278,7 @@
         <v>2849</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>2858</v>
@@ -16908,7 +17290,7 @@
         <v>2912</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J137" s="1" t="s">
         <v>2917</v>
@@ -16931,7 +17313,7 @@
         <v>2810</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>2858</v>
@@ -16966,7 +17348,7 @@
         <v>2851</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>2816</v>
@@ -16978,7 +17360,7 @@
         <v>2817</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J139" s="1" t="s">
         <v>2952</v>
@@ -17001,7 +17383,7 @@
         <v>2849</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>2849</v>
+        <v>3070</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>2860</v>
@@ -17013,7 +17395,7 @@
         <v>2817</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J140" s="1" t="s">
         <v>2918</v>
@@ -17036,7 +17418,7 @@
         <v>2851</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>2858</v>
@@ -17071,7 +17453,7 @@
         <v>2810</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>2860</v>
@@ -17106,19 +17488,19 @@
         <v>2851</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>2891</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>2891</v>
+        <v>3056</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>2817</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J143" s="1" t="s">
         <v>2813</v>
@@ -17141,7 +17523,7 @@
         <v>2851</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>2860</v>
@@ -17153,7 +17535,7 @@
         <v>2817</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J144" s="1" t="s">
         <v>2953</v>
@@ -17176,7 +17558,7 @@
         <v>2851</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>2866</v>
@@ -17188,7 +17570,7 @@
         <v>2817</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J145" s="1" t="s">
         <v>2954</v>
@@ -17211,7 +17593,7 @@
         <v>2852</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>2858</v>
@@ -17223,7 +17605,7 @@
         <v>2911</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J146" s="1" t="s">
         <v>2917</v>
@@ -17246,13 +17628,13 @@
         <v>2851</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>2896</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>2896</v>
+        <v>3059</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>2910</v>
@@ -17281,7 +17663,7 @@
         <v>2810</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>2860</v>
@@ -17316,7 +17698,7 @@
         <v>2851</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>2893</v>
@@ -17328,7 +17710,7 @@
         <v>2817</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J149" s="1" t="s">
         <v>2917</v>
@@ -17351,7 +17733,7 @@
         <v>2810</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>2858</v>
@@ -17386,7 +17768,7 @@
         <v>2810</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>2858</v>
@@ -17398,7 +17780,7 @@
         <v>2912</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J151" s="1" t="s">
         <v>2917</v>
@@ -17421,7 +17803,7 @@
         <v>2851</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>2872</v>
@@ -17433,7 +17815,7 @@
         <v>2914</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>2914</v>
+        <v>3035</v>
       </c>
       <c r="J152" s="1" t="s">
         <v>2917</v>
@@ -17456,7 +17838,7 @@
         <v>2852</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>2816</v>
@@ -17468,7 +17850,7 @@
         <v>2817</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J153" s="1" t="s">
         <v>2917</v>
@@ -17491,13 +17873,13 @@
         <v>2852</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>2895</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>2895</v>
+        <v>3058</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>2910</v>
@@ -17526,7 +17908,7 @@
         <v>2810</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>2858</v>
@@ -17538,7 +17920,7 @@
         <v>2817</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J155" s="1" t="s">
         <v>2955</v>
@@ -17561,7 +17943,7 @@
         <v>2852</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>2897</v>
@@ -17596,7 +17978,7 @@
         <v>2851</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>2866</v>
@@ -17608,7 +17990,7 @@
         <v>2911</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J157" s="1" t="s">
         <v>2918</v>
@@ -17631,13 +18013,13 @@
         <v>2851</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>2898</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>2898</v>
+        <v>3046</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>2812</v>
@@ -17666,7 +18048,7 @@
         <v>2851</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>2860</v>
@@ -17701,7 +18083,7 @@
         <v>2851</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>2858</v>
@@ -17736,7 +18118,7 @@
         <v>2810</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>2816</v>
@@ -17771,7 +18153,7 @@
         <v>2851</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>2858</v>
@@ -17783,7 +18165,7 @@
         <v>2817</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J162" s="1" t="s">
         <v>2944</v>
@@ -17806,7 +18188,7 @@
         <v>2810</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>2858</v>
@@ -17818,7 +18200,7 @@
         <v>2817</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J163" s="1" t="s">
         <v>2951</v>
@@ -17841,7 +18223,7 @@
         <v>2851</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>2858</v>
@@ -17876,7 +18258,7 @@
         <v>2851</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>2860</v>
@@ -17888,7 +18270,7 @@
         <v>2817</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J165" s="1" t="s">
         <v>2940</v>
@@ -17911,7 +18293,7 @@
         <v>2851</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>2893</v>
@@ -17923,7 +18305,7 @@
         <v>2817</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J166" s="1" t="s">
         <v>2917</v>
@@ -17946,19 +18328,19 @@
         <v>2851</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>2899</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>2899</v>
+        <v>3047</v>
       </c>
       <c r="H167" s="1" t="s">
         <v>2911</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J167" s="1" t="s">
         <v>2813</v>
@@ -17981,7 +18363,7 @@
         <v>2851</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>2851</v>
+        <v>3068</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>2893</v>
@@ -17993,7 +18375,7 @@
         <v>2817</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J168" s="1" t="s">
         <v>2917</v>
@@ -18016,7 +18398,7 @@
         <v>2810</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>2810</v>
+        <v>3066</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>2860</v>
@@ -18051,13 +18433,13 @@
         <v>2852</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>2852</v>
+        <v>3069</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>2890</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>2890</v>
+        <v>3044</v>
       </c>
       <c r="H170" s="1" t="s">
         <v>2812</v>
@@ -18086,7 +18468,7 @@
         <v>2855</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>2860</v>
@@ -18098,7 +18480,7 @@
         <v>2911</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J171" s="1" t="s">
         <v>2927</v>
@@ -18121,7 +18503,7 @@
         <v>2855</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>2816</v>
@@ -18133,7 +18515,7 @@
         <v>2817</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>2817</v>
+        <v>3032</v>
       </c>
       <c r="J172" s="1" t="s">
         <v>2940</v>
@@ -18156,7 +18538,7 @@
         <v>2855</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>2860</v>
@@ -18191,7 +18573,7 @@
         <v>2855</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>2872</v>
@@ -18226,7 +18608,7 @@
         <v>2854</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>2854</v>
+        <v>3006</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>2900</v>
@@ -18238,7 +18620,7 @@
         <v>2911</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>2911</v>
+        <v>3031</v>
       </c>
       <c r="J175" s="1" t="s">
         <v>2927</v>
@@ -18261,7 +18643,7 @@
         <v>2855</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>2860</v>
@@ -18296,7 +18678,7 @@
         <v>2854</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>2854</v>
+        <v>3006</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>2860</v>
@@ -18331,7 +18713,7 @@
         <v>2856</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>2856</v>
+        <v>3071</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>2858</v>
@@ -18366,7 +18748,7 @@
         <v>2855</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>2860</v>
@@ -18401,7 +18783,7 @@
         <v>2855</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>2860</v>
@@ -18436,7 +18818,7 @@
         <v>2854</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>2854</v>
+        <v>3006</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>2816</v>
@@ -18471,7 +18853,7 @@
         <v>2854</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>2854</v>
+        <v>3006</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>2858</v>
@@ -18483,7 +18865,7 @@
         <v>2912</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>2912</v>
+        <v>3033</v>
       </c>
       <c r="J182" s="1" t="s">
         <v>2944</v>
@@ -18506,7 +18888,7 @@
         <v>2855</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>2816</v>
@@ -18541,7 +18923,7 @@
         <v>2855</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>2855</v>
+        <v>2992</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>2858</v>
@@ -18584,6 +18966,12 @@
       <c r="G185" s="1" t="s">
         <v>2858</v>
       </c>
+      <c r="I185" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K185" s="1" t="s">
+        <v>3084</v>
+      </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A186" s="12">
@@ -18604,6 +18992,12 @@
       <c r="G186" s="1" t="s">
         <v>2901</v>
       </c>
+      <c r="I186" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>2917</v>
+      </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A187" s="12">
@@ -18624,6 +19018,12 @@
       <c r="G187" s="1" t="s">
         <v>3023</v>
       </c>
+      <c r="I187" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K187" s="1" t="s">
+        <v>3084</v>
+      </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A188" s="12">
@@ -18644,6 +19044,12 @@
       <c r="G188" s="1" t="s">
         <v>2858</v>
       </c>
+      <c r="I188" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>2917</v>
+      </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A189" s="12">
@@ -18664,6 +19070,12 @@
       <c r="G189" s="1" t="s">
         <v>2901</v>
       </c>
+      <c r="I189" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K189" s="1" t="s">
+        <v>2917</v>
+      </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A190" s="12">
@@ -18684,6 +19096,12 @@
       <c r="G190" s="1" t="s">
         <v>3024</v>
       </c>
+      <c r="I190" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K190" s="1" t="s">
+        <v>3085</v>
+      </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A191" s="12">
@@ -18704,6 +19122,12 @@
       <c r="G191" s="1" t="s">
         <v>2904</v>
       </c>
+      <c r="I191" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K191" s="1" t="s">
+        <v>2998</v>
+      </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A192" s="12">
@@ -18724,8 +19148,14 @@
       <c r="G192" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I192" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K192" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A193" s="12">
         <v>192</v>
       </c>
@@ -18744,8 +19174,14 @@
       <c r="G193" s="1" t="s">
         <v>3025</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I193" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K193" s="1" t="s">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A194" s="12">
         <v>193</v>
       </c>
@@ -18764,8 +19200,14 @@
       <c r="G194" s="1" t="s">
         <v>2901</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I194" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K194" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A195" s="12">
         <v>194</v>
       </c>
@@ -18784,8 +19226,14 @@
       <c r="G195" s="1" t="s">
         <v>3026</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I195" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K195" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A196" s="12">
         <v>195</v>
       </c>
@@ -18804,8 +19252,14 @@
       <c r="G196" s="1" t="s">
         <v>3026</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I196" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K196" s="1" t="s">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A197" s="12">
         <v>196</v>
       </c>
@@ -18824,8 +19278,14 @@
       <c r="G197" s="1" t="s">
         <v>3025</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I197" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K197" s="1" t="s">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A198" s="12">
         <v>197</v>
       </c>
@@ -18844,8 +19304,14 @@
       <c r="G198" s="1" t="s">
         <v>3026</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I198" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K198" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A199" s="12">
         <v>198</v>
       </c>
@@ -18864,8 +19330,14 @@
       <c r="G199" s="1" t="s">
         <v>2816</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I199" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K199" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A200" s="12">
         <v>199</v>
       </c>
@@ -18884,8 +19356,14 @@
       <c r="G200" s="1" t="s">
         <v>3026</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I200" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K200" s="1" t="s">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A201" s="12">
         <v>200</v>
       </c>
@@ -18904,8 +19382,14 @@
       <c r="G201" s="1" t="s">
         <v>3025</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I201" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K201" s="1" t="s">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A202" s="12">
         <v>201</v>
       </c>
@@ -18924,8 +19408,14 @@
       <c r="G202" s="1" t="s">
         <v>3026</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I202" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K202" s="1" t="s">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A203" s="12">
         <v>202</v>
       </c>
@@ -18944,8 +19434,14 @@
       <c r="G203" s="1" t="s">
         <v>3026</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I203" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K203" s="1" t="s">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A204" s="12">
         <v>203</v>
       </c>
@@ -18964,8 +19460,14 @@
       <c r="G204" s="1" t="s">
         <v>3025</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I204" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K204" s="1" t="s">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A205" s="12">
         <v>204</v>
       </c>
@@ -18984,8 +19486,14 @@
       <c r="G205" s="1" t="s">
         <v>3026</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I205" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K205" s="1" t="s">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A206" s="12">
         <v>205</v>
       </c>
@@ -19004,8 +19512,14 @@
       <c r="G206" s="1" t="s">
         <v>2904</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I206" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K206" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A207" s="12">
         <v>206</v>
       </c>
@@ -19024,8 +19538,14 @@
       <c r="G207" s="1" t="s">
         <v>3026</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I207" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K207" s="1" t="s">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A208" s="12">
         <v>207</v>
       </c>
@@ -19044,8 +19564,14 @@
       <c r="G208" s="1" t="s">
         <v>2907</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I208" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K208" s="1" t="s">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A209" s="12">
         <v>208</v>
       </c>
@@ -19064,8 +19590,14 @@
       <c r="G209" s="1" t="s">
         <v>2907</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I209" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K209" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A210" s="12">
         <v>209</v>
       </c>
@@ -19084,8 +19616,14 @@
       <c r="G210" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I210" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K210" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A211" s="12">
         <v>210</v>
       </c>
@@ -19104,8 +19642,14 @@
       <c r="G211" s="1" t="s">
         <v>2860</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I211" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K211" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A212" s="12">
         <v>211</v>
       </c>
@@ -19124,8 +19668,14 @@
       <c r="G212" s="1" t="s">
         <v>2901</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I212" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K212" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A213" s="12">
         <v>212</v>
       </c>
@@ -19144,8 +19694,14 @@
       <c r="G213" s="1" t="s">
         <v>2816</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I213" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K213" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A214" s="12">
         <v>213</v>
       </c>
@@ -19164,8 +19720,14 @@
       <c r="G214" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I214" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K214" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A215" s="12">
         <v>214</v>
       </c>
@@ -19184,8 +19746,14 @@
       <c r="G215" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I215" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K215" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A216" s="12">
         <v>215</v>
       </c>
@@ -19202,10 +19770,16 @@
         <v>2908</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>2908</v>
-      </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.45">
+        <v>3027</v>
+      </c>
+      <c r="I216" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K216" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A217" s="12">
         <v>216</v>
       </c>
@@ -19224,8 +19798,14 @@
       <c r="G217" s="1" t="s">
         <v>2901</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I217" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K217" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A218" s="12">
         <v>217</v>
       </c>
@@ -19244,8 +19824,14 @@
       <c r="G218" s="1" t="s">
         <v>2901</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I218" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K218" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A219" s="12">
         <v>218</v>
       </c>
@@ -19264,8 +19850,14 @@
       <c r="G219" s="1" t="s">
         <v>2904</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I219" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K219" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A220" s="12">
         <v>219</v>
       </c>
@@ -19284,8 +19876,14 @@
       <c r="G220" s="1" t="s">
         <v>2904</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I220" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K220" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A221" s="12">
         <v>220</v>
       </c>
@@ -19304,8 +19902,14 @@
       <c r="G221" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I221" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K221" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A222" s="12">
         <v>221</v>
       </c>
@@ -19324,8 +19928,14 @@
       <c r="G222" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I222" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K222" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A223" s="12">
         <v>222</v>
       </c>
@@ -19344,8 +19954,14 @@
       <c r="G223" s="1" t="s">
         <v>2901</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I223" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K223" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A224" s="12">
         <v>223</v>
       </c>
@@ -19364,8 +19980,14 @@
       <c r="G224" s="1" t="s">
         <v>2907</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I224" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K224" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A225" s="12">
         <v>224</v>
       </c>
@@ -19384,8 +20006,14 @@
       <c r="G225" s="1" t="s">
         <v>2907</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I225" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K225" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A226" s="12">
         <v>225</v>
       </c>
@@ -19404,8 +20032,14 @@
       <c r="G226" s="1" t="s">
         <v>2816</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I226" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K226" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A227" s="12">
         <v>226</v>
       </c>
@@ -19424,8 +20058,14 @@
       <c r="G227" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I227" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K227" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A228" s="12">
         <v>227</v>
       </c>
@@ -19444,8 +20084,14 @@
       <c r="G228" s="1" t="s">
         <v>2816</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I228" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K228" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A229" s="12">
         <v>228</v>
       </c>
@@ -19464,8 +20110,14 @@
       <c r="G229" s="1" t="s">
         <v>2909</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I229" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K229" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A230" s="12">
         <v>229</v>
       </c>
@@ -19484,8 +20136,14 @@
       <c r="G230" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I230" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K230" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A231" s="12">
         <v>230</v>
       </c>
@@ -19504,8 +20162,14 @@
       <c r="G231" s="1" t="s">
         <v>2904</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I231" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K231" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A232" s="12">
         <v>231</v>
       </c>
@@ -19524,8 +20188,14 @@
       <c r="G232" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I232" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K232" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A233" s="12">
         <v>232</v>
       </c>
@@ -19544,8 +20214,14 @@
       <c r="G233" s="1" t="s">
         <v>2858</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I233" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K233" s="1" t="s">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A234" s="12">
         <v>233</v>
       </c>
@@ -19563,6 +20239,12 @@
       </c>
       <c r="G234" s="1" t="s">
         <v>2907</v>
+      </c>
+      <c r="I234" s="1" t="s">
+        <v>3028</v>
+      </c>
+      <c r="K234" s="1" t="s">
+        <v>2917</v>
       </c>
     </row>
   </sheetData>
@@ -19950,10 +20632,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B193"/>
+  <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19963,15 +20645,48 @@
     <col min="3" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="3" t="s">
+        <v>2803</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2804</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>2845</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3089</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3090</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2806</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2847</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>2807</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>2848</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>2808</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -19979,7 +20694,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -19987,7 +20702,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -19995,7 +20710,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -20003,7 +20718,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -20011,7 +20726,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -20019,7 +20734,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -20027,7 +20742,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -20035,7 +20750,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -20043,7 +20758,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -20051,7 +20766,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -20059,7 +20774,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -20067,7 +20782,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -20075,7 +20790,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -20083,7 +20798,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Several design improvements and fixes
- Now shrinks text in specific fields on character sheet
- Fixed combat technique values of newer professions
- Unified RCP views
- Added RCP info views
- Fixed routine check modifiers on character sheet
</commit_message>
<xml_diff>
--- a/src/data/TDE5_de-DE.xlsx
+++ b/src/data/TDE5_de-DE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="30" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5264" uniqueCount="3091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5440" uniqueCount="3223">
   <si>
     <t>id</t>
   </si>
@@ -9328,6 +9328,402 @@
   </si>
   <si>
     <t>kpcostShort</t>
+  </si>
+  <si>
+    <t>areaKnowledgeShort</t>
+  </si>
+  <si>
+    <t>areaKnowledge</t>
+  </si>
+  <si>
+    <t>commonMundaneProfessions</t>
+  </si>
+  <si>
+    <t>commonMagicalProfessions</t>
+  </si>
+  <si>
+    <t>commonBlessedProfessions</t>
+  </si>
+  <si>
+    <t>commonNames</t>
+  </si>
+  <si>
+    <t>Heimat</t>
+  </si>
+  <si>
+    <t>je nach Heimatort (z.B. Andergast-Stadt, Joborn)</t>
+  </si>
+  <si>
+    <t>alle außer Gladiatoren und Stammeskrieger</t>
+  </si>
+  <si>
+    <t>Hexe, Magier</t>
+  </si>
+  <si>
+    <t>Borongeweihte, Hesindegeweihte, Perainegeweihte, Phexgeweihte, Praiosgeweihte, Rondrageweihte</t>
+  </si>
+  <si>
+    <t>Richtungssinn, Zäher Hund</t>
+  </si>
+  <si>
+    <t>* *männlich*: Arnbold, Borkhelm, Eichward, Gartwald, Ludewich, Marik, Strammgert, Wendolyn, Wenzelaus, Zoltan\n* *weiblich*: Andra, Berga, Domela, Ernka, Hadwiga, Irmela, Larja, Marmelunde, Trashka, Wendeline\n* *Familiennamen*: Alrikshuber, Borkmeister, Eichinger, Haubeiler, Holzgut, Kuhbauer, Marktbauer, Sattelhuber, Schweinwirt, Zibbelbart\n* *Adelsfamilien*: von Anderstein, von Borkenfeld, von Steinbaum, von Tatzenstein, von Teshkal</t>
+  </si>
+  <si>
+    <t>je nach Heimatort (z.B. Baburin, Elburum, Llanka, Palmyrabad, Zorgan)</t>
+  </si>
+  <si>
+    <t>alle ausser Ritter, Gladiator und Stammeskrieger</t>
+  </si>
+  <si>
+    <t>Hexe (vor allem Katzenhexen), Magier (selten)</t>
+  </si>
+  <si>
+    <t>Begabung in Gesellschaftstalenten, Entfernungssinn</t>
+  </si>
+  <si>
+    <t>* *männlich*: Assaf, Djafardeon, Eslam, Faizal, Kazan, Mahdul, Marwamir, Nazir, Seyychaban, Zahir\n* *weiblich*: Aischanka, Belima, Delilah, Harizeth, Majula, Neraida, Rhayadaque, Shilaldara, Yamira, Zulhaminai\n* Namen werden mit *Ibn* bei Männern und *saba* oder *-sunni* bei Frauen mit dem Namen des Vaters oder der Mutter verbunden, beispielsweise Yamira saba Delihah, Belima Majulasunni oder Assaf ibn Eslam</t>
+  </si>
+  <si>
+    <t>je nach Heimatort (z.B. Festum, Norburg, Notmark, Ouvennmas, Rodebrannt)</t>
+  </si>
+  <si>
+    <t>alle ausser Gladiatoren und Stammeskrieger</t>
+  </si>
+  <si>
+    <t>Kälteresistenz, Richtungssinn, Zäher Hund</t>
+  </si>
+  <si>
+    <t>Hitzeempfindlich, Persönlichkeitsschwächen (Vorurteile - vor allem gegen Orks, Goblins, Al'Anfaner und Norbarden), Schlechte Eigenschaft (Aberglaube)</t>
+  </si>
+  <si>
+    <t>keine</t>
+  </si>
+  <si>
+    <t>* *männlich*: Bosjew, Danow, Elkwin, Firunew, Irjan, Jaakon, Jucho, Oswin, Travin, Vito\n* *weiblich*: Alwinja, Dunjascha, Elwinja, Hesinja, Irinja, Jadvine, Karinja, Nadjescha, Rowena, Vanjescha\n* *Familiennamen*: Alwinnen, Baerow, Bornski, Firunkis, Gartimpski, Gerberow, Karenkis, Larinow, Saraski, Timpski\n* *Adelsfamilien*: von Salderkeim, von Quelldunkel, von Ouvenstam, von Wosna, von Eschenfurt</t>
+  </si>
+  <si>
+    <t>Wegstrecke</t>
+  </si>
+  <si>
+    <t>Hexe (vor allem Kröten- und Rabenhexe), Magier</t>
+  </si>
+  <si>
+    <t>Persönlichkeitsschwächen (Eitelkeit, Vorurteile - vor allem gegen Novadis und Magier), Schlechte Eigenschaften (Aberglaube), Zerbrechlich</t>
+  </si>
+  <si>
+    <t>Persönlichkeitsschwächen (Vorurteile) – vor allem gegen Nostrier und Frauen, Weltfremd – vor allem gegenüber Fortschritt, Welt außerhalb des Königreichs), Schlechte Eigenschaften (Aberglaube)</t>
+  </si>
+  <si>
+    <t>Das Gegenüber ist bereit, mehr für den Helden zu tun.</t>
+  </si>
+  <si>
+    <t>Dem Held gelingt es nicht, sein Gegenüber zu überreden.</t>
+  </si>
+  <si>
+    <t>Die Person, die der Held überreden wollte, tut weit mehr als sie muss.</t>
+  </si>
+  <si>
+    <t>Die Person, die der Held überreden wollte, ist wütend auf den Helden und lässt sich in nächster Zeit nicht mehr überreden.</t>
+  </si>
+  <si>
+    <t>Die Verkleidung ist schwerer zu durchschauen.</t>
+  </si>
+  <si>
+    <t>Die Verkleidung ist nicht gut gewählt und hält einem prüfenden Blick nicht stand.</t>
+  </si>
+  <si>
+    <t>Die Verkleidung funktioniert tadellos.</t>
+  </si>
+  <si>
+    <t>Die Kleidung wird sofort durchschaut und der Held handelt sich in der Regel Ärger ein.</t>
+  </si>
+  <si>
+    <t>Die Auswirkungen von Verführungs- oder Überredensversuchen sind deutlich abgeschwächt oder es wird ihnen ganz widerstanden.</t>
+  </si>
+  <si>
+    <t>Der Held kann nicht widerstehen.</t>
+  </si>
+  <si>
+    <t>Der Held widersteht und kann von dieser Person oder Sache in nächster Zeit nicht mehr beeinflusst werden.</t>
+  </si>
+  <si>
+    <t>Der Held ist der Person, die ihn beeinflussen will, vollkommen verfallen oder fällt bei Anblick eines scheußlichen Dämons in Ohnmacht.</t>
+  </si>
+  <si>
+    <t>über die Qualitätsstufe kann der Held mehr Details in der Fährte erkennen.</t>
+  </si>
+  <si>
+    <t>Der Held findet keine Spur oder kann keine neuen Erkenntnisse gewinnen.</t>
+  </si>
+  <si>
+    <t>Sofern die Spur nicht komplett zerstört wurde, kann der Held ihr zielsicher bis zum Ende folgen. Er erhält mehr Informationen als üblich. Täuschungsmanöver wie das Verwischen der Spuren durchschaut er sofort.</t>
+  </si>
+  <si>
+    <t>Der Held verwechselt die Spur und folgt einer falschen Fährte. So trifft er vielleicht auf eine gefährliche Kreatur oder jagt den falschen Leuten hinterher.</t>
+  </si>
+  <si>
+    <t>Die Fessel hält länger und kann gegebenenfalls schwerer geöffnet werden.</t>
+  </si>
+  <si>
+    <t>Dem Held gelingt nur ein Knoten von schlechter Qualität. Das Befreien daraus ist leichter als üblich.</t>
+  </si>
+  <si>
+    <t>Der Held hat einen stabilen Knoten gemacht. Für Qualitätsstufen, Vergleichs- und Sammelproben gilt: FP = doppelter FW.</t>
+  </si>
+  <si>
+    <t>Der Held hat einen Knoten gemacht, der sich in jeder Lage löst - oder der denkbar ungünstigsten.</t>
+  </si>
+  <si>
+    <t>Die Fische sind wohlschmeckender als bei einem durchschnittlichen Fang.</t>
+  </si>
+  <si>
+    <t>Kein Fisch beißt an oder geht ins Netz.</t>
+  </si>
+  <si>
+    <t>Die Zahl der Rationen ist sehr hoch. Für Qualitätsstufen, Vergleichs- und Sammelproben gilt: FP = doppelter FW.</t>
+  </si>
+  <si>
+    <t>Der Angler fällt ins Wasser und die Angel geht verloren.</t>
+  </si>
+  <si>
+    <t>Der Held findet schneller heraus, in welche Richtung er sich bewegt.</t>
+  </si>
+  <si>
+    <t>Der Held weiß nicht sicher, wo es langgeht.</t>
+  </si>
+  <si>
+    <t>Der Held findet den Weg ohne Schwierigkeiten selbst unter schlechtesten Bedingungen.</t>
+  </si>
+  <si>
+    <t>Der Held hat sich komplett verlaufen und bewegt sich in die falsche Richtung, was ihm jedoch nicht bewusst ist.</t>
+  </si>
+  <si>
+    <t>genauere Informationen zu einer Pflanze</t>
+  </si>
+  <si>
+    <t>Der Held hat keine Ahnung.</t>
+  </si>
+  <si>
+    <t>Der Held weiß alles über die Pflanze, auch besondere Wirkungen, und kann sie doppelt so lange haltbar machen wie üblich.</t>
+  </si>
+  <si>
+    <t>Der Held verwechselt die Pflanze mit einer anderen.</t>
+  </si>
+  <si>
+    <t>genauere Informationen zu einem Tier</t>
+  </si>
+  <si>
+    <t>Der Held weiß alles über das Tier.</t>
+  </si>
+  <si>
+    <t>Der Held glaubt, etwas über das Tier zu wissen, liegt aber gefährlich falsch (schätzt es ungiftig ein, obwohl es sehr giftig ist, oder als Pflanzenfresser, obwohl es Fleischfresser ist).</t>
+  </si>
+  <si>
+    <t>Der Held benötigt nicht so lange, um ein Lager zu finden oder aufzubauen.</t>
+  </si>
+  <si>
+    <t>Der Lagerplatz ist schlecht gewählt. Die Regeneration ist um 1 gesenkt.</t>
+  </si>
+  <si>
+    <t>Ein phantastischer Schlafplatz! Die Regeneration ist um 1 Punkt erhöht.</t>
+  </si>
+  <si>
+    <t>Das Lager wird überschwemmt oder von Ungeziefer heimgesucht.</t>
+  </si>
+  <si>
+    <t>Der Held hat einen guten Spielzug gemacht.</t>
+  </si>
+  <si>
+    <t>Der Held verliert.</t>
+  </si>
+  <si>
+    <t>Der Held gewinnt auf spektakuläre Art und Weise. Wurde um Geld gespielt, verdoppelt sich sein Gewinn.</t>
+  </si>
+  <si>
+    <t>Der Held wird fälschlicherweise des Falschspiels verdächtigt oder hat eine Pechsträne. Wird um Geld gespielt, verliert er mindestens den kompletten Einsatz (oder mehr).</t>
+  </si>
+  <si>
+    <t>mehr Detailinformationen zur Bevölkerung, Örtlichkeiten und Flussübergängen</t>
+  </si>
+  <si>
+    <t>Der Held kennt viele Details der Region: Herrscher, Bevölkerungszahlen, Bräuche, Flussverläufe und Brücken.</t>
+  </si>
+  <si>
+    <t>Der Held erinnert sich an völlig falsche geographische Details: Einwohnerzahlen von Städten stimmen nicht, Brücken befinden sich an anderer Stelle als gedacht.</t>
+  </si>
+  <si>
+    <t>mehr Details zu historischen Persönlichkeiten und Epochen</t>
+  </si>
+  <si>
+    <t>Der Held kennt besonders viele Details über ein bestimmtes Ereignis oder eine historische Person.</t>
+  </si>
+  <si>
+    <t>Der Held kann zu diesem Thema nur falsche Informationen beitragen: er irrt sich in Daten und Ereignissen.</t>
+  </si>
+  <si>
+    <t>mehr Details zu Kulten, Göttern und Priestern</t>
+  </si>
+  <si>
+    <t>Der Held hat detaillierte Einsichten in das Thema und kennt selbst spezielle Rituale, Gebetstexte oder philosophische Grundlagen.</t>
+  </si>
+  <si>
+    <t>Der Held verwechselt kultische Handlungen und Ansichten dieser Kirche mit einer anderen.</t>
+  </si>
+  <si>
+    <t>bessere Vorteile während des Gefechts</t>
+  </si>
+  <si>
+    <t>Der Held unterliegt einer Fehleinschätzung.</t>
+  </si>
+  <si>
+    <t>Der Held hat einen vortrefflichen Plan, der ihm zusätzliche Vorteile im Kampf einbringt.</t>
+  </si>
+  <si>
+    <t>Der Held begeht einen kapitalen Planungsfehler, der den Kampf zu seinen Ungunsten beeinflusst oder ihm zumindest extreme Nachteile beschert.</t>
+  </si>
+  <si>
+    <t>mehr Details zu Zaubern, magischen Wesen oder exotischer Magieanwendung</t>
+  </si>
+  <si>
+    <t>Der Held kennt Herkunft, wirkenden Zauber und Auslöser eines alten Artefaktes.</t>
+  </si>
+  <si>
+    <t>Der Held hat falsche Vorstellungen und irrt sich, sodass es zu einem gravierenden Fehlurteil kommt.</t>
+  </si>
+  <si>
+    <t>schnellere Planung</t>
+  </si>
+  <si>
+    <t>Die geplante Mechanik funktioniert nicht.</t>
+  </si>
+  <si>
+    <t>Der doppelte FW zählt als FP.</t>
+  </si>
+  <si>
+    <t>Was immer der Held konstruieren wollte: Das Objekt ist gefährlich oder die Konstruktion fällt in sich zusammen. Eine Falle wird mit größtmöglichem Erfolg ausgelöst.</t>
+  </si>
+  <si>
+    <t>schnelleres Ergebnis</t>
+  </si>
+  <si>
+    <t>Das Ergebnis ist falsch.</t>
+  </si>
+  <si>
+    <t>Schnelle und exakte Bestimmung der Lösung</t>
+  </si>
+  <si>
+    <t>Das Ergebnis ist komplett falsch, der Held aber von der Richtigkeit absolut überzeugt.</t>
+  </si>
+  <si>
+    <t>mehr Optionen zur Lösung eines Falls</t>
+  </si>
+  <si>
+    <t>Der Held kennt sich mit Besonderheiten des Gesetzes aus und kann einen Plan entwickeln, es zu seinem Vorteil auszulegen.</t>
+  </si>
+  <si>
+    <t>Die Auslegung des Gesetzes ist falsch oder der Held übersieht einen wichtigen Passus.</t>
+  </si>
+  <si>
+    <t>mehr Details oder verschiedene Versionen einer Geschichte</t>
+  </si>
+  <si>
+    <t>Der Held kennt die Legende nicht.</t>
+  </si>
+  <si>
+    <t>Der Held kann sich an viele Details der Geschichte erinnern und kennt mehrere Varianten.</t>
+  </si>
+  <si>
+    <t>Der Held verwechselt die Geschichte mit einer anderen oder meint sich an völlig andere Details zu erinnern.</t>
+  </si>
+  <si>
+    <t>mehr Details zu Sphären oder dem Limbus</t>
+  </si>
+  <si>
+    <t>Der Held weiß nichts über das spezielle Thema.</t>
+  </si>
+  <si>
+    <t>Der Held erinnert sich an bemerkenswerte Details über einen einzelnen Dämon oder den Weg in eine verborgene Globule.</t>
+  </si>
+  <si>
+    <t>Der Held unterliegt einer gefährlichen Fehleinschätzung.</t>
+  </si>
+  <si>
+    <t>schnellere Horoskoperstellung</t>
+  </si>
+  <si>
+    <t>Der Held kann sehr genau die Bewegungen der Himmelskörper berechnen.</t>
+  </si>
+  <si>
+    <t>Eine Fehleinschätzung bei einem Horoskop, einer Mondfinsternis etc.</t>
+  </si>
+  <si>
+    <t>Der Trank weist eine bessere Qualität auf.</t>
+  </si>
+  <si>
+    <t>Das Elixier ist misslungen oder eine Analyse hat kein Ergebnis gebracht.</t>
+  </si>
+  <si>
+    <t>Der Held weiß exakt, welches Elixier er vor sich hat, welche Stufe es besitzt und wie lange haltbar es ist.</t>
+  </si>
+  <si>
+    <t>Das Elixier sorgt für einen unangenehmen Nebeneffekt.</t>
+  </si>
+  <si>
+    <t>Die Distanz bis zum Ziel kann schneller überwunden werden.</t>
+  </si>
+  <si>
+    <t>Der Held kommt mit dem Boot oder Schiff kaum voran.</t>
+  </si>
+  <si>
+    <t>Der Held nutzt günstige Strömungen und Winde, um doppelt so schnell voranzukommen wie üblich.</t>
+  </si>
+  <si>
+    <t>Der Held fällt von Bord oder ein wichtiger Teil des Wasserfahrzeugs wurde beschädigt.</t>
+  </si>
+  <si>
+    <t>Das Fahrzeug bewegt isch schwerfällig oder dem Helden gelingt es nicht, es in Bewegung zu setzen.</t>
+  </si>
+  <si>
+    <t>Das Fahrzeug kommt gut voran und schafft die Strecke in Rekordzeit.</t>
+  </si>
+  <si>
+    <t>Das Fahrzeug erleidet einen Achsenbruch oder fällt während der Fahrt mitsamt dem Fahrer um, und der Held erleidet Fallschaden.</t>
+  </si>
+  <si>
+    <t>Der Held kann präziser den Preis bestimmen.</t>
+  </si>
+  <si>
+    <t>Der Held bekommt nicht so viel wie erhofft.</t>
+  </si>
+  <si>
+    <t>Der Held bekommt die Ware zu einem Spottpreis bzw. kann sie zu Wucherpreisen loswerden - ohne dass sein Handelspartner es ihm übel nimmt. Die Preiserhöhung oder der Nachlass sollte mindestens 50 % betragen.</t>
+  </si>
+  <si>
+    <t>Der Held wird über den Tisch gezogen oder der Handelspartner weigert sich, Geschäfte mit dem Helden zu machen. Die Preiserhöhung oder der Nachlass sollte mindestens 50 % betragen.</t>
+  </si>
+  <si>
+    <t>Der Held kann das Gift schneller bestimmen.</t>
+  </si>
+  <si>
+    <t>Der Held hat keine Ahnung und kennt keine Möglichkeit der Heilung.</t>
+  </si>
+  <si>
+    <t>Der Patient kann vollständig entgiftet werden, ohne dass der Held das passende Gegenmittel verwenden musste.</t>
+  </si>
+  <si>
+    <t>Der Held ordnet einen (schädlichen) Aderlass an oder hat den Patienten bei der Behandlung verletzt oder gar zusätzlich vergiftet (1W6 SP).</t>
+  </si>
+  <si>
+    <t>Die Unterdrückung des Nachteils hält länger an.</t>
+  </si>
+  <si>
+    <t>Der Held hat keine Ahnung, wie er dem Patienten helfen kann.</t>
+  </si>
+  <si>
+    <t>Der Patient kann einen Nachteil (Angst, Persönlichkeitsschwäche oder Schlechte Eigenschaft) für einen ganzen Tag unterdrücken.</t>
+  </si>
+  <si>
+    <t>Der Held hat den Patienten</t>
   </si>
 </sst>
 </file>
@@ -9447,7 +9843,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9513,6 +9909,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Erklärender Text 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
@@ -9520,40 +9932,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
-  <dxfs count="130">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="135">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -9815,6 +10194,39 @@
           <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -10189,6 +10601,59 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -10287,7 +10752,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="129"/>
+      <tableStyleElement type="headerRow" dxfId="134"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -10651,20 +11116,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="133" dataDxfId="132">
   <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <sortState ref="A2:B10">
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="125"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="131"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="130"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:M1048576" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+  <autoFilter ref="A1:M1048576" xr:uid="{00000000-0009-0000-0100-000004000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="effect" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="castingtime" dataDxfId="64"/>
+    <tableColumn id="10" xr3:uid="{D89CFCD8-0667-4532-ADCB-656E0F380FC9}" name="castingtimeShort" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="aecost" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{AA76CB3A-D16A-4989-ACEE-9057F8B23848}" name="aecostShort" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="range" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{DD92ED00-D630-4075-AFBB-75382F298664}" name="rangeShort" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="duration" dataDxfId="58"/>
+    <tableColumn id="13" xr3:uid="{35897220-D86D-43E4-9246-750CE8AD5E3B}" name="durationShort" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="target" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="src" dataDxfId="55"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table14" displayName="Table14" ref="A1:B44" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:B44" xr:uid="{00000000-0009-0000-0100-00000E000000}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -10678,7 +11168,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:M193" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A1:M193" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -10698,38 +11188,38 @@
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="48"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{452BCF15-63D6-4F0D-8237-F453C9931794}" name="effect" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{3C4B8B30-E7ED-4AB5-BC66-F5C283820DD3}" name="castingtime" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{EDD4FA58-CDB8-416C-923B-13AE644AA21A}" name="castingtimeShort" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{E3A80605-B07C-400F-9DD6-DA1ECD45B17F}" name="kpcost" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{3735962A-FF4F-4E3D-9AFC-95B48BCF0758}" name="kpcostShort" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{4D0248C5-34EF-49A3-B1B4-33D1C05D9FBB}" name="range" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{D6111C84-C6C2-4C98-9BAC-040E9A31F2B9}" name="rangeShort" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{F33F5A8B-FEA1-4B00-AE2D-20CCBB24FF2A}" name="duration" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{66749CC6-D9C4-4BF4-BA63-F5A58FD8E6CB}" name="durationShort" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{BE17D95F-F42A-48F5-9E7F-A545D95D81C2}" name="target" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{1E0275F4-0996-4EC0-B571-4BB2870B8257}" name="src" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{452BCF15-63D6-4F0D-8237-F453C9931794}" name="effect" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{3C4B8B30-E7ED-4AB5-BC66-F5C283820DD3}" name="castingtime" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{EDD4FA58-CDB8-416C-923B-13AE644AA21A}" name="castingtimeShort" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{E3A80605-B07C-400F-9DD6-DA1ECD45B17F}" name="kpcost" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{3735962A-FF4F-4E3D-9AFC-95B48BCF0758}" name="kpcostShort" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{4D0248C5-34EF-49A3-B1B4-33D1C05D9FBB}" name="range" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{D6111C84-C6C2-4C98-9BAC-040E9A31F2B9}" name="rangeShort" dataDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{F33F5A8B-FEA1-4B00-AE2D-20CCBB24FF2A}" name="duration" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{66749CC6-D9C4-4BF4-BA63-F5A58FD8E6CB}" name="durationShort" dataDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{BE17D95F-F42A-48F5-9E7F-A545D95D81C2}" name="target" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{1E0275F4-0996-4EC0-B571-4BB2870B8257}" name="src" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="A1:B13" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="A1:B13" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:B13" xr:uid="{00000000-0009-0000-0100-000010000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:J502" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:J502" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:J502" xr:uid="{00000000-0009-0000-0100-000006000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10743,37 +11233,37 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="sel" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="input" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column1" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column2" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column3" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Column4" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Column5" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Column6" dataDxfId="31"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A1:B111" xr:uid="{00000000-0009-0000-0100-00000A000000}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="sel" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="input" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column1" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column2" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column3" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Column4" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Column5" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Column6" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:B111" xr:uid="{00000000-0009-0000-0100-00000A000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:D76" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10781,45 +11271,45 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="spec" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="specInput" dataDxfId="21"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:B36" xr:uid="{00000000-0009-0000-0100-00000B000000}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="spec" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="specInput" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table15" displayName="Table15" ref="A1:B466" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:B36" xr:uid="{00000000-0009-0000-0100-00000B000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table15" displayName="Table15" ref="A1:B466" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:B466" xr:uid="{00000000-0009-0000-0100-00000F000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="14" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="3" dataCellStyle="Excel Built-in Normal"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:B484" totalsRowShown="0" headerRowDxfId="13">
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:B484" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:B484" xr:uid="{00000000-0009-0000-0100-000009000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10828,29 +11318,29 @@
     <sortCondition ref="A1:A474"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
   <autoFilter ref="A1:B8" xr:uid="{00000000-0009-0000-0100-00000D000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="122"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="121"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="127"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:K13" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:K13" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
   <autoFilter ref="A1:K13" xr:uid="{00000000-0009-0000-0100-000012000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10862,23 +11352,59 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="attributeAdjustments" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="automaticAdvantages" dataDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="stronglyRecommendedAdvantages" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="stronglyRecommendedDisadvantages" dataDxfId="113"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="commonAdvantages" dataDxfId="112"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="commonDisadvantages" dataDxfId="111"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="uncommonAdvantages" dataDxfId="110"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="uncommonDisadvantages" dataDxfId="109"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="src" dataDxfId="108"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="attributeAdjustments" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="automaticAdvantages" dataDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="stronglyRecommendedAdvantages" dataDxfId="119"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="stronglyRecommendedDisadvantages" dataDxfId="118"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="commonAdvantages" dataDxfId="117"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="commonDisadvantages" dataDxfId="116"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="uncommonAdvantages" dataDxfId="115"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="uncommonDisadvantages" dataDxfId="114"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="src" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{B4F1794A-E7C4-468F-B8D8-970C354AABE6}" name="Tabelle19" displayName="Tabelle19" ref="A1:M27" totalsRowShown="0" headerRowDxfId="112">
+  <autoFilter ref="A1:M27" xr:uid="{CF034C78-9071-47EC-AB34-3D606EE1BBA0}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{323211C5-81FD-41D0-9F64-A33241693AC3}" name="id" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{FDC1B446-D119-4AB0-BFD5-ACF6E75BA8A5}" name="name" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{92A07580-4496-4839-BDFD-3E1CD0593E78}" name="areaKnowledgeShort" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{44EF4FF0-9A41-48CA-BC45-CC1B1304A096}" name="areaKnowledge"/>
+    <tableColumn id="5" xr3:uid="{3A9496F5-2D90-4F09-9E2B-F936A6E5B397}" name="commonMundaneProfessions"/>
+    <tableColumn id="6" xr3:uid="{7D2183EE-15A4-4FF4-9222-723CACFF8CAA}" name="commonMagicalProfessions"/>
+    <tableColumn id="7" xr3:uid="{88CDD512-140B-4BF4-8F6C-75F9220452A7}" name="commonBlessedProfessions"/>
+    <tableColumn id="8" xr3:uid="{0886B565-04C1-413E-9E68-0C9819C638A1}" name="commonAdvantages"/>
+    <tableColumn id="9" xr3:uid="{2C6F7161-6DB9-4A45-A0C3-D2E4001E1BC3}" name="commonDisadvantages"/>
+    <tableColumn id="10" xr3:uid="{745A9F74-C60C-4CBC-9102-98FE33FC8526}" name="uncommonAdvantages"/>
+    <tableColumn id="11" xr3:uid="{C1FC4429-9AFB-46A3-A828-99A029A30219}" name="uncommonDisadvantages"/>
+    <tableColumn id="12" xr3:uid="{839A4140-773B-4A98-9156-075E987FA39A}" name="commonNames"/>
+    <tableColumn id="13" xr3:uid="{8C51E69A-3B2D-4662-B403-D59D4610C76D}" name="src" dataDxfId="108"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A1:G95" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -10902,7 +11428,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -10918,7 +11444,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:D76" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="A1:D76" xr:uid="{00000000-0009-0000-0100-000008000000}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -10936,7 +11462,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:D72" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
   <autoFilter ref="A1:D72" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -10954,7 +11480,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
   <autoFilter ref="A1:J60" xr:uid="{00000000-0009-0000-0100-000007000000}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -10982,31 +11508,6 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="critical" dataDxfId="72"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="botch" dataDxfId="71"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="src" dataDxfId="70"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:M1048576" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
-  <autoFilter ref="A1:M1048576" xr:uid="{00000000-0009-0000-0100-000004000000}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="effect" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="castingtime" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{D89CFCD8-0667-4532-ADCB-656E0F380FC9}" name="castingtimeShort" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="aecost" dataDxfId="62"/>
-    <tableColumn id="11" xr3:uid="{AA76CB3A-D16A-4989-ACEE-9057F8B23848}" name="aecostShort" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="range" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{DD92ED00-D630-4075-AFBB-75382F298664}" name="rangeShort" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="duration" dataDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{35897220-D86D-43E4-9246-750CE8AD5E3B}" name="durationShort" dataDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="target" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="src" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11413,8 +11914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12006,6 +12507,21 @@
       <c r="C22" s="11" t="s">
         <v>2284</v>
       </c>
+      <c r="F22" s="28" t="s">
+        <v>3119</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>3120</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>3121</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>3122</v>
+      </c>
+      <c r="J22" s="27">
+        <v>197</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="10">
@@ -12017,6 +12533,21 @@
       <c r="C23" s="11" t="s">
         <v>2285</v>
       </c>
+      <c r="F23" s="28" t="s">
+        <v>3123</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>3124</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>3125</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>3126</v>
+      </c>
+      <c r="J23" s="27">
+        <v>198</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="10">
@@ -12028,6 +12559,21 @@
       <c r="C24" s="11" t="s">
         <v>2286</v>
       </c>
+      <c r="F24" s="28" t="s">
+        <v>3127</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>3128</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>3129</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>3130</v>
+      </c>
+      <c r="J24" s="27">
+        <v>198</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="10">
@@ -12039,6 +12585,21 @@
       <c r="C25" s="11" t="s">
         <v>2287</v>
       </c>
+      <c r="F25" s="28" t="s">
+        <v>3131</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>3132</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>3133</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>3134</v>
+      </c>
+      <c r="J25" s="27">
+        <v>198</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="10">
@@ -12050,6 +12611,21 @@
       <c r="C26" s="11" t="s">
         <v>2288</v>
       </c>
+      <c r="F26" s="28" t="s">
+        <v>3135</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>3136</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>3137</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>3138</v>
+      </c>
+      <c r="J26" s="27">
+        <v>199</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="10">
@@ -12061,6 +12637,21 @@
       <c r="C27" s="11" t="s">
         <v>2289</v>
       </c>
+      <c r="F27" s="28" t="s">
+        <v>3139</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>3140</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>3141</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>3142</v>
+      </c>
+      <c r="J27" s="27">
+        <v>199</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="10">
@@ -12072,6 +12663,21 @@
       <c r="C28" s="11" t="s">
         <v>2290</v>
       </c>
+      <c r="F28" s="28" t="s">
+        <v>3143</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>3144</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>3145</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>3146</v>
+      </c>
+      <c r="J28" s="27">
+        <v>200</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="10">
@@ -12083,6 +12689,21 @@
       <c r="C29" s="11" t="s">
         <v>2291</v>
       </c>
+      <c r="F29" s="28" t="s">
+        <v>3147</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>3149</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>3150</v>
+      </c>
+      <c r="J29" s="27">
+        <v>200</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="10">
@@ -12094,6 +12715,21 @@
       <c r="C30" s="11" t="s">
         <v>2292</v>
       </c>
+      <c r="F30" s="28" t="s">
+        <v>3151</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>3152</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>3153</v>
+      </c>
+      <c r="J30" s="27">
+        <v>200</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="10">
@@ -12105,6 +12741,21 @@
       <c r="C31" s="11" t="s">
         <v>2293</v>
       </c>
+      <c r="F31" s="28" t="s">
+        <v>3154</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>3155</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>3156</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>3157</v>
+      </c>
+      <c r="J31" s="27">
+        <v>201</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="10">
@@ -12116,8 +12767,23 @@
       <c r="C32" s="11" t="s">
         <v>2294</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F32" s="28" t="s">
+        <v>3158</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>3159</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>3160</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>3161</v>
+      </c>
+      <c r="J32" s="27">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -12127,8 +12793,23 @@
       <c r="C33" s="11" t="s">
         <v>2295</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F33" s="28" t="s">
+        <v>3162</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H33" s="28" t="s">
+        <v>3163</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>3164</v>
+      </c>
+      <c r="J33" s="27">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -12138,8 +12819,23 @@
       <c r="C34" s="11" t="s">
         <v>2295</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F34" s="28" t="s">
+        <v>3165</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>3166</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>3167</v>
+      </c>
+      <c r="J34" s="27">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -12152,8 +12848,23 @@
       <c r="D35" s="10" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F35" s="28" t="s">
+        <v>3168</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>3169</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>3170</v>
+      </c>
+      <c r="J35" s="27">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -12163,8 +12874,23 @@
       <c r="C36" s="11" t="s">
         <v>2297</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F36" s="28" t="s">
+        <v>3171</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>3172</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>3173</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>3174</v>
+      </c>
+      <c r="J36" s="27">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -12174,8 +12900,23 @@
       <c r="C37" s="11" t="s">
         <v>2298</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F37" s="28" t="s">
+        <v>3175</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>3176</v>
+      </c>
+      <c r="I37" s="28" t="s">
+        <v>3177</v>
+      </c>
+      <c r="J37" s="27">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -12185,8 +12926,23 @@
       <c r="C38" s="11" t="s">
         <v>2299</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F38" s="28" t="s">
+        <v>3178</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>3179</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>3180</v>
+      </c>
+      <c r="I38" s="28" t="s">
+        <v>3181</v>
+      </c>
+      <c r="J38" s="27">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -12196,8 +12952,23 @@
       <c r="C39" s="11" t="s">
         <v>2300</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F39" s="28" t="s">
+        <v>3182</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>3183</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>3184</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>3185</v>
+      </c>
+      <c r="J39" s="27">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -12207,8 +12978,23 @@
       <c r="C40" s="11" t="s">
         <v>2295</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F40" s="28" t="s">
+        <v>3186</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>3187</v>
+      </c>
+      <c r="I40" s="28" t="s">
+        <v>3188</v>
+      </c>
+      <c r="J40" s="27">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -12218,8 +13004,23 @@
       <c r="C41" s="11" t="s">
         <v>2295</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F41" s="28" t="s">
+        <v>3189</v>
+      </c>
+      <c r="G41" s="28" t="s">
+        <v>3190</v>
+      </c>
+      <c r="H41" s="28" t="s">
+        <v>3191</v>
+      </c>
+      <c r="I41" s="28" t="s">
+        <v>3192</v>
+      </c>
+      <c r="J41" s="27">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -12229,8 +13030,23 @@
       <c r="C42" s="11" t="s">
         <v>2301</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F42" s="28" t="s">
+        <v>3193</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>3194</v>
+      </c>
+      <c r="H42" s="28" t="s">
+        <v>3195</v>
+      </c>
+      <c r="I42" s="28" t="s">
+        <v>3196</v>
+      </c>
+      <c r="J42" s="27">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="10">
         <v>42</v>
       </c>
@@ -12240,8 +13056,23 @@
       <c r="C43" s="11" t="s">
         <v>2302</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F43" s="28" t="s">
+        <v>3197</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>3148</v>
+      </c>
+      <c r="H43" s="28" t="s">
+        <v>3198</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>3199</v>
+      </c>
+      <c r="J43" s="27">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="10">
         <v>43</v>
       </c>
@@ -12251,8 +13082,23 @@
       <c r="C44" s="11" t="s">
         <v>2303</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F44" s="28" t="s">
+        <v>3200</v>
+      </c>
+      <c r="G44" s="28" t="s">
+        <v>3201</v>
+      </c>
+      <c r="H44" s="28" t="s">
+        <v>3202</v>
+      </c>
+      <c r="I44" s="28" t="s">
+        <v>3203</v>
+      </c>
+      <c r="J44" s="27">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="10">
         <v>44</v>
       </c>
@@ -12262,8 +13108,23 @@
       <c r="C45" s="11" t="s">
         <v>2304</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F45" s="28" t="s">
+        <v>3204</v>
+      </c>
+      <c r="G45" s="28" t="s">
+        <v>3205</v>
+      </c>
+      <c r="H45" s="28" t="s">
+        <v>3206</v>
+      </c>
+      <c r="I45" s="28" t="s">
+        <v>3207</v>
+      </c>
+      <c r="J45" s="27">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="10">
         <v>45</v>
       </c>
@@ -12273,8 +13134,23 @@
       <c r="C46" s="11" t="s">
         <v>2305</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F46" s="28" t="s">
+        <v>3204</v>
+      </c>
+      <c r="G46" s="28" t="s">
+        <v>3208</v>
+      </c>
+      <c r="H46" s="28" t="s">
+        <v>3209</v>
+      </c>
+      <c r="I46" s="28" t="s">
+        <v>3210</v>
+      </c>
+      <c r="J46" s="27">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="10">
         <v>46</v>
       </c>
@@ -12284,8 +13160,23 @@
       <c r="C47" s="11" t="s">
         <v>2306</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F47" s="28" t="s">
+        <v>3211</v>
+      </c>
+      <c r="G47" s="28" t="s">
+        <v>3212</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>3213</v>
+      </c>
+      <c r="I47" s="28" t="s">
+        <v>3214</v>
+      </c>
+      <c r="J47" s="27">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="10">
         <v>47</v>
       </c>
@@ -12295,8 +13186,23 @@
       <c r="C48" s="11" t="s">
         <v>2307</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F48" s="28" t="s">
+        <v>3215</v>
+      </c>
+      <c r="G48" s="28" t="s">
+        <v>3216</v>
+      </c>
+      <c r="H48" s="28" t="s">
+        <v>3217</v>
+      </c>
+      <c r="I48" s="28" t="s">
+        <v>3218</v>
+      </c>
+      <c r="J48" s="27">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -12306,8 +13212,20 @@
       <c r="C49" s="11" t="s">
         <v>2308</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="F49" s="28" t="s">
+        <v>3219</v>
+      </c>
+      <c r="G49" s="28" t="s">
+        <v>3220</v>
+      </c>
+      <c r="H49" s="28" t="s">
+        <v>3221</v>
+      </c>
+      <c r="I49" s="28" t="s">
+        <v>3222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="10">
         <v>49</v>
       </c>
@@ -12318,7 +13236,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="10">
         <v>50</v>
       </c>
@@ -12329,7 +13247,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="10">
         <v>51</v>
       </c>
@@ -12340,7 +13258,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="10">
         <v>52</v>
       </c>
@@ -12351,7 +13269,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="10">
         <v>53</v>
       </c>
@@ -12362,7 +13280,7 @@
         <v>2313</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="10">
         <v>54</v>
       </c>
@@ -12373,7 +13291,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="10">
         <v>55</v>
       </c>
@@ -12384,7 +13302,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="10">
         <v>56</v>
       </c>
@@ -12395,7 +13313,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="10">
         <v>57</v>
       </c>
@@ -12406,7 +13324,7 @@
         <v>2317</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="10">
         <v>58</v>
       </c>
@@ -12417,7 +13335,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="10">
         <v>59</v>
       </c>
@@ -20634,7 +21552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -36188,7 +37106,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -36541,240 +37459,672 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.6640625" style="1"/>
+    <col min="3" max="12" width="10.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
+      <c r="C1" s="25" t="s">
+        <v>3091</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>3092</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>3093</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>3094</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>3095</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>2798</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>2799</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>2800</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>2801</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>3096</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
+      <c r="C2" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>3098</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>3099</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>3100</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>3101</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>3102</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>3118</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>3103</v>
+      </c>
+      <c r="M2" s="26">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
+      <c r="C3" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>3104</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>3105</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>3106</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>3101</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>3107</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>3117</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>3108</v>
+      </c>
+      <c r="M3" s="26"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
+      <c r="C4" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>3109</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>3110</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>3116</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>3101</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>3111</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>3112</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>3113</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>3114</v>
+      </c>
+      <c r="M4" s="26"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="24">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
+      <c r="C5" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="26"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="24">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
+      <c r="C6" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="26"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="24">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
+      <c r="C7" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="24">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
+      <c r="C8" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="26"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="24">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
+      <c r="C9" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="26"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="24">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
+      <c r="C10" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="26"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="24">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
+      <c r="C11" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="26"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="24">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
+      <c r="C12" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="26"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="24">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="1">
+      <c r="C13" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="26"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="24">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
+      <c r="C14" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="26"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="24">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="1">
+      <c r="C15" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="26"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="24">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="1">
+      <c r="C16" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="26"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A17" s="24">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="1">
+      <c r="C17" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="26"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="24">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="1">
+      <c r="C18" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="26"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A19" s="24">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="1">
+      <c r="C19" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="26"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" s="24">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
+      <c r="C20" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A21" s="24">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
+      <c r="C21" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="26"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" s="24">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
+      <c r="C22" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="26"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A23" s="24">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="1">
+      <c r="C23" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="26"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A24" s="24">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="24" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="1">
+      <c r="C24" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="26"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A25" s="24">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="1">
+      <c r="C25" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="26"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A26" s="24">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="1">
+      <c r="C26" s="24" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="26"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A27" s="24">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="24" t="s">
         <v>2502</v>
       </c>
+      <c r="C27" s="24" t="s">
+        <v>3115</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="26"/>
     </row>
   </sheetData>
   <sortState ref="A2:B26">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed effect text of *Mächtiger Angriff*
</commit_message>
<xml_diff>
--- a/src/data/TDE5_de-DE.xlsx
+++ b/src/data/TDE5_de-DE.xlsx
@@ -12075,9 +12075,6 @@
     <t>Der Borongeweihte ist in der Lage, alle Geister zu sehen, die sich in einem Radius von QS x 3 Schritt befinden, selbst wenn sie mit bloßem Auge nicht sichtbar wären.</t>
   </si>
   <si>
-    <t>Bis zu QS/2 Grundeinheiten eines Rauschmittels verlieren nach Anwendung der Liturgie viele negative Eigenschaften. Sie können weiterhin den Geisteszustand der konsumierenden Person beeinflussen, werden jedoch keine Sucht herbeiführen, Kopfschmerzen hervorrufen oder Schaden/ Zustände verursachen. Auch nach Ablauf der Wirkungsdauer tritt keine dieser Wirkungen ein, solange der Verzehr bereits erfolgt ist.</t>
-  </si>
-  <si>
     <t>Der Ertrag von landwirtschaftlich genutztem Getreide (z. B. Weizen, Roggen, Reis) erhöht sich um QS x 5 %, wenn das Getreide angepflanzt wird.</t>
   </si>
   <si>
@@ -12087,9 +12084,6 @@
     <t>Der Giftbann neutralisiert ein Gift. Die maximale Giftstufe darf die QS nicht übersteigen, sonst wirkt die Liturgie nicht und gilt als misslungen.</t>
   </si>
   <si>
-    <t>Durch eine Berührung kann ein Objekt bis zur Größe eines Apfels in Gold, Silber&lt;/p&gt;\n&lt;p&gt;oder Edelsteine verwandelt werden. Der Wert des veränderten Objektes entspricht 50 Dukaten.</t>
-  </si>
-  <si>
     <t>Die Haut des Betroffenen überzieht sich mit einem golden leuchtenden Schein, der ihm RS verleiht. Die Höhe des gewünschten RS muss der Geweihte vor der Probe festlegen. Maximal ist so ein RS von 3 möglich. Der RS ist kombinierbar mit anderem, profanem RS, nicht aber mit magischem RS. Gegen Dämonen und magische Angriffe verleiht die Liturgie noch einen Punkt zusätzlichen RS.</t>
   </si>
   <si>
@@ -12625,6 +12619,12 @@
   </si>
   <si>
     <t>153&amp;159</t>
+  </si>
+  <si>
+    <t>Bis zu QS/2 Grundeinheiten eines Rauschmittels verlieren nach Anwendung der Liturgie viele negative Eigenschaften. Sie können weiterhin den Geisteszustand der konsumierenden Person beeinflussen, werden jedoch keine Sucht herbeiführen, Kopfschmerzen hervorrufen oder Schaden/Zustände verursachen. Auch nach Ablauf der Wirkungsdauer tritt keine dieser Wirkungen ein, solange der Verzehr bereits erfolgt ist.</t>
+  </si>
+  <si>
+    <t>Durch eine Berührung kann ein Objekt bis zur Größe eines Apfels in Gold, Silber oder Edelsteine verwandelt werden. Der Wert des veränderten Objektes entspricht 50 Dukaten.</t>
   </si>
 </sst>
 </file>
@@ -19781,7 +19781,7 @@
         <v>2947</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>4081</v>
+        <v>4079</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>2929</v>
@@ -19904,7 +19904,7 @@
         <v>2951</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>4075</v>
+        <v>4073</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>3104</v>
@@ -20027,7 +20027,7 @@
         <v>2949</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>4076</v>
+        <v>4074</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>2761</v>
@@ -20068,7 +20068,7 @@
         <v>2949</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>4077</v>
+        <v>4075</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>2773</v>
@@ -20642,7 +20642,7 @@
         <v>2949</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>4078</v>
+        <v>4076</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>2708</v>
@@ -20724,7 +20724,7 @@
         <v>2949</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>4076</v>
+        <v>4074</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>2761</v>
@@ -20970,7 +20970,7 @@
         <v>2948</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>4076</v>
+        <v>4074</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>2761</v>
@@ -21011,7 +21011,7 @@
         <v>2949</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>4079</v>
+        <v>4077</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>2756</v>
@@ -21298,7 +21298,7 @@
         <v>2951</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>4080</v>
+        <v>4078</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>2943</v>
@@ -21456,7 +21456,7 @@
         <v>3835</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>4082</v>
+        <v>4080</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>2949</v>
@@ -22030,7 +22030,7 @@
         <v>3852</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>4083</v>
+        <v>4081</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>2950</v>
@@ -22112,7 +22112,7 @@
         <v>3853</v>
       </c>
       <c r="D132" s="17" t="s">
-        <v>4083</v>
+        <v>4081</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>2950</v>
@@ -22487,7 +22487,7 @@
         <v>2949</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>4084</v>
+        <v>4082</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>2749</v>
@@ -22938,7 +22938,7 @@
         <v>2949</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>4076</v>
+        <v>4074</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>2761</v>
@@ -22973,7 +22973,7 @@
         <v>3880</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>4083</v>
+        <v>4081</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>2950</v>
@@ -23055,7 +23055,7 @@
         <v>3881</v>
       </c>
       <c r="D155" s="17" t="s">
-        <v>4087</v>
+        <v>4085</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>2947</v>
@@ -23178,13 +23178,13 @@
         <v>3884</v>
       </c>
       <c r="D158" s="17" t="s">
-        <v>4085</v>
+        <v>4083</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>2949</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>4086</v>
+        <v>4084</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>2929</v>
@@ -23963,7 +23963,7 @@
         <v>2892</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>4088</v>
+        <v>4086</v>
       </c>
       <c r="G177" s="1" t="s">
         <v>2750</v>
@@ -26334,7 +26334,7 @@
   <dimension ref="A1:M193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26396,7 +26396,7 @@
         <v>330</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>4089</v>
+        <v>4087</v>
       </c>
       <c r="M2" s="35">
         <v>324</v>
@@ -26410,7 +26410,7 @@
         <v>331</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>4090</v>
+        <v>4088</v>
       </c>
       <c r="M3" s="35">
         <v>324</v>
@@ -26438,7 +26438,7 @@
         <v>333</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>4091</v>
+        <v>4089</v>
       </c>
       <c r="M5" s="35">
         <v>324</v>
@@ -26480,7 +26480,7 @@
         <v>336</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>4092</v>
+        <v>4090</v>
       </c>
       <c r="M8" s="35">
         <v>325</v>
@@ -26508,7 +26508,7 @@
         <v>338</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>4093</v>
+        <v>4091</v>
       </c>
       <c r="M10" s="35">
         <v>325</v>
@@ -26522,7 +26522,7 @@
         <v>339</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="M11" s="35">
         <v>325</v>
@@ -26536,7 +26536,7 @@
         <v>340</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>4006</v>
+        <v>4004</v>
       </c>
       <c r="M12" s="35">
         <v>326</v>
@@ -26550,7 +26550,7 @@
         <v>341</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>4094</v>
+        <v>4092</v>
       </c>
       <c r="M13" s="35">
         <v>326</v>
@@ -26564,7 +26564,7 @@
         <v>342</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>4010</v>
+        <v>4008</v>
       </c>
       <c r="M14" s="35">
         <v>326</v>
@@ -26578,7 +26578,7 @@
         <v>343</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>4020</v>
+        <v>4018</v>
       </c>
       <c r="M15" s="35">
         <v>327</v>
@@ -26592,7 +26592,7 @@
         <v>344</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>4021</v>
+        <v>4019</v>
       </c>
       <c r="M16" s="35">
         <v>327</v>
@@ -26606,7 +26606,7 @@
         <v>345</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>4022</v>
+        <v>4020</v>
       </c>
       <c r="M17" s="35">
         <v>327</v>
@@ -26620,7 +26620,7 @@
         <v>346</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>4095</v>
+        <v>4093</v>
       </c>
       <c r="M18" s="35">
         <v>327</v>
@@ -26634,7 +26634,7 @@
         <v>364</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>4026</v>
+        <v>4024</v>
       </c>
       <c r="M19" s="35">
         <v>328</v>
@@ -26648,7 +26648,7 @@
         <v>365</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>4096</v>
+        <v>4094</v>
       </c>
       <c r="M20" s="35">
         <v>328</v>
@@ -26662,7 +26662,7 @@
         <v>366</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>4029</v>
+        <v>4027</v>
       </c>
       <c r="M21" s="35">
         <v>328</v>
@@ -26676,7 +26676,7 @@
         <v>367</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>4097</v>
+        <v>4095</v>
       </c>
       <c r="M22" s="35">
         <v>328</v>
@@ -26690,7 +26690,7 @@
         <v>368</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>4033</v>
+        <v>4031</v>
       </c>
       <c r="M23" s="35">
         <v>328</v>
@@ -26704,7 +26704,7 @@
         <v>369</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>4098</v>
+        <v>4096</v>
       </c>
       <c r="M24" s="35">
         <v>329</v>
@@ -26718,7 +26718,7 @@
         <v>370</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>4040</v>
+        <v>4038</v>
       </c>
       <c r="M25" s="35">
         <v>329</v>
@@ -26732,7 +26732,7 @@
         <v>371</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>4042</v>
+        <v>4040</v>
       </c>
       <c r="M26" s="35">
         <v>329</v>
@@ -26746,7 +26746,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>4099</v>
+        <v>4097</v>
       </c>
       <c r="M27" s="35">
         <v>329</v>
@@ -26760,7 +26760,7 @@
         <v>373</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>4100</v>
+        <v>4098</v>
       </c>
       <c r="M28" s="35">
         <v>329</v>
@@ -26774,7 +26774,7 @@
         <v>374</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>4047</v>
+        <v>4045</v>
       </c>
       <c r="M29" s="35">
         <v>330</v>
@@ -26788,7 +26788,7 @@
         <v>375</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>4101</v>
+        <v>4099</v>
       </c>
       <c r="M30" s="35">
         <v>330</v>
@@ -26802,7 +26802,7 @@
         <v>376</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>4049</v>
+        <v>4047</v>
       </c>
       <c r="M31" s="35">
         <v>330</v>
@@ -26816,7 +26816,7 @@
         <v>377</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>4102</v>
+        <v>4100</v>
       </c>
       <c r="M32" s="35">
         <v>330</v>
@@ -26830,7 +26830,7 @@
         <v>378</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>4065</v>
+        <v>4063</v>
       </c>
       <c r="M33" s="35">
         <v>331</v>
@@ -26844,7 +26844,7 @@
         <v>379</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>4103</v>
+        <v>4101</v>
       </c>
       <c r="M34" s="35">
         <v>331</v>
@@ -26858,7 +26858,7 @@
         <v>380</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>4104</v>
+        <v>4102</v>
       </c>
       <c r="M35" s="35">
         <v>331</v>
@@ -26900,7 +26900,7 @@
         <v>383</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="M38" s="35">
         <v>331</v>
@@ -26914,7 +26914,7 @@
         <v>386</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>4105</v>
+        <v>4103</v>
       </c>
       <c r="M39" s="35">
         <v>332</v>
@@ -26928,7 +26928,7 @@
         <v>384</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>4106</v>
+        <v>4104</v>
       </c>
       <c r="M40" s="35">
         <v>332</v>
@@ -26942,7 +26942,7 @@
         <v>385</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>4107</v>
+        <v>4105</v>
       </c>
       <c r="M41" s="35">
         <v>333</v>
@@ -26970,10 +26970,10 @@
         <v>2541</v>
       </c>
       <c r="C43" s="35" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
       <c r="M43" s="35" t="s">
-        <v>4170</v>
+        <v>4168</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.45">
@@ -26984,7 +26984,7 @@
         <v>2542</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>4109</v>
+        <v>4107</v>
       </c>
       <c r="M44" s="35">
         <v>112</v>
@@ -27054,7 +27054,7 @@
         <v>2547</v>
       </c>
       <c r="C49" s="35" t="s">
-        <v>4110</v>
+        <v>4108</v>
       </c>
       <c r="M49" s="35">
         <v>114</v>
@@ -27068,7 +27068,7 @@
         <v>2548</v>
       </c>
       <c r="C50" s="35" t="s">
-        <v>4111</v>
+        <v>4109</v>
       </c>
       <c r="M50" s="35">
         <v>114</v>
@@ -27166,7 +27166,7 @@
         <v>2555</v>
       </c>
       <c r="C57" s="35" t="s">
-        <v>4112</v>
+        <v>4110</v>
       </c>
       <c r="M57" s="35">
         <v>117</v>
@@ -27180,7 +27180,7 @@
         <v>2556</v>
       </c>
       <c r="C58" s="35" t="s">
-        <v>4113</v>
+        <v>4111</v>
       </c>
       <c r="M58" s="35">
         <v>117</v>
@@ -27194,7 +27194,7 @@
         <v>2557</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>4114</v>
+        <v>4112</v>
       </c>
       <c r="M59" s="35">
         <v>117</v>
@@ -27211,7 +27211,7 @@
         <v>3981</v>
       </c>
       <c r="M60" s="35" t="s">
-        <v>4171</v>
+        <v>4169</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.45">
@@ -27222,7 +27222,7 @@
         <v>2559</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>4115</v>
+        <v>4113</v>
       </c>
       <c r="M61" s="35">
         <v>118</v>
@@ -27236,7 +27236,7 @@
         <v>2560</v>
       </c>
       <c r="C62" s="35" t="s">
-        <v>4116</v>
+        <v>4114</v>
       </c>
       <c r="M62" s="35">
         <v>118</v>
@@ -27250,7 +27250,7 @@
         <v>2561</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>4117</v>
+        <v>4115</v>
       </c>
       <c r="M63" s="35">
         <v>118</v>
@@ -27264,7 +27264,7 @@
         <v>2562</v>
       </c>
       <c r="C64" s="35" t="s">
-        <v>4118</v>
+        <v>4116</v>
       </c>
       <c r="M64" s="35">
         <v>119</v>
@@ -27306,7 +27306,7 @@
         <v>2565</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>4119</v>
+        <v>4117</v>
       </c>
       <c r="M67" s="35">
         <v>119</v>
@@ -27334,7 +27334,7 @@
         <v>2567</v>
       </c>
       <c r="C69" s="35" t="s">
-        <v>4120</v>
+        <v>4118</v>
       </c>
       <c r="M69" s="35">
         <v>120</v>
@@ -27348,7 +27348,7 @@
         <v>2568</v>
       </c>
       <c r="C70" s="35" t="s">
-        <v>4121</v>
+        <v>4119</v>
       </c>
       <c r="M70" s="35">
         <v>120</v>
@@ -27362,7 +27362,7 @@
         <v>2569</v>
       </c>
       <c r="C71" s="35" t="s">
-        <v>4122</v>
+        <v>4120</v>
       </c>
       <c r="M71" s="35">
         <v>121</v>
@@ -27390,7 +27390,7 @@
         <v>2571</v>
       </c>
       <c r="C73" s="35" t="s">
-        <v>3998</v>
+        <v>4180</v>
       </c>
       <c r="M73" s="35">
         <v>122</v>
@@ -27404,7 +27404,7 @@
         <v>2572</v>
       </c>
       <c r="C74" s="35" t="s">
-        <v>3999</v>
+        <v>3998</v>
       </c>
       <c r="M74" s="35">
         <v>122</v>
@@ -27418,7 +27418,7 @@
         <v>2573</v>
       </c>
       <c r="C75" s="35" t="s">
-        <v>4002</v>
+        <v>4181</v>
       </c>
       <c r="M75" s="35">
         <v>122</v>
@@ -27432,7 +27432,7 @@
         <v>2574</v>
       </c>
       <c r="C76" s="35" t="s">
-        <v>4003</v>
+        <v>4001</v>
       </c>
       <c r="M76" s="35">
         <v>123</v>
@@ -27446,7 +27446,7 @@
         <v>2575</v>
       </c>
       <c r="C77" s="35" t="s">
-        <v>4123</v>
+        <v>4121</v>
       </c>
       <c r="M77" s="35">
         <v>123</v>
@@ -27460,7 +27460,7 @@
         <v>2576</v>
       </c>
       <c r="C78" s="35" t="s">
-        <v>4005</v>
+        <v>4003</v>
       </c>
       <c r="M78" s="35">
         <v>123</v>
@@ -27474,7 +27474,7 @@
         <v>2577</v>
       </c>
       <c r="C79" s="35" t="s">
-        <v>4008</v>
+        <v>4006</v>
       </c>
       <c r="M79" s="35">
         <v>123</v>
@@ -27488,7 +27488,7 @@
         <v>2578</v>
       </c>
       <c r="C80" s="35" t="s">
-        <v>4124</v>
+        <v>4122</v>
       </c>
       <c r="M80" s="35">
         <v>124</v>
@@ -27502,10 +27502,10 @@
         <v>2579</v>
       </c>
       <c r="C81" s="35" t="s">
-        <v>4009</v>
+        <v>4007</v>
       </c>
       <c r="M81" s="35" t="s">
-        <v>4172</v>
+        <v>4170</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.45">
@@ -27516,7 +27516,7 @@
         <v>2580</v>
       </c>
       <c r="C82" s="35" t="s">
-        <v>4011</v>
+        <v>4009</v>
       </c>
       <c r="M82" s="35">
         <v>124</v>
@@ -27530,7 +27530,7 @@
         <v>2581</v>
       </c>
       <c r="C83" s="35" t="s">
-        <v>4125</v>
+        <v>4123</v>
       </c>
       <c r="M83" s="35">
         <v>124</v>
@@ -27544,7 +27544,7 @@
         <v>2582</v>
       </c>
       <c r="C84" s="35" t="s">
-        <v>4012</v>
+        <v>4010</v>
       </c>
       <c r="M84" s="35">
         <v>125</v>
@@ -27558,7 +27558,7 @@
         <v>2583</v>
       </c>
       <c r="C85" s="35" t="s">
-        <v>4013</v>
+        <v>4011</v>
       </c>
       <c r="M85" s="35">
         <v>126</v>
@@ -27572,7 +27572,7 @@
         <v>2584</v>
       </c>
       <c r="C86" s="35" t="s">
-        <v>4014</v>
+        <v>4012</v>
       </c>
       <c r="M86" s="35">
         <v>126</v>
@@ -27586,7 +27586,7 @@
         <v>2585</v>
       </c>
       <c r="C87" s="35" t="s">
-        <v>4015</v>
+        <v>4013</v>
       </c>
       <c r="M87" s="35">
         <v>127</v>
@@ -27600,7 +27600,7 @@
         <v>2586</v>
       </c>
       <c r="C88" s="35" t="s">
-        <v>4126</v>
+        <v>4124</v>
       </c>
       <c r="M88" s="35">
         <v>128</v>
@@ -27614,7 +27614,7 @@
         <v>2688</v>
       </c>
       <c r="C89" s="35" t="s">
-        <v>4017</v>
+        <v>4015</v>
       </c>
       <c r="M89" s="35">
         <v>128</v>
@@ -27628,7 +27628,7 @@
         <v>2587</v>
       </c>
       <c r="C90" s="35" t="s">
-        <v>4127</v>
+        <v>4125</v>
       </c>
       <c r="M90" s="35">
         <v>128</v>
@@ -27642,7 +27642,7 @@
         <v>2588</v>
       </c>
       <c r="C91" s="35" t="s">
-        <v>4128</v>
+        <v>4126</v>
       </c>
       <c r="M91" s="35">
         <v>128</v>
@@ -27656,10 +27656,10 @@
         <v>2589</v>
       </c>
       <c r="C92" s="35" t="s">
-        <v>4019</v>
+        <v>4017</v>
       </c>
       <c r="M92" s="35" t="s">
-        <v>4173</v>
+        <v>4171</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.45">
@@ -27670,7 +27670,7 @@
         <v>2590</v>
       </c>
       <c r="C93" s="35" t="s">
-        <v>4023</v>
+        <v>4021</v>
       </c>
       <c r="M93" s="35">
         <v>129</v>
@@ -27684,7 +27684,7 @@
         <v>2591</v>
       </c>
       <c r="C94" s="35" t="s">
-        <v>4024</v>
+        <v>4022</v>
       </c>
       <c r="M94" s="35">
         <v>129</v>
@@ -27698,7 +27698,7 @@
         <v>2592</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>4129</v>
+        <v>4127</v>
       </c>
       <c r="M95" s="35">
         <v>132</v>
@@ -27712,7 +27712,7 @@
         <v>2593</v>
       </c>
       <c r="C96" s="35" t="s">
-        <v>4025</v>
+        <v>4023</v>
       </c>
       <c r="M96" s="35">
         <v>129</v>
@@ -27726,7 +27726,7 @@
         <v>2594</v>
       </c>
       <c r="C97" s="35" t="s">
-        <v>4130</v>
+        <v>4128</v>
       </c>
       <c r="M97" s="35">
         <v>130</v>
@@ -27740,7 +27740,7 @@
         <v>2595</v>
       </c>
       <c r="C98" s="35" t="s">
-        <v>4131</v>
+        <v>4129</v>
       </c>
       <c r="M98" s="35">
         <v>130</v>
@@ -27754,7 +27754,7 @@
         <v>2596</v>
       </c>
       <c r="C99" s="35" t="s">
-        <v>4028</v>
+        <v>4026</v>
       </c>
       <c r="M99" s="35">
         <v>131</v>
@@ -27768,7 +27768,7 @@
         <v>2597</v>
       </c>
       <c r="C100" s="35" t="s">
-        <v>4030</v>
+        <v>4028</v>
       </c>
       <c r="M100" s="35">
         <v>131</v>
@@ -27782,7 +27782,7 @@
         <v>2598</v>
       </c>
       <c r="C101" s="35" t="s">
-        <v>4132</v>
+        <v>4130</v>
       </c>
       <c r="M101" s="35">
         <v>131</v>
@@ -27796,7 +27796,7 @@
         <v>2599</v>
       </c>
       <c r="C102" s="35" t="s">
-        <v>4133</v>
+        <v>4131</v>
       </c>
       <c r="M102" s="35">
         <v>131</v>
@@ -27810,7 +27810,7 @@
         <v>2600</v>
       </c>
       <c r="C103" s="35" t="s">
-        <v>4134</v>
+        <v>4132</v>
       </c>
       <c r="M103" s="35">
         <v>132</v>
@@ -27824,7 +27824,7 @@
         <v>2601</v>
       </c>
       <c r="C104" s="35" t="s">
-        <v>4032</v>
+        <v>4030</v>
       </c>
       <c r="M104" s="35">
         <v>132</v>
@@ -27838,7 +27838,7 @@
         <v>2602</v>
       </c>
       <c r="C105" s="35" t="s">
-        <v>4034</v>
+        <v>4032</v>
       </c>
       <c r="M105" s="35">
         <v>133</v>
@@ -27852,7 +27852,7 @@
         <v>2603</v>
       </c>
       <c r="C106" s="35" t="s">
-        <v>4035</v>
+        <v>4033</v>
       </c>
       <c r="M106" s="35">
         <v>133</v>
@@ -27866,7 +27866,7 @@
         <v>2604</v>
       </c>
       <c r="C107" s="35" t="s">
-        <v>4135</v>
+        <v>4133</v>
       </c>
       <c r="M107" s="35">
         <v>133</v>
@@ -27880,7 +27880,7 @@
         <v>2605</v>
       </c>
       <c r="C108" s="35" t="s">
-        <v>4038</v>
+        <v>4036</v>
       </c>
       <c r="M108" s="35">
         <v>134</v>
@@ -27894,7 +27894,7 @@
         <v>2606</v>
       </c>
       <c r="C109" s="35" t="s">
-        <v>4136</v>
+        <v>4134</v>
       </c>
       <c r="M109" s="35">
         <v>134</v>
@@ -27908,7 +27908,7 @@
         <v>2607</v>
       </c>
       <c r="C110" s="35" t="s">
-        <v>4044</v>
+        <v>4042</v>
       </c>
       <c r="M110" s="35">
         <v>135</v>
@@ -27922,7 +27922,7 @@
         <v>2608</v>
       </c>
       <c r="C111" s="35" t="s">
-        <v>4048</v>
+        <v>4046</v>
       </c>
       <c r="M111" s="35">
         <v>135</v>
@@ -27936,7 +27936,7 @@
         <v>2609</v>
       </c>
       <c r="C112" s="35" t="s">
-        <v>4137</v>
+        <v>4135</v>
       </c>
       <c r="M112" s="35">
         <v>135</v>
@@ -27950,7 +27950,7 @@
         <v>2610</v>
       </c>
       <c r="C113" s="35" t="s">
-        <v>4051</v>
+        <v>4049</v>
       </c>
       <c r="M113" s="35">
         <v>136</v>
@@ -27964,7 +27964,7 @@
         <v>2611</v>
       </c>
       <c r="C114" s="35" t="s">
-        <v>4053</v>
+        <v>4051</v>
       </c>
       <c r="M114" s="35">
         <v>136</v>
@@ -27978,10 +27978,10 @@
         <v>2612</v>
       </c>
       <c r="C115" s="35" t="s">
-        <v>4054</v>
+        <v>4052</v>
       </c>
       <c r="M115" s="35" t="s">
-        <v>4174</v>
+        <v>4172</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.45">
@@ -27992,7 +27992,7 @@
         <v>2613</v>
       </c>
       <c r="C116" s="35" t="s">
-        <v>4138</v>
+        <v>4136</v>
       </c>
       <c r="M116" s="35">
         <v>136</v>
@@ -28006,7 +28006,7 @@
         <v>2614</v>
       </c>
       <c r="C117" s="35" t="s">
-        <v>4139</v>
+        <v>4137</v>
       </c>
       <c r="M117" s="35">
         <v>137</v>
@@ -28020,7 +28020,7 @@
         <v>2615</v>
       </c>
       <c r="C118" s="35" t="s">
-        <v>4058</v>
+        <v>4056</v>
       </c>
       <c r="M118" s="35">
         <v>137</v>
@@ -28034,7 +28034,7 @@
         <v>2616</v>
       </c>
       <c r="C119" s="35" t="s">
-        <v>4140</v>
+        <v>4138</v>
       </c>
       <c r="M119" s="35">
         <v>138</v>
@@ -28048,7 +28048,7 @@
         <v>2617</v>
       </c>
       <c r="C120" s="35" t="s">
-        <v>4059</v>
+        <v>4057</v>
       </c>
       <c r="M120" s="35">
         <v>138</v>
@@ -28062,7 +28062,7 @@
         <v>2618</v>
       </c>
       <c r="C121" s="35" t="s">
-        <v>4141</v>
+        <v>4139</v>
       </c>
       <c r="M121" s="35">
         <v>138</v>
@@ -28076,10 +28076,10 @@
         <v>2619</v>
       </c>
       <c r="C122" s="35" t="s">
-        <v>4060</v>
+        <v>4058</v>
       </c>
       <c r="M122" s="35" t="s">
-        <v>4175</v>
+        <v>4173</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.45">
@@ -28090,7 +28090,7 @@
         <v>2620</v>
       </c>
       <c r="C123" s="35" t="s">
-        <v>4063</v>
+        <v>4061</v>
       </c>
       <c r="M123" s="35">
         <v>139</v>
@@ -28104,10 +28104,10 @@
         <v>2621</v>
       </c>
       <c r="C124" s="35" t="s">
-        <v>4066</v>
+        <v>4064</v>
       </c>
       <c r="M124" s="35" t="s">
-        <v>4176</v>
+        <v>4174</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.45">
@@ -28118,7 +28118,7 @@
         <v>2622</v>
       </c>
       <c r="C125" s="35" t="s">
-        <v>4070</v>
+        <v>4068</v>
       </c>
       <c r="M125" s="35">
         <v>139</v>
@@ -28132,10 +28132,10 @@
         <v>2623</v>
       </c>
       <c r="C126" s="35" t="s">
-        <v>4071</v>
+        <v>4069</v>
       </c>
       <c r="M126" s="35" t="s">
-        <v>4177</v>
+        <v>4175</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.45">
@@ -28146,7 +28146,7 @@
         <v>2624</v>
       </c>
       <c r="C127" s="35" t="s">
-        <v>4142</v>
+        <v>4140</v>
       </c>
       <c r="M127" s="35">
         <v>140</v>
@@ -28160,7 +28160,7 @@
         <v>2625</v>
       </c>
       <c r="C128" s="35" t="s">
-        <v>4143</v>
+        <v>4141</v>
       </c>
       <c r="M128" s="35">
         <v>140</v>
@@ -28188,7 +28188,7 @@
         <v>2627</v>
       </c>
       <c r="C130" s="35" t="s">
-        <v>4144</v>
+        <v>4142</v>
       </c>
       <c r="M130" s="35">
         <v>141</v>
@@ -28202,7 +28202,7 @@
         <v>2628</v>
       </c>
       <c r="C131" s="35" t="s">
-        <v>4145</v>
+        <v>4143</v>
       </c>
       <c r="M131" s="35">
         <v>141</v>
@@ -28244,7 +28244,7 @@
         <v>2631</v>
       </c>
       <c r="C134" s="35" t="s">
-        <v>4146</v>
+        <v>4144</v>
       </c>
       <c r="M134" s="35">
         <v>142</v>
@@ -28272,7 +28272,7 @@
         <v>2633</v>
       </c>
       <c r="C136" s="35" t="s">
-        <v>4147</v>
+        <v>4145</v>
       </c>
       <c r="M136" s="35">
         <v>143</v>
@@ -28286,10 +28286,10 @@
         <v>2634</v>
       </c>
       <c r="C137" s="35" t="s">
-        <v>4148</v>
+        <v>4146</v>
       </c>
       <c r="M137" s="35" t="s">
-        <v>4178</v>
+        <v>4176</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.45">
@@ -28412,7 +28412,7 @@
         <v>2689</v>
       </c>
       <c r="C146" s="35" t="s">
-        <v>4149</v>
+        <v>4147</v>
       </c>
       <c r="M146" s="35">
         <v>147</v>
@@ -28426,7 +28426,7 @@
         <v>2643</v>
       </c>
       <c r="C147" s="35" t="s">
-        <v>4004</v>
+        <v>4002</v>
       </c>
       <c r="M147" s="35">
         <v>147</v>
@@ -28440,7 +28440,7 @@
         <v>2644</v>
       </c>
       <c r="C148" s="35" t="s">
-        <v>4007</v>
+        <v>4005</v>
       </c>
       <c r="M148" s="35">
         <v>148</v>
@@ -28454,10 +28454,10 @@
         <v>2645</v>
       </c>
       <c r="C149" s="35" t="s">
-        <v>4150</v>
+        <v>4148</v>
       </c>
       <c r="M149" s="35" t="s">
-        <v>4179</v>
+        <v>4177</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.45">
@@ -28468,7 +28468,7 @@
         <v>2646</v>
       </c>
       <c r="C150" s="35" t="s">
-        <v>4151</v>
+        <v>4149</v>
       </c>
       <c r="M150" s="35">
         <v>149</v>
@@ -28482,7 +28482,7 @@
         <v>2647</v>
       </c>
       <c r="C151" s="35" t="s">
-        <v>4152</v>
+        <v>4150</v>
       </c>
       <c r="M151" s="35">
         <v>149</v>
@@ -28496,7 +28496,7 @@
         <v>2648</v>
       </c>
       <c r="C152" s="35" t="s">
-        <v>4153</v>
+        <v>4151</v>
       </c>
       <c r="M152" s="35">
         <v>149</v>
@@ -28510,7 +28510,7 @@
         <v>2649</v>
       </c>
       <c r="C153" s="35" t="s">
-        <v>4016</v>
+        <v>4014</v>
       </c>
       <c r="M153" s="35">
         <v>150</v>
@@ -28524,7 +28524,7 @@
         <v>2650</v>
       </c>
       <c r="C154" s="35" t="s">
-        <v>4154</v>
+        <v>4152</v>
       </c>
       <c r="M154" s="35">
         <v>150</v>
@@ -28538,7 +28538,7 @@
         <v>2651</v>
       </c>
       <c r="C155" s="35" t="s">
-        <v>4155</v>
+        <v>4153</v>
       </c>
       <c r="M155" s="35">
         <v>150</v>
@@ -28552,7 +28552,7 @@
         <v>2652</v>
       </c>
       <c r="C156" s="35" t="s">
-        <v>4018</v>
+        <v>4016</v>
       </c>
       <c r="M156" s="35">
         <v>151</v>
@@ -28566,10 +28566,10 @@
         <v>2653</v>
       </c>
       <c r="C157" s="35" t="s">
-        <v>4156</v>
+        <v>4154</v>
       </c>
       <c r="M157" s="35" t="s">
-        <v>4180</v>
+        <v>4178</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.45">
@@ -28580,7 +28580,7 @@
         <v>2654</v>
       </c>
       <c r="C158" s="35" t="s">
-        <v>4157</v>
+        <v>4155</v>
       </c>
       <c r="M158" s="35">
         <v>151</v>
@@ -28594,7 +28594,7 @@
         <v>2655</v>
       </c>
       <c r="C159" s="35" t="s">
-        <v>4158</v>
+        <v>4156</v>
       </c>
       <c r="M159" s="35">
         <v>152</v>
@@ -28608,7 +28608,7 @@
         <v>2656</v>
       </c>
       <c r="C160" s="35" t="s">
-        <v>4159</v>
+        <v>4157</v>
       </c>
       <c r="M160" s="35">
         <v>152</v>
@@ -28622,7 +28622,7 @@
         <v>2657</v>
       </c>
       <c r="C161" s="35" t="s">
-        <v>4027</v>
+        <v>4025</v>
       </c>
       <c r="M161" s="35">
         <v>152</v>
@@ -28636,7 +28636,7 @@
         <v>2658</v>
       </c>
       <c r="C162" s="35" t="s">
-        <v>4160</v>
+        <v>4158</v>
       </c>
       <c r="M162" s="35">
         <v>153</v>
@@ -28650,7 +28650,7 @@
         <v>2659</v>
       </c>
       <c r="C163" s="35" t="s">
-        <v>4031</v>
+        <v>4029</v>
       </c>
       <c r="M163" s="35">
         <v>153</v>
@@ -28664,10 +28664,10 @@
         <v>3576</v>
       </c>
       <c r="C164" s="35" t="s">
-        <v>4161</v>
+        <v>4159</v>
       </c>
       <c r="M164" s="35" t="s">
-        <v>4181</v>
+        <v>4179</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.45">
@@ -28678,7 +28678,7 @@
         <v>2660</v>
       </c>
       <c r="C165" s="35" t="s">
-        <v>4162</v>
+        <v>4160</v>
       </c>
       <c r="M165" s="35">
         <v>153</v>
@@ -28692,7 +28692,7 @@
         <v>2661</v>
       </c>
       <c r="C166" s="35" t="s">
-        <v>4036</v>
+        <v>4034</v>
       </c>
       <c r="M166" s="35">
         <v>154</v>
@@ -28706,7 +28706,7 @@
         <v>2662</v>
       </c>
       <c r="C167" s="35" t="s">
-        <v>4037</v>
+        <v>4035</v>
       </c>
       <c r="M167" s="35">
         <v>154</v>
@@ -28720,7 +28720,7 @@
         <v>2663</v>
       </c>
       <c r="C168" s="35" t="s">
-        <v>4039</v>
+        <v>4037</v>
       </c>
       <c r="M168" s="35">
         <v>155</v>
@@ -28734,7 +28734,7 @@
         <v>2664</v>
       </c>
       <c r="C169" s="35" t="s">
-        <v>4163</v>
+        <v>4161</v>
       </c>
       <c r="M169" s="35">
         <v>155</v>
@@ -28748,7 +28748,7 @@
         <v>2665</v>
       </c>
       <c r="C170" s="35" t="s">
-        <v>4041</v>
+        <v>4039</v>
       </c>
       <c r="M170" s="35">
         <v>155</v>
@@ -28762,7 +28762,7 @@
         <v>2666</v>
       </c>
       <c r="C171" s="35" t="s">
-        <v>4043</v>
+        <v>4041</v>
       </c>
       <c r="M171" s="35">
         <v>156</v>
@@ -28776,7 +28776,7 @@
         <v>2667</v>
       </c>
       <c r="C172" s="35" t="s">
-        <v>4045</v>
+        <v>4043</v>
       </c>
       <c r="M172" s="35">
         <v>156</v>
@@ -28790,7 +28790,7 @@
         <v>2668</v>
       </c>
       <c r="C173" s="35" t="s">
-        <v>4046</v>
+        <v>4044</v>
       </c>
       <c r="M173" s="35">
         <v>157</v>
@@ -28804,7 +28804,7 @@
         <v>2669</v>
       </c>
       <c r="C174" s="35" t="s">
-        <v>4050</v>
+        <v>4048</v>
       </c>
       <c r="M174" s="35">
         <v>157</v>
@@ -28818,7 +28818,7 @@
         <v>2670</v>
       </c>
       <c r="C175" s="35" t="s">
-        <v>4052</v>
+        <v>4050</v>
       </c>
       <c r="M175" s="35">
         <v>158</v>
@@ -28832,7 +28832,7 @@
         <v>2671</v>
       </c>
       <c r="C176" s="35" t="s">
-        <v>4164</v>
+        <v>4162</v>
       </c>
       <c r="M176" s="35">
         <v>158</v>
@@ -28846,7 +28846,7 @@
         <v>2672</v>
       </c>
       <c r="C177" s="35" t="s">
-        <v>4165</v>
+        <v>4163</v>
       </c>
       <c r="M177" s="35">
         <v>158</v>
@@ -28860,7 +28860,7 @@
         <v>2673</v>
       </c>
       <c r="C178" s="35" t="s">
-        <v>4166</v>
+        <v>4164</v>
       </c>
       <c r="M178" s="35">
         <v>158</v>
@@ -28874,7 +28874,7 @@
         <v>2674</v>
       </c>
       <c r="C179" s="35" t="s">
-        <v>4055</v>
+        <v>4053</v>
       </c>
       <c r="M179" s="35">
         <v>159</v>
@@ -28888,7 +28888,7 @@
         <v>2675</v>
       </c>
       <c r="C180" s="35" t="s">
-        <v>4056</v>
+        <v>4054</v>
       </c>
       <c r="M180" s="35">
         <v>159</v>
@@ -28902,7 +28902,7 @@
         <v>2676</v>
       </c>
       <c r="C181" s="35" t="s">
-        <v>4167</v>
+        <v>4165</v>
       </c>
       <c r="M181" s="35">
         <v>159</v>
@@ -28916,7 +28916,7 @@
         <v>2677</v>
       </c>
       <c r="C182" s="35" t="s">
-        <v>4057</v>
+        <v>4055</v>
       </c>
       <c r="M182" s="35">
         <v>160</v>
@@ -28930,7 +28930,7 @@
         <v>2678</v>
       </c>
       <c r="C183" s="35" t="s">
-        <v>4168</v>
+        <v>4166</v>
       </c>
       <c r="M183" s="35">
         <v>160</v>
@@ -28944,7 +28944,7 @@
         <v>2679</v>
       </c>
       <c r="C184" s="35" t="s">
-        <v>4169</v>
+        <v>4167</v>
       </c>
       <c r="M184" s="35">
         <v>161</v>
@@ -28958,7 +28958,7 @@
         <v>2680</v>
       </c>
       <c r="C185" s="35" t="s">
-        <v>4061</v>
+        <v>4059</v>
       </c>
       <c r="M185" s="35">
         <v>161</v>
@@ -28972,7 +28972,7 @@
         <v>2681</v>
       </c>
       <c r="C186" s="35" t="s">
-        <v>4062</v>
+        <v>4060</v>
       </c>
       <c r="M186" s="35">
         <v>161</v>
@@ -28986,7 +28986,7 @@
         <v>2682</v>
       </c>
       <c r="C187" s="35" t="s">
-        <v>4064</v>
+        <v>4062</v>
       </c>
       <c r="M187" s="35">
         <v>162</v>
@@ -29000,7 +29000,7 @@
         <v>1704</v>
       </c>
       <c r="C188" s="35" t="s">
-        <v>4067</v>
+        <v>4065</v>
       </c>
       <c r="M188" s="35">
         <v>162</v>
@@ -29014,7 +29014,7 @@
         <v>2683</v>
       </c>
       <c r="C189" s="35" t="s">
-        <v>4068</v>
+        <v>4066</v>
       </c>
       <c r="M189" s="35">
         <v>162</v>
@@ -29028,7 +29028,7 @@
         <v>2684</v>
       </c>
       <c r="C190" s="35" t="s">
-        <v>4069</v>
+        <v>4067</v>
       </c>
       <c r="M190" s="35">
         <v>162</v>
@@ -29042,7 +29042,7 @@
         <v>2685</v>
       </c>
       <c r="C191" s="35" t="s">
-        <v>4072</v>
+        <v>4070</v>
       </c>
       <c r="M191" s="35">
         <v>163</v>
@@ -29056,7 +29056,7 @@
         <v>2686</v>
       </c>
       <c r="C192" s="35" t="s">
-        <v>4073</v>
+        <v>4071</v>
       </c>
       <c r="M192" s="35">
         <v>163</v>
@@ -29070,7 +29070,7 @@
         <v>2687</v>
       </c>
       <c r="C193" s="35" t="s">
-        <v>4074</v>
+        <v>4072</v>
       </c>
       <c r="M193" s="35">
         <v>163</v>
@@ -29078,8 +29078,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added cantrips/blessing wiki texts and info boxes
</commit_message>
<xml_diff>
--- a/src/data/TDE5_de-DE.xlsx
+++ b/src/data/TDE5_de-DE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="7583" tabRatio="1000" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="30" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6809" uniqueCount="4182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7071" uniqueCount="4287">
   <si>
     <t>id</t>
   </si>
@@ -12625,6 +12625,321 @@
   </si>
   <si>
     <t>Durch eine Berührung kann ein Objekt bis zur Größe eines Apfels in Gold, Silber oder Edelsteine verwandelt werden. Der Wert des veränderten Objektes entspricht 50 Dukaten.</t>
+  </si>
+  <si>
+    <t>Der Zauberer senkt die Temperatur einer kleinen Menge Flüssigkeit (maximal ein Becher voll) um bis zu 10 Grad.</t>
+  </si>
+  <si>
+    <t>Körperhaare werden durch diesen Zaubertrick entfernt. Der Zauberer kann festlegen, dass bestimmte Körperstellen nicht enthaart werden (beispielsweise, damit Augenbrauen oder ein Bart nicht entfernt werden).</t>
+  </si>
+  <si>
+    <t>Kulturschaffende</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Khelbara ay Baburia)</t>
+  </si>
+  <si>
+    <t>Der Druide kann seinen Bart augenblicklich auf bis zu 1 Schritt Länge wachsen lassen. Normales und magisches Haar unterscheidet sich optisch nicht voneinander. Schneidet der Druide den durch den Zaubertrick gewachsenen Bart ab, lösen sich die abgeschnittenen Haare sofort auf.</t>
+  </si>
+  <si>
+    <t>Druiden</t>
+  </si>
+  <si>
+    <t>Ein einzelnes Wort oder ein anderes kurzes, nicht allzu lautes Geräusch nach Wahl erklingt bis zu 8 Schritt entfernt vom Zaubernden.</t>
+  </si>
+  <si>
+    <t>Mit Hilfe dieses Zaubertricks sendet der Druide einen Befehl an ein nahes, kleines Tier (z. B. Eichhörnchen, Amsel), das ihm eine Nuss oder einige Beeren bringt. Zum Sattwerden reicht dies jedoch nicht aus, erst 30 Anwendungen des Zaubertricks ergeben eine Ration Nahrung.</t>
+  </si>
+  <si>
+    <t>64 Schritt</t>
+  </si>
+  <si>
+    <t>Ein schreiender Patient wird für kurze Zeit still, seine Angst verschwindet in dieser Zeit aber nicht. Das Ziel muss vorher den Status *Fixiert* erlitten haben, damit der Zaubertrick funktioniert.</t>
+  </si>
+  <si>
+    <t>1 Stunde</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Perricum)</t>
+  </si>
+  <si>
+    <t>In einem Radius von 16 Schritt um den Magier verströmt die Umgebung einen angenehmen Geruch nach Blüten und Waldesgrün.</t>
+  </si>
+  <si>
+    <t>Elfen, Gildenmagier (Gerasim)</t>
+  </si>
+  <si>
+    <t>Der Zauberer riecht für etwa 5 Minuten nach einem Parfüm oder einem anderen für ihn angenehmen Geruch.</t>
+  </si>
+  <si>
+    <t>Ein Diener, Bauer oder eine andere, gegenüber dem Zauberer mit Ehrfurcht erfüllte Person weicht ihm sich verneigend aus. Personen, auf die dies nicht zutrifft, sind von dem Zaubertrick nicht betroffen.</t>
+  </si>
+  <si>
+    <t>30 Sekunden</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Fasar Beherrschung)</t>
+  </si>
+  <si>
+    <t>Einem maximal 1 Stein wiegenden Objekt wachsen ein oder mehrere Paar kurze Beine, die es auf Befehl des Zauberers umhertragen.</t>
+  </si>
+  <si>
+    <t>Eine kleine Flamme entsteht etwa einen Zentimeter über einem Finger des Zaubernden. Sie brennt bis zu 5 Minuten. Der Zaubertrick schützt die Hand nicht vor der Hitze der Flamme.</t>
+  </si>
+  <si>
+    <t>Der Zaubernde kann aus einer überschaubaren Menge Objekte gezielt das gewünschte herausgreifen. Er kann aus einem Kartenstapel eine bestimmte Karte ziehen, aus einem Beutel eine gewünschte Münze oder von einem Schlüsselbund den richtigen Schlüssel. Er muss dazu das gewünschte Objekt kennen und dieses muss auch wirklich an dem Ort vorhanden sein.</t>
+  </si>
+  <si>
+    <t>Mit diesem Zaubertrick kann der Zauberer telepathisch jemandem einige Grußworte übermitteln.</t>
+  </si>
+  <si>
+    <t>Elfen, Gildenmagier (Donnerbach)</t>
+  </si>
+  <si>
+    <t>Das Ziel des Zaubertricks erwidert freundlich den Gruß des Zauberers. Der Trick funktioniert nur bei Personen, die dem Zauberer zumindest neutral gegenüber eingestellt sind.</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Hesindius Lichtblick)</t>
+  </si>
+  <si>
+    <t>Der Zauberer kann die Farbe seines Haupthaars nach Belieben bestimmen. Gleiches gilt für die Länge, solange sie 1 Schritt nicht überschreitet. Schneidet der Zauberer die durch den Zaubertrick gewachsenen Haare ab, lösen sich diese sofort auf. Nachwachsende Haare sind von der Veränderung nicht betroffen.</t>
+  </si>
+  <si>
+    <t>Hexen</t>
+  </si>
+  <si>
+    <t>Dieser Zaubertrick hält die Temperatur eines maximal faustgroßen Objektes konstant, so lange es in der Hand gehalten wird, maximal jedoch 5 Minuten.</t>
+  </si>
+  <si>
+    <t>Der Zauberer zeigt auf einen Stern oder ein Sternzeichen am Himmel, der daraufhin kurz für den Zauberer und das Ziel aufleuchtet.</t>
+  </si>
+  <si>
+    <t>5 Sekunden</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Töchter Niobaras)</t>
+  </si>
+  <si>
+    <t>Mittels Hexenblick kann eine Hexe herausfinden, ob eine andere Person ebenfalls die hexische Tradition beherrscht. Sollte das ausgewählte Ziel die Tradition besitzen, so leuchten ihre Augen kurz Purpur auf, was aber nur für die zaubernde Hexe sichtbar ist.</t>
+  </si>
+  <si>
+    <t>ausschließlich Hexen</t>
+  </si>
+  <si>
+    <t>In einem Radius von 16 Schritt um den Zauberer ist eine angenehme, zum Ort passende, Hintergrundmusik zu hören. Das Stück kann der Zauberer selbst bestimmten, es muss aber zum Ambiente passen.</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Zorgan), Zauberbarden</t>
+  </si>
+  <si>
+    <t>Die Zauberin wird nicht von einfachen Insekten wie Fliegen oder Mücken belästigt. Der Zaubertrick schützt nicht vor Moskitos oder anderen Insekten, die bei Helden Schaden verursachen, Krankheiten übertragen oder ihnen gefährlich werden können. Die Insekten müssen der Größenkategorie winzig angehören.</t>
+  </si>
+  <si>
+    <t>6 Stunden</t>
+  </si>
+  <si>
+    <t>Hexen, Gildenmagier (Sinoda)</t>
+  </si>
+  <si>
+    <t>Die Hexe kann einem beliebigen Besen innerhalb der Reichweite befehlen, den Boden in einem Radius von 8 Schritt zu kehren. Der Besen weicht dabei Hindernissen aus und versucht Lebewesen der Größenkategorie klein und größer aus dem Weg zu gehen. Wird der Besen berührt, endet der Zaubertrick augenblicklich.</t>
+  </si>
+  <si>
+    <t>Objekte (Besen)</t>
+  </si>
+  <si>
+    <t>Aus dem rechten Zeigefinger des Magiers leuchtet ein schwaches Licht. Das Licht ist nicht hell genug, um Sichtmodifikatoren zu ändern, aber es reicht aus, um in der Dunkelheit ein Buch zu lesen.</t>
+  </si>
+  <si>
+    <t>Gildenmagier</t>
+  </si>
+  <si>
+    <t>Ein kleines Tier (Eichhörnchen, Taube) kommt neugierig auf den Zaubernden zu. Die Wirkung hält 5 Minuten an.</t>
+  </si>
+  <si>
+    <t>Ein kleiner Lufthauch bläst Kerzen und ähnlich große Flammen innerhalb eines Radius von 8 Schritt um den Zauberer aus.</t>
+  </si>
+  <si>
+    <t>Objekte (kleine Flammen)</t>
+  </si>
+  <si>
+    <t>Elfen, Gildenmagier</t>
+  </si>
+  <si>
+    <t>Durch diesen Trick kann der Zauberer beliebig viele seiner Finger- oder Fußnägel in einer beliebigen Farbe lackieren.</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Al’Anfa), Hexen</t>
+  </si>
+  <si>
+    <t>Dieser Zaubertrick sorgt dafür, dass die Kleidung einer Person ordentlich sitzt.</t>
+  </si>
+  <si>
+    <t>Objekte (Kleidung)</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Halle der Antimagie zu Kuslik)</t>
+  </si>
+  <si>
+    <t>Berührt der Druide eine Pflanze, kann er sich ein Bild von ihrem Gesundheitszustand machen und herausfinden, ob sie von Schädlingen befallen, vergiftet wurde oder Ähnliches.</t>
+  </si>
+  <si>
+    <t>Pflanzen</t>
+  </si>
+  <si>
+    <t>Die Augenfarbe des Zaubernden ändert sich für 5 Minuten. Es sind unnatürliche Farben möglich.</t>
+  </si>
+  <si>
+    <t>Dieser Zaubertrick sorgt dafür, dass jemand einen kleinen Schlag auf die Finger abbekommt, ganz so, als ob ihn jemand mit einem Rohrstock geschlagen hat. Schaden erleidet das Ziel dadurch nicht.</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Akademie Schwert &amp; Stab zu Gareth)</t>
+  </si>
+  <si>
+    <t>Eine Handvoll Sand beginnt sich zu einer ca. 10 Halbfinger großen Figur zu formen, die nach dem Willen des Zauberers kleine Tricks zur Unterhaltung aufführt. Die Sandfigur muss in einem Radius von 10 Halbfingern verbleiben.</t>
+  </si>
+  <si>
+    <t>Objekte (Sand)</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Vadif)</t>
+  </si>
+  <si>
+    <t>Ein aus einer Bibliothek geliehenes Buch fliegt wieder dorthin, woher es der Zauberer aus dem Regal entnommen hat. Dieser Zaubertrick funktioniert nur bei Büchern, die der Zauberer selbst ausgeliehen und aus der Bibliothek entnommen hat.</t>
+  </si>
+  <si>
+    <t>Objekte (Bücher)</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Lowangen Verwandlung)</t>
+  </si>
+  <si>
+    <t>Durch diesen Zaubertrick tragen Schminkutensilien die Schminke so wie gewünscht auf, ohne dass der Zauberer seine Hände benutzen muss. Das Ziel muss in einem ruhigen Zustand verharren, bis der Schminkvorgang vollendet ist.</t>
+  </si>
+  <si>
+    <t>Gildenmagier, Hexen, Scharlatane, Zaubertänzer</t>
+  </si>
+  <si>
+    <t>Eine kurze telekinetische Entladung mit einer Reichweite von 4 Schritt, die beispielsweise eine Münze von einem Tisch fegen kann. Sie ist nicht stark genug, um eine Glasflasche zu zerbrechen, genügt aber für eine Ohrfeige.</t>
+  </si>
+  <si>
+    <t>Objekt und Wesen</t>
+  </si>
+  <si>
+    <t>Die Hand- und Fingerknochen des Zaubernden werden sehr flexibel, sodass sie durch enge Öffnungen gezwängt werden können. Die Wirkung hält 5 Minuten an.</t>
+  </si>
+  <si>
+    <t>Auf einem leblosen Objekt nach Wahl des Zaubernden erscheint eine Glyphe oder ein Symbol und verbleibt dauerhaft. Der Zaubernde muss das Objekt berühren. Das Symbol wirkt wie gemalt und kann weggeputzt werden. Mittels dieses Tricks kann man jeweils nur eine Art von Zeichen auftauchen lassen (z. B. ein Piktogramm).</t>
+  </si>
+  <si>
+    <t>Auf dem Körper des Verzauberten entsteht eine maximal 10 Halbfinger auf 10 Halbfinger große Tätowierung nach Wunsch des Zauberers. Bei den Tätowierungen muss es sich um einfache Runen oder einfache Muster handeln.</t>
+  </si>
+  <si>
+    <t>Der Zaubernde und seine Kleidung sind etwa 5 Minuten vor Nässe, beispielsweise durch Regen oder Schnee, geschützt. Nasse Kleidung wird durch den Trick nicht wieder trocken.</t>
+  </si>
+  <si>
+    <t>Objekt und Kulturschaffende</t>
+  </si>
+  <si>
+    <t>Das Lachen des Zauberers hört sich bedrohlich und unheimlich an. Weitere regeltechnische Auswirkungen hat das Lachen jedoch nicht.</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Demirion Ophenos), Hexen</t>
+  </si>
+  <si>
+    <t>Dieser Zaubertrick reinigt eine beliebige Waffe, die der Zauberer berührt, vollständig von Flugrost, Blut und anderen Verschmutzungen.</t>
+  </si>
+  <si>
+    <t>Objekte (Waffen)</t>
+  </si>
+  <si>
+    <t>Der Zauberer kann sagen, ob ein Gewässer vor ihm tiefer ist, als er selbst groß ist.</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Thorwaler)</t>
+  </si>
+  <si>
+    <t>Die Hörer innerhalb einer Reichweite von 8 Schritt Radius um den Zauberer vernehmen eine Stimme, die ihnen eine Passage aus einem Zauberbuch vorliest. Der Text muss dem Zaubernden bekannt sein. Die Passage kann er selbst auswählen, sie muss aber innerhalb von 10 Sekunden vorlesbar sein. Nur die Personen, die die Passage hören sollen, hören sie auch, alle übrigen bekommen von der Belehrung nichts mit.</t>
+  </si>
+  <si>
+    <t>max. 10 Sekunden</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Alrik Dagabor)</t>
+  </si>
+  <si>
+    <t>Die Hexe kann mit diesem Zaubertrick eine einfache Speise, etwa eine Suppe, würzen, auch ohne über passende Gewürze wie Salz und Pfeffer zu verfügen. Ob die Speise gut gewürzt ist oder z. B. versalzen, hängt weiterhin von den Kochkünsten der Hexe ab. Die Hexe kann nur den Geschmack von Gewürzen erzeugen, die sie selbst schon einmal gekostet hat.</t>
+  </si>
+  <si>
+    <t>Objekte (Essen)</t>
+  </si>
+  <si>
+    <t>Dieser Trick verzaubert einen Federkiel, sodass dieser alles wortgetreu auf einem bereitgelegten Papier oder in ein Buch notiert, was der Zauberer sagt. Der Federkiel kann die Seiten des Buches umschlagen und taucht sich selbst in ein Tintenfäßchen ein, solange es maximal einen Schritt weit entfernt ist.</t>
+  </si>
+  <si>
+    <t>10 Minuten</t>
+  </si>
+  <si>
+    <t>Objekte (Federkiele)</t>
+  </si>
+  <si>
+    <t>Gildenmagier (Punin)</t>
+  </si>
+  <si>
+    <t>Auf der Handfläche oder dem Zeigefinger des Geweihten entsteht eine kleine Flamme, die einen Raum erhellt oder ausreicht, um eine Kerze zu entzünden. Der Geweihte kann durch die Flamme nicht verletzt werden (wohl aber durch Flammen, die durch den Feuersegen entzündet werden). Die Helligkeit der Flamme entspricht einer gewöhnlichen Kerze normaler Machart.</t>
+  </si>
+  <si>
+    <t>Ein Neugeborenes wird gesegnet und in die Gemeinschaft der Gläubigen aufgenommen. Es ist bis zum Ende der Wirkungsdauer vor dem Raub durch Kobolde, Feen und niedere Dämonen geschützt. Diese Segnung kann nur bis maximal 12 Tage nach der Geburt eingesetzt werden, danach wirkt sie nicht mehr auf das Neugeborene.</t>
+  </si>
+  <si>
+    <t>in Zwölfgötterkirchen bis zum 12. Lebensjahr</t>
+  </si>
+  <si>
+    <t>Der Gesegnete hat einmal während der Wirkungsdauer der Segnung ein Fünkchen Glück. Er kann nach dem Ablegen einer Fertigkeitsprobe 1 FP hinzuaddieren, um z. B. eine höhere Qualitätsstufe zu erreichen.</t>
+  </si>
+  <si>
+    <t>12 Stunden</t>
+  </si>
+  <si>
+    <t>12 Monate</t>
+  </si>
+  <si>
+    <t>Wer durch einen Harmoniesegen gesegnet wurde, der erfreut sich einen ganzen Tag lang positiver Gefühle. Alle Effekte, die Furcht auslösen, erhalten eine Erschwernis von 1.</t>
+  </si>
+  <si>
+    <t>Der Gesegnete erhält 1 Lebenspunkt zurück. Die Person kann nur einmal pro Tag von dieser Segnung profitieren.</t>
+  </si>
+  <si>
+    <t>4 Kampfrunden</t>
+  </si>
+  <si>
+    <t>Das gesegnete Essen ist wohlschmeckend und nahrhaft. Gifte bis Stufe 2 und Verunreinigungen werden in der Speise neutralisiert. Die Segnung reicht für eine Portion.</t>
+  </si>
+  <si>
+    <t>12 Kampfrunden</t>
+  </si>
+  <si>
+    <t>Wer von dem gesegneten Getränk trinkt, fühlt sich erfrischt. Gifte bis Stufe 2 und Verunreinigungen werden im Getränk neutralisiert. Die Segnung reicht für einen Liter.</t>
+  </si>
+  <si>
+    <t>Der Gesegnete wird von Weisheit erfüllt. Er kann die Lösung eines Problems besser erfassen und bei einer Probe auf ein Wissenstalent einen Würfel neu würfeln (wie unter dem Einsatz des Vorteils Begabung). Pro Tag kann nur ein Weisheitssegen auf eine Person angewandt werden. Nachdem die Segnung genutzt wurde, ist sie verbraucht.</t>
+  </si>
+  <si>
+    <t>Der Geweihte lässt jemanden einen Eid ablegen. Der Gesegnete empfindet den Eid als bindend und kann sich diesem nur durch eine Probe entziehen. Der Eidsprechende muss den Eid freiwillig leisten. Der Eid kann nur durch eine Probe auf *Willenskraft* erschwert um 1 gebrochen werden.</t>
+  </si>
+  <si>
+    <t>Das Grab eines Verstorbenen wird gesegnet. Um die Leiche auszugraben und das Grab zu entweihen, muss dem Grabräuber eine Probe auf *Willenskraft (Bedrohungen standhalten)* erschwert um 1 gelingen. Bei Misslingen verspürt er ein Unwohlsein, das ihn von der Grabschändung zurückhält. Nekromantische Zauber auf die Leiche sind um 1 erschwert, so lange der Körper sich im gesegneten Grab befindet.</t>
+  </si>
+  <si>
+    <t>Der Schutzsegen kann einige als unheilig geltende Wesen fernhalten. Folgende Typen von Wesen können aufgehalten werden: Untote (Hirnlose) und Dämonen (niedere Dämonen).\nBei Errichtung des kleinen Schutzsegens muss entschieden werden, welcher von beiden Typen aufgehalten wird. Das Wesen kann während der Wirkungsdauer das gesegnete Gebiet nicht betreten. Ist das Wesen gezwungen, das Gebiet zu betreten, dann versucht es sofort, sich wieder aus der Zone zurückzuziehen.\nDer Kleine Schutzsegen darf nicht größer sein als 4 Schritt Radius, sehr wohl aber kleiner. Die Zone ist stationär und bewegt sich nicht mit dem Geweihten. Wenn sich Personen innerhalb der Zone an den Rand der Zone bewegen, um dort lauernde Wesen im Nahkampf anzugreifen, können die Wesen ebenfalls angreifen.</t>
+  </si>
+  <si>
+    <t>Der Gesegnete verspürt keine Mattigkeit und Erschöpfung mehr. Er kann bei einer Probe auf *Selbstbeherrschung* einen Würfel neu würfeln (wie unter dem Einsatz des Vorteils Begabung). Pro Tag kann nur ein Stärkungssegen auf eine Person angewandt werden. Nachdem die Segnung genutzt wurde, ist sie verbraucht.</t>
+  </si>
+  <si>
+    <t>112&amp;166</t>
   </si>
 </sst>
 </file>
@@ -12916,7 +13231,40 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
-  <dxfs count="140">
+  <dxfs count="151">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -13813,7 +14161,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="139"/>
+      <tableStyleElement type="headerRow" dxfId="150"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -14177,21 +14525,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:B10" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
   <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <sortState ref="A2:B10">
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="136"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="135"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="147"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="146"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:M1048576" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:M1048576" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:M1048576" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14208,40 +14556,55 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="effect" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="castingtime" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{D89CFCD8-0667-4532-ADCB-656E0F380FC9}" name="castingtimeShort" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="aecost" dataDxfId="65"/>
-    <tableColumn id="11" xr3:uid="{AA76CB3A-D16A-4989-ACEE-9057F8B23848}" name="aecostShort" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="range" dataDxfId="63"/>
-    <tableColumn id="12" xr3:uid="{DD92ED00-D630-4075-AFBB-75382F298664}" name="rangeShort" dataDxfId="62"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="duration" dataDxfId="61"/>
-    <tableColumn id="13" xr3:uid="{35897220-D86D-43E4-9246-750CE8AD5E3B}" name="durationShort" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="target" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="src" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="effect" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="castingtime" dataDxfId="78"/>
+    <tableColumn id="10" xr3:uid="{D89CFCD8-0667-4532-ADCB-656E0F380FC9}" name="castingtimeShort" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="aecost" dataDxfId="76"/>
+    <tableColumn id="11" xr3:uid="{AA76CB3A-D16A-4989-ACEE-9057F8B23848}" name="aecostShort" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="range" dataDxfId="74"/>
+    <tableColumn id="12" xr3:uid="{DD92ED00-D630-4075-AFBB-75382F298664}" name="rangeShort" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="duration" dataDxfId="72"/>
+    <tableColumn id="13" xr3:uid="{35897220-D86D-43E4-9246-750CE8AD5E3B}" name="durationShort" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="target" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="src" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table14" displayName="Table14" ref="A1:B44" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
-  <autoFilter ref="A1:B44" xr:uid="{00000000-0009-0000-0100-00000E000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table14" displayName="Table14" ref="A1:H44" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+  <autoFilter ref="A1:H44" xr:uid="{00000000-0009-0000-0100-00000E000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="id" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="name" dataDxfId="54"/>
+  <sortState ref="A2:H44">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="id" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="name" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{7C0356E8-3E12-4648-AED9-D4476F17A0CC}" name="effect" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{03F4DA49-0E9B-4841-B835-1233F9A33781}" name="range" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{1B189756-8D73-4A73-878A-C6D669265233}" name="duration" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{39D35FEE-F7F7-43E2-8D36-B288D27F4FED}" name="target" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{05155ABB-B917-4A7E-A43F-F1AF0533E4BC}" name="note" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{0202CF45-C4D3-4A21-820D-5E5F4A183383}" name="src" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:M193" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:M193" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <autoFilter ref="A1:M193" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14261,40 +14624,50 @@
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{452BCF15-63D6-4F0D-8237-F453C9931794}" name="effect" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{3C4B8B30-E7ED-4AB5-BC66-F5C283820DD3}" name="castingtime" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{EDD4FA58-CDB8-416C-923B-13AE644AA21A}" name="castingtimeShort" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{E3A80605-B07C-400F-9DD6-DA1ECD45B17F}" name="kpcost" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{3735962A-FF4F-4E3D-9AFC-95B48BCF0758}" name="kpcostShort" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{4D0248C5-34EF-49A3-B1B4-33D1C05D9FBB}" name="range" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{D6111C84-C6C2-4C98-9BAC-040E9A31F2B9}" name="rangeShort" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{F33F5A8B-FEA1-4B00-AE2D-20CCBB24FF2A}" name="duration" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{66749CC6-D9C4-4BF4-BA63-F5A58FD8E6CB}" name="durationShort" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{BE17D95F-F42A-48F5-9E7F-A545D95D81C2}" name="target" dataDxfId="40"/>
-    <tableColumn id="13" xr3:uid="{1E0275F4-0996-4EC0-B571-4BB2870B8257}" name="src" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{452BCF15-63D6-4F0D-8237-F453C9931794}" name="effect" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{3C4B8B30-E7ED-4AB5-BC66-F5C283820DD3}" name="castingtime" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{EDD4FA58-CDB8-416C-923B-13AE644AA21A}" name="castingtimeShort" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{E3A80605-B07C-400F-9DD6-DA1ECD45B17F}" name="kpcost" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{3735962A-FF4F-4E3D-9AFC-95B48BCF0758}" name="kpcostShort" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{4D0248C5-34EF-49A3-B1B4-33D1C05D9FBB}" name="range" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{D6111C84-C6C2-4C98-9BAC-040E9A31F2B9}" name="rangeShort" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{F33F5A8B-FEA1-4B00-AE2D-20CCBB24FF2A}" name="duration" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{66749CC6-D9C4-4BF4-BA63-F5A58FD8E6CB}" name="durationShort" dataDxfId="52"/>
+    <tableColumn id="12" xr3:uid="{BE17D95F-F42A-48F5-9E7F-A545D95D81C2}" name="target" dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{1E0275F4-0996-4EC0-B571-4BB2870B8257}" name="src" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="A1:B13" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="A1:B13" xr:uid="{00000000-0009-0000-0100-000010000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="A1:G13" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="A1:G13" xr:uid="{00000000-0009-0000-0100-000010000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="35"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{459C17AD-3409-41D7-8801-F6FE1515AFC9}" name="effect" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{6753AB3A-2424-4D10-84BF-032777BAF818}" name="range" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4411F645-F9D2-4514-A703-39B5D9965BFB}" name="duration" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{F4CC0549-F8A2-48BA-8FC4-7D4AD9A2368C}" name="target" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C43A0203-6258-4D01-A81A-CBAD9FBB7A23}" name="src" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:J664" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:J664" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A1:J664" xr:uid="{00000000-0009-0000-0100-000006000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14308,37 +14681,37 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="sel" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="input" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column1" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column2" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column3" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Column4" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Column5" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Column6" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="sel" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="input" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column1" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column2" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column3" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Column4" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Column5" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Column6" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:B111" xr:uid="{00000000-0009-0000-0100-00000A000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:D76" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14346,73 +14719,73 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="spec" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="specInput" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="spec" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="specInput" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:B36" xr:uid="{00000000-0009-0000-0100-00000B000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table15" displayName="Table15" ref="A1:B466" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table15" displayName="Table15" ref="A1:B466" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A1:B466" xr:uid="{00000000-0009-0000-0100-00000F000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="6" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="17" dataCellStyle="Excel Built-in Normal"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{BB3927CB-5698-4DFF-B48D-425D7E21C02B}" name="Tabelle20" displayName="Tabelle20" ref="A1:B577" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{BB3927CB-5698-4DFF-B48D-425D7E21C02B}" name="Tabelle20" displayName="Tabelle20" ref="A1:B577" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A1:B577" xr:uid="{27BF4B55-7C3C-4E9B-A139-DBDDC3FBF905}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3B1007AC-E41F-48C9-90A0-CCE4A91720CD}" name="id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{2C7E5741-9086-4357-A3F3-05CB168DE409}" name="name" dataDxfId="3" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="1" xr3:uid="{3B1007AC-E41F-48C9-90A0-CCE4A91720CD}" name="id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{2C7E5741-9086-4357-A3F3-05CB168DE409}" name="name" dataDxfId="14" dataCellStyle="Excel Built-in Normal"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="145" dataDxfId="144">
   <autoFilter ref="A1:B8" xr:uid="{00000000-0009-0000-0100-00000D000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="132"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="131"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="143"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="142"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:B546" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:B546" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:B546" xr:uid="{00000000-0009-0000-0100-000009000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14421,15 +14794,15 @@
     <sortCondition ref="A1:A474"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:K13" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:K13" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140">
   <autoFilter ref="A1:K13" xr:uid="{00000000-0009-0000-0100-000012000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14441,24 +14814,24 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="128"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="attributeAdjustments" dataDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="automaticAdvantages" dataDxfId="125"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="stronglyRecommendedAdvantages" dataDxfId="124"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="stronglyRecommendedDisadvantages" dataDxfId="123"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="commonAdvantages" dataDxfId="122"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="commonDisadvantages" dataDxfId="121"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="uncommonAdvantages" dataDxfId="120"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="uncommonDisadvantages" dataDxfId="119"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="src" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="139"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="138"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="attributeAdjustments" dataDxfId="137"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="automaticAdvantages" dataDxfId="136"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="stronglyRecommendedAdvantages" dataDxfId="135"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="stronglyRecommendedDisadvantages" dataDxfId="134"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="commonAdvantages" dataDxfId="133"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="commonDisadvantages" dataDxfId="132"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="uncommonAdvantages" dataDxfId="131"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="uncommonDisadvantages" dataDxfId="130"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="src" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{B4F1794A-E7C4-468F-B8D8-970C354AABE6}" name="Tabelle19" displayName="Tabelle19" ref="A1:M27" totalsRowShown="0" headerRowDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{B4F1794A-E7C4-468F-B8D8-970C354AABE6}" name="Tabelle19" displayName="Tabelle19" ref="A1:M27" totalsRowShown="0" headerRowDxfId="128">
   <autoFilter ref="A1:M27" xr:uid="{CF034C78-9071-47EC-AB34-3D606EE1BBA0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14475,9 +14848,9 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{323211C5-81FD-41D0-9F64-A33241693AC3}" name="id" dataDxfId="116"/>
-    <tableColumn id="2" xr3:uid="{FDC1B446-D119-4AB0-BFD5-ACF6E75BA8A5}" name="name" dataDxfId="115"/>
-    <tableColumn id="3" xr3:uid="{92A07580-4496-4839-BDFD-3E1CD0593E78}" name="areaKnowledgeShort" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{323211C5-81FD-41D0-9F64-A33241693AC3}" name="id" dataDxfId="127"/>
+    <tableColumn id="2" xr3:uid="{FDC1B446-D119-4AB0-BFD5-ACF6E75BA8A5}" name="name" dataDxfId="126"/>
+    <tableColumn id="3" xr3:uid="{92A07580-4496-4839-BDFD-3E1CD0593E78}" name="areaKnowledgeShort" dataDxfId="125"/>
     <tableColumn id="4" xr3:uid="{44EF4FF0-9A41-48CA-BC45-CC1B1304A096}" name="areaKnowledge"/>
     <tableColumn id="5" xr3:uid="{3A9496F5-2D90-4F09-9E2B-F936A6E5B397}" name="commonMundaneProfessions"/>
     <tableColumn id="6" xr3:uid="{7D2183EE-15A4-4FF4-9222-723CACFF8CAA}" name="commonMagicalProfessions"/>
@@ -14487,14 +14860,14 @@
     <tableColumn id="10" xr3:uid="{745A9F74-C60C-4CBC-9102-98FE33FC8526}" name="uncommonAdvantages"/>
     <tableColumn id="11" xr3:uid="{C1FC4429-9AFB-46A3-A828-99A029A30219}" name="uncommonDisadvantages"/>
     <tableColumn id="12" xr3:uid="{839A4140-773B-4A98-9156-075E987FA39A}" name="commonNames"/>
-    <tableColumn id="13" xr3:uid="{8C51E69A-3B2D-4662-B403-D59D4610C76D}" name="src" dataDxfId="113"/>
+    <tableColumn id="13" xr3:uid="{8C51E69A-3B2D-4662-B403-D59D4610C76D}" name="src" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="A1:G95" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14505,20 +14878,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="id" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="name" dataDxfId="109"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="name_f" dataDxfId="108"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="subname" dataDxfId="107"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="subname_f" dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="req" dataDxfId="105"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="src" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="id" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="name" dataDxfId="120"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="name_f" dataDxfId="119"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="subname" dataDxfId="118"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="subname_f" dataDxfId="117"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="req" dataDxfId="116"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="src" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
   <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14527,18 +14900,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="id" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="name" dataDxfId="100"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="name_f" dataDxfId="99"/>
-    <tableColumn id="3" xr3:uid="{091296A4-103F-48ED-8EF3-B2FEB3C87545}" name="precedingText" dataDxfId="98"/>
-    <tableColumn id="4" xr3:uid="{7DC6E788-BCD5-45BD-8F54-8F4B65BB3D80}" name="concludingText" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="id" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="name" dataDxfId="111"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="name_f" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{091296A4-103F-48ED-8EF3-B2FEB3C87545}" name="precedingText" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{7DC6E788-BCD5-45BD-8F54-8F4B65BB3D80}" name="concludingText" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:D97" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:D97" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A1:D97" xr:uid="{00000000-0009-0000-0100-000008000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14546,17 +14919,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="93"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="sel" dataDxfId="92"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="input" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="104"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="sel" dataDxfId="103"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="input" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:D74" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:D74" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="A1:D74" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14564,17 +14937,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="id" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="name" dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="sel" dataDxfId="86"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="input" dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="id" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="name" dataDxfId="98"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="sel" dataDxfId="97"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="input" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A1:J60" xr:uid="{00000000-0009-0000-0100-000007000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -14591,16 +14964,16 @@
     <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="id" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="name" dataDxfId="81"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="spec" dataDxfId="80"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="spec_input" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="tools" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="quality" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="failed" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="critical" dataDxfId="75"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="botch" dataDxfId="74"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="src" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="id" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="name" dataDxfId="92"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="spec" dataDxfId="91"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="spec_input" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="tools" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="quality" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="failed" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="critical" dataDxfId="86"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="botch" dataDxfId="85"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="src" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14906,7 +15279,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -25957,374 +26330,1143 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="10.6640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="3.73046875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="18" t="s">
+        <v>2696</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>2699</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>2700</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>2701</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>4185</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" s="17" t="s">
+        <v>4182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>2855</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" s="17" t="s">
+        <v>4189</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>2741</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>2853</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" s="17" t="s">
+        <v>4197</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" s="17" t="s">
+        <v>4202</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" s="17" t="s">
+        <v>4203</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>2855</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7" s="17" t="s">
+        <v>4210</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>2855</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" s="17" t="s">
+        <v>4225</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>2856</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9" s="17" t="s">
+        <v>4236</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10" s="17" t="s">
+        <v>4249</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11" s="17" t="s">
+        <v>4247</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>4248</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12" s="17" t="s">
+        <v>4250</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>2855</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13" s="17" t="s">
+        <v>4252</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>4253</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1863</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14" s="17" t="s">
+        <v>4187</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>4188</v>
+      </c>
+      <c r="H14" s="17">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1864</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C15" s="17" t="s">
+        <v>4190</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>4191</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>2856</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>4188</v>
+      </c>
+      <c r="H15" s="17">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1865</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C16" s="17" t="s">
+        <v>4214</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>4215</v>
+      </c>
+      <c r="H16" s="17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1866</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C17" s="17" t="s">
+        <v>4221</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>2746</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>4222</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>4209</v>
+      </c>
+      <c r="H17" s="17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1867</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C18" s="17" t="s">
+        <v>4223</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>2799</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>2746</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>4224</v>
+      </c>
+      <c r="H18" s="17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1868</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C19" s="17" t="s">
+        <v>4234</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>4235</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>4188</v>
+      </c>
+      <c r="H19" s="17">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1869</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C20" s="17" t="s">
+        <v>4256</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>4257</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>4224</v>
+      </c>
+      <c r="H20" s="17">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1870</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C21" s="17" t="s">
+        <v>4263</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>2799</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>4264</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>4209</v>
+      </c>
+      <c r="H21" s="17">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1871</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C22" s="17" t="s">
+        <v>4183</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>4186</v>
+      </c>
+      <c r="H22" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1872</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C23" s="17" t="s">
+        <v>4192</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>4193</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>4194</v>
+      </c>
+      <c r="H23" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1873</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C24" s="17" t="s">
+        <v>4195</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>2812</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>4196</v>
+      </c>
+      <c r="H24" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1874</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C25" s="17" t="s">
+        <v>4198</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>4199</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>4200</v>
+      </c>
+      <c r="H25" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>1875</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C26" s="17" t="s">
+        <v>4201</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>2798</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>2866</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>1876</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C27" s="17" t="s">
+        <v>4204</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>4205</v>
+      </c>
+      <c r="H27" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>1877</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C28" s="17" t="s">
+        <v>4206</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>4207</v>
+      </c>
+      <c r="H28" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>1878</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C29" s="17" t="s">
+        <v>4208</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>4209</v>
+      </c>
+      <c r="H29" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>1879</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C30" s="17" t="s">
+        <v>4211</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>4212</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>4213</v>
+      </c>
+      <c r="H30" s="17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>1880</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C31" s="17" t="s">
+        <v>4216</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>2853</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>4217</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1881</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C32" s="17" t="s">
+        <v>4218</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>4219</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>4220</v>
+      </c>
+      <c r="H32" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>1882</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C33" s="17" t="s">
+        <v>4226</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>4227</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>4228</v>
+      </c>
+      <c r="H33" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>1883</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C34" s="17" t="s">
+        <v>4229</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>4230</v>
+      </c>
+      <c r="H34" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>1884</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C35" s="17" t="s">
+        <v>4231</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>4219</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>4232</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>4233</v>
+      </c>
+      <c r="H35" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>1885</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C36" s="17" t="s">
+        <v>4237</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>4238</v>
+      </c>
+      <c r="H36" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>1886</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C37" s="17" t="s">
+        <v>4239</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>2799</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>2812</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>4240</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>4241</v>
+      </c>
+      <c r="H37" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>1887</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C38" s="17" t="s">
+        <v>4245</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>4246</v>
+      </c>
+      <c r="H38" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>1888</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C39" s="17" t="s">
+        <v>4242</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>2798</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>4243</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>4244</v>
+      </c>
+      <c r="H39" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>1889</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C40" s="17" t="s">
+        <v>4251</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>4193</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>4224</v>
+      </c>
+      <c r="H40" s="17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>1890</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C41" s="17" t="s">
+        <v>4254</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>4255</v>
+      </c>
+      <c r="H41" s="17">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>1891</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C42" s="17" t="s">
+        <v>4258</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>2853</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>4259</v>
+      </c>
+      <c r="H42" s="17">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>1892</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C43" s="17" t="s">
+        <v>4260</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>4261</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>4262</v>
+      </c>
+      <c r="H43" s="17">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>1893</v>
       </c>
+      <c r="C44" s="17" t="s">
+        <v>4265</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>2799</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>4266</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>4267</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>4268</v>
+      </c>
+      <c r="H44" s="17">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -26333,7 +27475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
@@ -29087,120 +30229,316 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.73046875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="18" t="s">
+        <v>2696</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>2699</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>2700</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>2701</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" s="17" t="s">
+        <v>4282</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2839</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G2" s="17">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" s="17" t="s">
+        <v>4269</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>2747</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G3" s="17">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" s="17" t="s">
+        <v>4270</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>4271</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G4" s="17">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" s="17" t="s">
+        <v>4272</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>4273</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G5" s="17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" s="17" t="s">
+        <v>4283</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>4274</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>2853</v>
+      </c>
+      <c r="G6" s="17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7" s="17" t="s">
+        <v>4275</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>4273</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G7" s="17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" s="17" t="s">
+        <v>4276</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G8" s="17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9" s="17" t="s">
+        <v>4284</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>4277</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>2853</v>
+      </c>
+      <c r="G9" s="17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10" s="17" t="s">
+        <v>4278</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>2855</v>
+      </c>
+      <c r="G10" s="17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11" s="17" t="s">
+        <v>4285</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>4279</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G11" s="17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12" s="17" t="s">
+        <v>4280</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>2803</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>2855</v>
+      </c>
+      <c r="G12" s="17">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>502</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>4281</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>4273</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>4184</v>
+      </c>
+      <c r="G13" s="17">
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed autoUpdater infos and magical professions text for culture "Erzzwerge"
</commit_message>
<xml_diff>
--- a/src/data/TDE5_de-DE.xlsx
+++ b/src/data/TDE5_de-DE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="7755" firstSheet="13" activeTab="20" xr2:uid="{20ED8CD0-32B3-4B44-9637-7F04B1E30A79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="7755" firstSheet="1" activeTab="3" xr2:uid="{20ED8CD0-32B3-4B44-9637-7F04B1E30A79}"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="30" r:id="rId1"/>
@@ -51523,7 +51523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BDF849A-84B1-4731-B5ED-CC1BDC8FBE84}">
   <dimension ref="A1:C577"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C577"/>
     </sheetView>
   </sheetViews>
@@ -62640,8 +62640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -63621,7 +63621,7 @@
         <v>4453</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>4453</v>
+        <v>4545</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16" t="s">

</xml_diff>

<commit_message>
Reworked races representation to fit Core Rules
</commit_message>
<xml_diff>
--- a/src/data/TDE5_de-DE.xlsx
+++ b/src/data/TDE5_de-DE.xlsx
@@ -9,31 +9,32 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="7755" xr2:uid="{20ED8CD0-32B3-4B44-9637-7F04B1E30A79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="7755" activeTab="3" xr2:uid="{20ED8CD0-32B3-4B44-9637-7F04B1E30A79}"/>
   </bookViews>
   <sheets>
     <sheet name="BOOKS" sheetId="30" r:id="rId1"/>
     <sheet name="EXPERIENCE_LEVELS" sheetId="25" r:id="rId2"/>
     <sheet name="RACES" sheetId="2" r:id="rId3"/>
-    <sheet name="CULTURES" sheetId="5" r:id="rId4"/>
-    <sheet name="PROFESSIONS" sheetId="7" r:id="rId5"/>
-    <sheet name="PROFESSION_VARIANTS" sheetId="16" r:id="rId6"/>
-    <sheet name="ADVANTAGES" sheetId="8" r:id="rId7"/>
-    <sheet name="DISADVANTAGES" sheetId="11" r:id="rId8"/>
-    <sheet name="ATTRIBUTES" sheetId="18" r:id="rId9"/>
-    <sheet name="SKILLS" sheetId="9" r:id="rId10"/>
-    <sheet name="COMBAT_TECHNIQUES" sheetId="10" r:id="rId11"/>
-    <sheet name="SPELLS" sheetId="12" r:id="rId12"/>
-    <sheet name="CANTRIPS" sheetId="28" r:id="rId13"/>
-    <sheet name="CHANTS" sheetId="13" r:id="rId14"/>
-    <sheet name="BLESSINGS" sheetId="29" r:id="rId15"/>
-    <sheet name="SPECIAL_ABILITIES" sheetId="14" r:id="rId16"/>
-    <sheet name="TradeSecr" sheetId="22" r:id="rId17"/>
-    <sheet name="Languages" sheetId="24" r:id="rId18"/>
-    <sheet name="Scripts" sheetId="23" r:id="rId19"/>
-    <sheet name="SpellX" sheetId="27" r:id="rId20"/>
-    <sheet name="ChantX" sheetId="31" r:id="rId21"/>
-    <sheet name="EQUIPMENT" sheetId="15" r:id="rId22"/>
+    <sheet name="RACE_VARIANTS" sheetId="32" r:id="rId4"/>
+    <sheet name="CULTURES" sheetId="5" r:id="rId5"/>
+    <sheet name="PROFESSIONS" sheetId="7" r:id="rId6"/>
+    <sheet name="PROFESSION_VARIANTS" sheetId="16" r:id="rId7"/>
+    <sheet name="ADVANTAGES" sheetId="8" r:id="rId8"/>
+    <sheet name="DISADVANTAGES" sheetId="11" r:id="rId9"/>
+    <sheet name="ATTRIBUTES" sheetId="18" r:id="rId10"/>
+    <sheet name="SKILLS" sheetId="9" r:id="rId11"/>
+    <sheet name="COMBAT_TECHNIQUES" sheetId="10" r:id="rId12"/>
+    <sheet name="SPELLS" sheetId="12" r:id="rId13"/>
+    <sheet name="CANTRIPS" sheetId="28" r:id="rId14"/>
+    <sheet name="CHANTS" sheetId="13" r:id="rId15"/>
+    <sheet name="BLESSINGS" sheetId="29" r:id="rId16"/>
+    <sheet name="SPECIAL_ABILITIES" sheetId="14" r:id="rId17"/>
+    <sheet name="TradeSecr" sheetId="22" r:id="rId18"/>
+    <sheet name="Languages" sheetId="24" r:id="rId19"/>
+    <sheet name="Scripts" sheetId="23" r:id="rId20"/>
+    <sheet name="SpellX" sheetId="27" r:id="rId21"/>
+    <sheet name="ChantX" sheetId="31" r:id="rId22"/>
+    <sheet name="EQUIPMENT" sheetId="15" r:id="rId23"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10056" uniqueCount="5284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10042" uniqueCount="5286">
   <si>
     <t>id</t>
   </si>
@@ -15931,6 +15932,12 @@
   </si>
   <si>
     <t>AMAI</t>
+  </si>
+  <si>
+    <t>Menschen</t>
+  </si>
+  <si>
+    <t>Elfen</t>
   </si>
 </sst>
 </file>
@@ -16264,7 +16271,31 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
-  <dxfs count="165">
+  <dxfs count="173">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -17252,7 +17283,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="164"/>
+      <tableStyleElement type="headerRow" dxfId="172"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -17616,7 +17647,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:C12" totalsRowShown="0" headerRowDxfId="163" dataDxfId="162">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table17" displayName="Table17" ref="A1:C12" totalsRowShown="0" headerRowDxfId="171" dataDxfId="170">
   <autoFilter ref="A1:C12" xr:uid="{00000000-0009-0000-0100-000011000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17626,16 +17657,49 @@
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{85D136C5-D53F-4434-AD97-0FFCD29F6BC8}" name="short" dataDxfId="160"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="159"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="169"/>
+    <tableColumn id="3" xr3:uid="{85D136C5-D53F-4434-AD97-0FFCD29F6BC8}" name="short" dataDxfId="168"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="167"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:M1048576" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+  <autoFilter ref="A1:J60" xr:uid="{00000000-0009-0000-0100-000007000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+  </autoFilter>
+  <sortState ref="A2:D60">
+    <sortCondition ref="A1:A60"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="id" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="name" dataDxfId="102"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="spec" dataDxfId="101"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="spec_input" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="tools" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="quality" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="failed" dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="critical" dataDxfId="96"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="botch" dataDxfId="95"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="src" dataDxfId="94"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabelle4" displayName="Tabelle4" ref="A1:M1048576" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="A1:M1048576" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17652,26 +17716,26 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="82"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="effect" dataDxfId="81"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="castingtime" dataDxfId="80"/>
-    <tableColumn id="10" xr3:uid="{D89CFCD8-0667-4532-ADCB-656E0F380FC9}" name="castingtimeShort" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="aecost" dataDxfId="78"/>
-    <tableColumn id="11" xr3:uid="{AA76CB3A-D16A-4989-ACEE-9057F8B23848}" name="aecostShort" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="range" dataDxfId="76"/>
-    <tableColumn id="12" xr3:uid="{DD92ED00-D630-4075-AFBB-75382F298664}" name="rangeShort" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="duration" dataDxfId="74"/>
-    <tableColumn id="13" xr3:uid="{35897220-D86D-43E4-9246-750CE8AD5E3B}" name="durationShort" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="target" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="src" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="id" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="name" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="effect" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="castingtime" dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{D89CFCD8-0667-4532-ADCB-656E0F380FC9}" name="castingtimeShort" dataDxfId="87"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="aecost" dataDxfId="86"/>
+    <tableColumn id="11" xr3:uid="{AA76CB3A-D16A-4989-ACEE-9057F8B23848}" name="aecostShort" dataDxfId="85"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="range" dataDxfId="84"/>
+    <tableColumn id="12" xr3:uid="{DD92ED00-D630-4075-AFBB-75382F298664}" name="rangeShort" dataDxfId="83"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="duration" dataDxfId="82"/>
+    <tableColumn id="13" xr3:uid="{35897220-D86D-43E4-9246-750CE8AD5E3B}" name="durationShort" dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="target" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="src" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table14" displayName="Table14" ref="A1:H44" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table14" displayName="Table14" ref="A1:H44" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A1:H44" xr:uid="{00000000-0009-0000-0100-00000E000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17686,21 +17750,21 @@
     <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="id" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="name" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{7C0356E8-3E12-4648-AED9-D4476F17A0CC}" name="effect" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{03F4DA49-0E9B-4841-B835-1233F9A33781}" name="range" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{1B189756-8D73-4A73-878A-C6D669265233}" name="duration" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{39D35FEE-F7F7-43E2-8D36-B288D27F4FED}" name="target" dataDxfId="63"/>
-    <tableColumn id="7" xr3:uid="{05155ABB-B917-4A7E-A43F-F1AF0533E4BC}" name="note" dataDxfId="62"/>
-    <tableColumn id="8" xr3:uid="{0202CF45-C4D3-4A21-820D-5E5F4A183383}" name="src" dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="id" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="name" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{7C0356E8-3E12-4648-AED9-D4476F17A0CC}" name="effect" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{03F4DA49-0E9B-4841-B835-1233F9A33781}" name="range" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{1B189756-8D73-4A73-878A-C6D669265233}" name="duration" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{39D35FEE-F7F7-43E2-8D36-B288D27F4FED}" name="target" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{05155ABB-B917-4A7E-A43F-F1AF0533E4BC}" name="note" dataDxfId="70"/>
+    <tableColumn id="8" xr3:uid="{0202CF45-C4D3-4A21-820D-5E5F4A183383}" name="src" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:M193" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabelle5" displayName="Tabelle5" ref="A1:M193" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A1:M193" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17720,26 +17784,26 @@
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{452BCF15-63D6-4F0D-8237-F453C9931794}" name="effect" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{3C4B8B30-E7ED-4AB5-BC66-F5C283820DD3}" name="castingtime" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{EDD4FA58-CDB8-416C-923B-13AE644AA21A}" name="castingtimeShort" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{E3A80605-B07C-400F-9DD6-DA1ECD45B17F}" name="kpcost" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{3735962A-FF4F-4E3D-9AFC-95B48BCF0758}" name="kpcostShort" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{4D0248C5-34EF-49A3-B1B4-33D1C05D9FBB}" name="range" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{D6111C84-C6C2-4C98-9BAC-040E9A31F2B9}" name="rangeShort" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{F33F5A8B-FEA1-4B00-AE2D-20CCBB24FF2A}" name="duration" dataDxfId="49"/>
-    <tableColumn id="11" xr3:uid="{66749CC6-D9C4-4BF4-BA63-F5A58FD8E6CB}" name="durationShort" dataDxfId="48"/>
-    <tableColumn id="12" xr3:uid="{BE17D95F-F42A-48F5-9E7F-A545D95D81C2}" name="target" dataDxfId="47"/>
-    <tableColumn id="13" xr3:uid="{1E0275F4-0996-4EC0-B571-4BB2870B8257}" name="src" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="id" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="name" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{452BCF15-63D6-4F0D-8237-F453C9931794}" name="effect" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{3C4B8B30-E7ED-4AB5-BC66-F5C283820DD3}" name="castingtime" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{EDD4FA58-CDB8-416C-923B-13AE644AA21A}" name="castingtimeShort" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{E3A80605-B07C-400F-9DD6-DA1ECD45B17F}" name="kpcost" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{3735962A-FF4F-4E3D-9AFC-95B48BCF0758}" name="kpcostShort" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{4D0248C5-34EF-49A3-B1B4-33D1C05D9FBB}" name="range" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{D6111C84-C6C2-4C98-9BAC-040E9A31F2B9}" name="rangeShort" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{F33F5A8B-FEA1-4B00-AE2D-20CCBB24FF2A}" name="duration" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{66749CC6-D9C4-4BF4-BA63-F5A58FD8E6CB}" name="durationShort" dataDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{BE17D95F-F42A-48F5-9E7F-A545D95D81C2}" name="target" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{1E0275F4-0996-4EC0-B571-4BB2870B8257}" name="src" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="A1:G13" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table16" displayName="Table16" ref="A1:G13" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:G13" xr:uid="{00000000-0009-0000-0100-000010000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17750,20 +17814,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{459C17AD-3409-41D7-8801-F6FE1515AFC9}" name="effect" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{6753AB3A-2424-4D10-84BF-032777BAF818}" name="range" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{4411F645-F9D2-4514-A703-39B5D9965BFB}" name="duration" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{F4CC0549-F8A2-48BA-8FC4-7D4AD9A2368C}" name="target" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{C43A0203-6258-4D01-A81A-CBAD9FBB7A23}" name="src" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="id" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="name" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{459C17AD-3409-41D7-8801-F6FE1515AFC9}" name="effect" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{6753AB3A-2424-4D10-84BF-032777BAF818}" name="range" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{4411F645-F9D2-4514-A703-39B5D9965BFB}" name="duration" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{F4CC0549-F8A2-48BA-8FC4-7D4AD9A2368C}" name="target" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{C43A0203-6258-4D01-A81A-CBAD9FBB7A23}" name="src" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:J664" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabelle6" displayName="Tabelle6" ref="A1:J664" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A1:J664" xr:uid="{00000000-0009-0000-0100-000006000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17777,37 +17841,37 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="sel" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="input" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column1" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column2" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column3" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Column4" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Column5" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Column6" dataDxfId="25"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:B111" xr:uid="{00000000-0009-0000-0100-00000A000000}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="id" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="name" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="sel" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="input" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column1" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column2" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column3" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="Column4" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="Column5" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="Column6" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table10" displayName="Table10" ref="A1:B111" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:B111" xr:uid="{00000000-0009-0000-0100-00000A000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="id" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="name" dataDxfId="29"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table12" displayName="Table12" ref="A1:D76" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:D76" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17815,77 +17879,77 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="spec" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="specInput" dataDxfId="15"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:B36" xr:uid="{00000000-0009-0000-0100-00000B000000}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="id" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="name" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="spec" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="specInput" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table15" displayName="Table15" ref="A1:C466" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table11" displayName="Table11" ref="A1:B36" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:B36" xr:uid="{00000000-0009-0000-0100-00000B000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="id" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="name" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table15" displayName="Table15" ref="A1:C466" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:C466" xr:uid="{00000000-0009-0000-0100-00000F000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="8" dataCellStyle="Excel Built-in Normal"/>
-    <tableColumn id="3" xr3:uid="{5F05CA31-8C2A-4303-BD9A-7E27EC13CA17}" name="effect" dataDxfId="7" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="id" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="name" dataDxfId="16" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="3" xr3:uid="{5F05CA31-8C2A-4303-BD9A-7E27EC13CA17}" name="effect" dataDxfId="15" dataCellStyle="Excel Built-in Normal"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{BB3927CB-5698-4DFF-B48D-425D7E21C02B}" name="Tabelle20" displayName="Tabelle20" ref="A1:C577" totalsRowShown="0" headerRowDxfId="6">
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165">
+  <autoFilter ref="A1:B8" xr:uid="{00000000-0009-0000-0100-00000D000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="164"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="163"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{BB3927CB-5698-4DFF-B48D-425D7E21C02B}" name="Tabelle20" displayName="Tabelle20" ref="A1:C577" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:C577" xr:uid="{27BF4B55-7C3C-4E9B-A139-DBDDC3FBF905}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3B1007AC-E41F-48C9-90A0-CCE4A91720CD}" name="id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{2C7E5741-9086-4357-A3F3-05CB168DE409}" name="name" dataDxfId="4" dataCellStyle="Excel Built-in Normal"/>
-    <tableColumn id="3" xr3:uid="{0656219C-B222-4E12-99AC-408E03225953}" name="effect" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3B1007AC-E41F-48C9-90A0-CCE4A91720CD}" name="id" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2C7E5741-9086-4357-A3F3-05CB168DE409}" name="name" dataDxfId="12" dataCellStyle="Excel Built-in Normal"/>
+    <tableColumn id="3" xr3:uid="{0656219C-B222-4E12-99AC-408E03225953}" name="effect" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B8" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157">
-  <autoFilter ref="A1:B8" xr:uid="{00000000-0009-0000-0100-00000D000000}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="156"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="name" dataDxfId="155"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:B546" totalsRowShown="0" headerRowDxfId="2">
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabelle9" displayName="Tabelle9" ref="A1:B546" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:B546" xr:uid="{00000000-0009-0000-0100-000009000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17894,16 +17958,16 @@
     <sortCondition ref="A1:A474"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="id" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="name" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:K13" totalsRowShown="0" headerRowDxfId="154" dataDxfId="153">
-  <autoFilter ref="A1:K13" xr:uid="{00000000-0009-0000-0100-000012000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle18" displayName="Tabelle18" ref="A1:K5" totalsRowShown="0" headerRowDxfId="162" dataDxfId="161">
+  <autoFilter ref="A1:K5" xr:uid="{00000000-0009-0000-0100-000012000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -17914,24 +17978,46 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="152"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="151"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="attributeAdjustments" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="automaticAdvantages" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="stronglyRecommendedAdvantages" dataDxfId="148"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="stronglyRecommendedDisadvantages" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="commonAdvantages" dataDxfId="146"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="commonDisadvantages" dataDxfId="145"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="uncommonAdvantages" dataDxfId="144"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="uncommonDisadvantages" dataDxfId="143"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="src" dataDxfId="142"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="160"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name" dataDxfId="159"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="attributeAdjustments" dataDxfId="158"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="automaticAdvantages" dataDxfId="157"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="stronglyRecommendedAdvantages" dataDxfId="156"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="stronglyRecommendedDisadvantages" dataDxfId="155"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="commonAdvantages" dataDxfId="154"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="commonDisadvantages" dataDxfId="153"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="uncommonAdvantages" dataDxfId="152"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="uncommonDisadvantages" dataDxfId="151"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="src" dataDxfId="150"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{B4F1794A-E7C4-468F-B8D8-970C354AABE6}" name="Tabelle19" displayName="Tabelle19" ref="A1:N28" totalsRowShown="0" headerRowDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{DA00A1B8-C21A-4F43-95C8-F1DADB44E1BF}" name="Tabelle21" displayName="Tabelle21" ref="A1:F11" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:F11" xr:uid="{2015DD2A-94FE-48A1-9A21-79210BEC8E55}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{68ECDEF1-44D6-4F79-827E-997DF7EB74ED}" name="id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F4F7839D-68A9-4C0A-9D9C-DE3DB776A2ED}" name="name" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{E9F2498B-1886-4D09-B068-B47D26834095}" name="commonAdvantages" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{0E599C63-430E-4B36-B37B-050F33DE8F76}" name="commonDisadvantages" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{6EFF4D94-3393-4282-B04D-B089D19495C2}" name="uncommonAdvantages" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{D350FF7F-C799-4DB8-9475-76B49505ABD6}" name="uncommonDisadvantages" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{B4F1794A-E7C4-468F-B8D8-970C354AABE6}" name="Tabelle19" displayName="Tabelle19" ref="A1:N28" totalsRowShown="0" headerRowDxfId="149">
   <autoFilter ref="A1:N28" xr:uid="{CF034C78-9071-47EC-AB34-3D606EE1BBA0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17948,9 +18034,9 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{323211C5-81FD-41D0-9F64-A33241693AC3}" name="id" dataDxfId="140"/>
-    <tableColumn id="2" xr3:uid="{FDC1B446-D119-4AB0-BFD5-ACF6E75BA8A5}" name="name" dataDxfId="139"/>
-    <tableColumn id="3" xr3:uid="{92A07580-4496-4839-BDFD-3E1CD0593E78}" name="areaKnowledgeShort" dataDxfId="138"/>
+    <tableColumn id="1" xr3:uid="{323211C5-81FD-41D0-9F64-A33241693AC3}" name="id" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{FDC1B446-D119-4AB0-BFD5-ACF6E75BA8A5}" name="name" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{92A07580-4496-4839-BDFD-3E1CD0593E78}" name="areaKnowledgeShort" dataDxfId="146"/>
     <tableColumn id="4" xr3:uid="{44EF4FF0-9A41-48CA-BC45-CC1B1304A096}" name="areaKnowledge"/>
     <tableColumn id="5" xr3:uid="{3A9496F5-2D90-4F09-9E2B-F936A6E5B397}" name="commonMundaneProfessions"/>
     <tableColumn id="6" xr3:uid="{7D2183EE-15A4-4FF4-9222-723CACFF8CAA}" name="commonMagicProfessions"/>
@@ -17960,15 +18046,15 @@
     <tableColumn id="10" xr3:uid="{745A9F74-C60C-4CBC-9102-98FE33FC8526}" name="uncommonAdvantages"/>
     <tableColumn id="11" xr3:uid="{C1FC4429-9AFB-46A3-A828-99A029A30219}" name="uncommonDisadvantages"/>
     <tableColumn id="12" xr3:uid="{839A4140-773B-4A98-9156-075E987FA39A}" name="commonNames"/>
-    <tableColumn id="13" xr3:uid="{8C51E69A-3B2D-4662-B403-D59D4610C76D}" name="src" dataDxfId="137"/>
-    <tableColumn id="14" xr3:uid="{97CC4A8C-51FE-4061-B8D7-F1FAF5164DF8}" name="Spalte1" dataDxfId="136"/>
+    <tableColumn id="13" xr3:uid="{8C51E69A-3B2D-4662-B403-D59D4610C76D}" name="src" dataDxfId="145"/>
+    <tableColumn id="14" xr3:uid="{97CC4A8C-51FE-4061-B8D7-F1FAF5164DF8}" name="Spalte1" dataDxfId="144"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:G95" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
   <autoFilter ref="A1:G95" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -17979,20 +18065,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="id" dataDxfId="133"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="name" dataDxfId="132"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="name_f" dataDxfId="131"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="subname" dataDxfId="130"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="subname_f" dataDxfId="129"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="req" dataDxfId="128"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="src" dataDxfId="127"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="id" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="name" dataDxfId="140"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="name_f" dataDxfId="139"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="subname" dataDxfId="138"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="subname_f" dataDxfId="137"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="req" dataDxfId="136"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="src" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle3" displayName="Tabelle3" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
   <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -18001,18 +18087,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="id" dataDxfId="124"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="name" dataDxfId="123"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="name_f" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{091296A4-103F-48ED-8EF3-B2FEB3C87545}" name="precedingText" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{7DC6E788-BCD5-45BD-8F54-8F4B65BB3D80}" name="concludingText" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="id" dataDxfId="132"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="name" dataDxfId="131"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="name_f" dataDxfId="130"/>
+    <tableColumn id="3" xr3:uid="{091296A4-103F-48ED-8EF3-B2FEB3C87545}" name="precedingText" dataDxfId="129"/>
+    <tableColumn id="4" xr3:uid="{7DC6E788-BCD5-45BD-8F54-8F4B65BB3D80}" name="concludingText" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:I97" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabelle8" displayName="Tabelle8" ref="A1:I97" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
   <autoFilter ref="A1:I97" xr:uid="{00000000-0009-0000-0100-000008000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -18025,22 +18111,22 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="117"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="sel" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="input" dataDxfId="114"/>
-    <tableColumn id="3" xr3:uid="{FC12F253-0C6F-41DB-A81E-5F24F57A658C}" name="rules" dataDxfId="113"/>
-    <tableColumn id="4" xr3:uid="{9F2EBD4E-ECC0-424F-95F5-50EAA6F5B5E7}" name="range" dataDxfId="112"/>
-    <tableColumn id="5" xr3:uid="{5AA75D55-59D7-4B4E-80C4-4F96782BBC49}" name="actions" dataDxfId="111"/>
-    <tableColumn id="8" xr3:uid="{2B63ADF8-714C-413C-BCF7-BB6C618249AA}" name="apValue" dataDxfId="110"/>
-    <tableColumn id="9" xr3:uid="{49DA2457-D486-45F3-AE88-F580827EB701}" name="apValueAppend" dataDxfId="109"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="id" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="name" dataDxfId="124"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="sel" dataDxfId="123"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="input" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{FC12F253-0C6F-41DB-A81E-5F24F57A658C}" name="rules" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{9F2EBD4E-ECC0-424F-95F5-50EAA6F5B5E7}" name="range" dataDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{5AA75D55-59D7-4B4E-80C4-4F96782BBC49}" name="actions" dataDxfId="119"/>
+    <tableColumn id="8" xr3:uid="{2B63ADF8-714C-413C-BCF7-BB6C618249AA}" name="apValue" dataDxfId="118"/>
+    <tableColumn id="9" xr3:uid="{49DA2457-D486-45F3-AE88-F580827EB701}" name="apValueAppend" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:I74" totalsRowShown="0" headerRowDxfId="108" dataDxfId="107">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:I74" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115">
   <autoFilter ref="A1:I74" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -18053,48 +18139,15 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="id" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="name" dataDxfId="105"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="sel" dataDxfId="104"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="input" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{C5214789-D9D9-4771-9706-EDB477595F41}" name="rules" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{2F14A9EB-F0B9-45C3-A8BF-5508A2BF2F22}" name="range" dataDxfId="101"/>
-    <tableColumn id="5" xr3:uid="{B50DBC4E-D373-4601-A386-FC91C8F2ED6F}" name="actions" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{7E9F07AC-3AE6-4DDB-8E2F-AC26B390C5D6}" name="apValue" dataDxfId="99"/>
-    <tableColumn id="9" xr3:uid="{6401E586-21B4-4C09-8B51-F19F7E31BF4F}" name="apValueAppend" dataDxfId="98"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabelle7" displayName="Tabelle7" ref="A1:J60" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
-  <autoFilter ref="A1:J60" xr:uid="{00000000-0009-0000-0100-000007000000}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-  </autoFilter>
-  <sortState ref="A2:D60">
-    <sortCondition ref="A1:A60"/>
-  </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="id" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="name" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="spec" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="spec_input" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="tools" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="quality" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="failed" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="critical" dataDxfId="88"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="botch" dataDxfId="87"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="src" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="id" dataDxfId="114"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="name" dataDxfId="113"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="sel" dataDxfId="112"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="input" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{C5214789-D9D9-4771-9706-EDB477595F41}" name="rules" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{2F14A9EB-F0B9-45C3-A8BF-5508A2BF2F22}" name="range" dataDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{B50DBC4E-D373-4601-A386-FC91C8F2ED6F}" name="actions" dataDxfId="108"/>
+    <tableColumn id="8" xr3:uid="{7E9F07AC-3AE6-4DDB-8E2F-AC26B390C5D6}" name="apValue" dataDxfId="107"/>
+    <tableColumn id="9" xr3:uid="{6401E586-21B4-4C09-8B51-F19F7E31BF4F}" name="apValueAppend" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18399,8 +18452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18551,6 +18604,124 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
@@ -20220,7 +20391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -20399,7 +20570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M234"/>
   <sheetViews>
@@ -29496,7 +29667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H44"/>
   <sheetViews>
@@ -30637,7 +30808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M193"/>
   <sheetViews>
@@ -38577,7 +38748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -38899,7 +39070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J664"/>
   <sheetViews>
@@ -44312,7 +44483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B111"/>
   <sheetViews>
@@ -45221,7 +45392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
@@ -45965,314 +46136,6 @@
       </c>
       <c r="B76" s="1" t="s">
         <v>1303</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:B36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="4.1328125" customWidth="1"/>
-    <col min="2" max="2" width="24.53125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>1315</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>1317</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1319</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>1324</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>1325</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>1326</v>
       </c>
     </row>
   </sheetData>
@@ -46370,6 +46233,314 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="4.1328125" customWidth="1"/>
+    <col min="2" max="2" width="24.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:C466"/>
   <sheetViews>
@@ -51519,7 +51690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BDF849A-84B1-4731-B5ED-CC1BDC8FBE84}">
   <dimension ref="A1:C577"/>
   <sheetViews>
@@ -57889,7 +58060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:B546"/>
   <sheetViews>
@@ -62282,23 +62453,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:K1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.6640625" style="1"/>
+    <col min="3" max="10" width="10.6640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -62341,7 +62507,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5284</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2693</v>
@@ -62355,19 +62521,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>5285</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2693</v>
+        <v>2717</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2718</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2719</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2720</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>2713</v>
+        <v>2721</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>165</v>
+        <v>2722</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>2723</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>2724</v>
       </c>
       <c r="K3" s="1">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -62375,13 +62556,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2693</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>2725</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>2726</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>2727</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>2728</v>
+      </c>
       <c r="K4" s="1">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -62389,241 +62582,30 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2693</v>
+        <v>2729</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2730</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2731</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>2714</v>
+        <v>2732</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>2715</v>
+        <v>160</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>2733</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>2734</v>
       </c>
       <c r="K5" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2693</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="K6" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>2693</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>2716</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="K7" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2693</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>2716</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="K8" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2717</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2718</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>2719</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>2720</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>2721</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>2722</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>2723</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>2724</v>
-      </c>
-      <c r="K9" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>2717</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>2718</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>2719</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>2720</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>2721</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>2722</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>2723</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>2724</v>
-      </c>
-      <c r="K10" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>2717</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2718</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>2719</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>2720</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>2721</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>2722</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>2723</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>2724</v>
-      </c>
-      <c r="K11" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>2693</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>2725</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>2726</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>2727</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>2728</v>
-      </c>
-      <c r="K12" s="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>2729</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>2730</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>2731</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>2732</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>2733</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>2734</v>
-      </c>
-      <c r="K13" s="1">
         <v>94</v>
       </c>
     </row>
@@ -62637,6 +62619,162 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083BD96D-43BC-4CEF-8439-DF499D6DDADF}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" style="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.9296875" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.796875" style="44" customWidth="1"/>
+    <col min="5" max="5" width="20.59765625" style="44" customWidth="1"/>
+    <col min="6" max="6" width="22.796875" style="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>2689</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>2690</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>2691</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>2692</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="44">
+        <v>1</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="44">
+        <v>2</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>2713</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="44">
+        <v>3</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="44">
+        <v>4</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>2714</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="44">
+        <v>5</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="44">
+        <v>6</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>2716</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="44">
+        <v>7</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>2716</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="44">
+        <v>8</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="44">
+        <v>9</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="44">
+        <v>10</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
@@ -63741,7 +63879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G95"/>
   <sheetViews>
@@ -65406,7 +65544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E162"/>
   <sheetViews>
@@ -67252,7 +67390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I97"/>
   <sheetViews>
@@ -68521,7 +68659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
@@ -69576,122 +69714,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="2.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>